<commit_message>
Moved to new get/fetch SQL model and updated home page.
</commit_message>
<xml_diff>
--- a/design/sienaDataArraysBuilder.xlsx
+++ b/design/sienaDataArraysBuilder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matttownsend/go/mwt-go-dev/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0978829D-F229-9546-861F-B51D56CC201A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA2F37-671D-8B41-B3EA-29939BE584C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-5600" windowWidth="38400" windowHeight="21600" xr2:uid="{8265F428-BA81-814D-9171-A3F66298AE69}"/>
+    <workbookView xWindow="-38120" yWindow="-4940" windowWidth="34980" windowHeight="18940" xr2:uid="{8265F428-BA81-814D-9171-A3F66298AE69}"/>
   </bookViews>
   <sheets>
     <sheet name="GO Struct Bits" sheetId="1" r:id="rId1"/>
@@ -58,147 +58,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>returnRecord.</t>
-  </si>
-  <si>
-    <t>var</t>
   </si>
   <si>
     <t>getSienaCounterpartyList</t>
   </si>
   <si>
-    <t>Firm</t>
-  </si>
-  <si>
-    <t>Centre</t>
-  </si>
-  <si>
-    <t>DealList</t>
-  </si>
-  <si>
     <t>SienaReference</t>
   </si>
   <si>
-    <t>CustomerSienaView</t>
+    <t xml:space="preserve">getSiena…List </t>
   </si>
   <si>
-    <t>Status</t>
+    <t>&gt;&gt;&gt;</t>
   </si>
   <si>
-    <t>MaturityDate</t>
+    <t>LegNo</t>
   </si>
   <si>
-    <t>ContractNumber</t>
+    <t>MMLegNo</t>
   </si>
   <si>
-    <t>ExternalReference</t>
+    <t>Narrative</t>
   </si>
   <si>
-    <t>Book</t>
+    <t>Amount</t>
   </si>
   <si>
-    <t>MandatedUser</t>
+    <t>StartInterestDate</t>
   </si>
   <si>
-    <t>Portfolio</t>
+    <t>EndInterestDate</t>
   </si>
   <si>
-    <t>AgreementId</t>
+    <t>Amortisation</t>
   </si>
   <si>
-    <t>BackOfficeRefNo</t>
+    <t>InterestAmount</t>
   </si>
   <si>
-    <t>ISIN</t>
+    <t>InterestAction</t>
   </si>
   <si>
-    <t>UTI</t>
+    <t>FixingDate</t>
   </si>
   <si>
-    <t>BookName</t>
+    <t>InterestCalculationDate</t>
   </si>
   <si>
-    <t>DealTypeShortName</t>
+    <t>AmendmentAmount</t>
   </si>
   <si>
-    <t>FullDealType</t>
+    <t>AccountTransactions</t>
   </si>
   <si>
-    <t>TradeDate</t>
-  </si>
-  <si>
-    <t>DealtCcy</t>
-  </si>
-  <si>
-    <t>DealtAmount</t>
-  </si>
-  <si>
-    <t>AgainstAmount</t>
-  </si>
-  <si>
-    <t>AgainstCcy</t>
-  </si>
-  <si>
-    <t>AllInRate</t>
-  </si>
-  <si>
-    <t>MktRate</t>
-  </si>
-  <si>
-    <t>SettleCcy</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>NpvRate</t>
-  </si>
-  <si>
-    <t>OriginUser</t>
-  </si>
-  <si>
-    <t>PayInstruction</t>
-  </si>
-  <si>
-    <t>ReceiptInstruction</t>
-  </si>
-  <si>
-    <t>NIName</t>
-  </si>
-  <si>
-    <t>CCYPair</t>
-  </si>
-  <si>
-    <t>Instrument</t>
-  </si>
-  <si>
-    <t>PortfolioName</t>
-  </si>
-  <si>
-    <t>RVDate</t>
-  </si>
-  <si>
-    <t>RVMTM</t>
-  </si>
-  <si>
-    <t>CounterBook</t>
-  </si>
-  <si>
-    <t>CounterBookName</t>
-  </si>
-  <si>
-    <t>Party</t>
-  </si>
-  <si>
-    <t>PartyName</t>
-  </si>
-  <si>
-    <t>ValueDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">getSiena…List </t>
+    <t>ACCTTX</t>
   </si>
 </sst>
 </file>
@@ -606,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4CE648-3973-0F42-A3A6-4E494BE264E6}">
   <dimension ref="B2:AG74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AG6" sqref="AG6:AG47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,46 +547,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
       <c r="D2" t="str">
         <f>"siena"&amp;B4&amp;".go"</f>
-        <v>sienaDealList.go</v>
+        <v>sienaAccountTransactions.go</v>
       </c>
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.2">
       <c r="I3" t="str">
         <f>"siena"&amp;B4</f>
-        <v>sienaDealList</v>
+        <v>sienaAccountTransactions</v>
       </c>
     </row>
     <row r="4" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>"siena"&amp;B4&amp;"Page"</f>
-        <v>sienaDealListPage</v>
+        <v>sienaAccountTransactionsPage</v>
       </c>
       <c r="E4" s="2" t="str">
         <f>"siena"&amp;B4&amp;"Item"</f>
-        <v>sienaDealListItem</v>
+        <v>sienaAccountTransactionsItem</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="str">
         <f>"newSiena"&amp;B4&amp;"Handler"</f>
-        <v>newSienaDealListHandler</v>
+        <v>newSienaAccountTransactionsHandler</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG4" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ref="D6:D39" si="0">B6&amp;"    string"</f>
@@ -689,8 +608,8 @@
         <v>SienaReference:    "",</v>
       </c>
       <c r="L6" t="str">
-        <f>$I$3&amp;"."&amp;B6&amp;" = "&amp;B6&amp;".String"</f>
-        <v>sienaDealList.SienaReference = SienaReference.String</v>
+        <f>$I$3&amp;"."&amp;B6&amp;" = sql"&amp;$B$2&amp;B6&amp;".String"</f>
+        <v>sienaAccountTransactions.SienaReference = sqlACCTTXSienaReference.String</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" ref="V6:V39" si="3">"item."&amp;B6&amp;" = r.FormValue("""&amp;B6&amp;""")"</f>
@@ -702,1524 +621,1466 @@
       </c>
       <c r="AG6" t="str">
         <f>$I$3&amp;"."&amp;B6&amp;" = sql"&amp;B6&amp;".String"</f>
-        <v>sienaDealList.SienaReference = sqlSienaReference.String</v>
+        <v>sienaAccountTransactions.SienaReference = sqlSienaReference.String</v>
       </c>
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>CustomerSienaView    string</v>
+        <v>LegNo    string</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" ref="E7:E39" si="5">D7</f>
-        <v>CustomerSienaView    string</v>
+        <v>LegNo    string</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>CustomerSienaView:    returnRecord.CustomerSienaView,</v>
+        <v>LegNo:    returnRecord.LegNo,</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="2"/>
-        <v>CustomerSienaView:    "",</v>
+        <v>LegNo:    "",</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" ref="L7:L39" si="6">$I$3&amp;"."&amp;B7&amp;" = "&amp;B7&amp;".String"</f>
-        <v>sienaDealList.CustomerSienaView = CustomerSienaView.String</v>
+        <f t="shared" ref="L7:L61" si="6">$I$3&amp;"."&amp;B7&amp;" = sql"&amp;$B$2&amp;B7&amp;".String"</f>
+        <v>sienaAccountTransactions.LegNo = sqlACCTTXLegNo.String</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="3"/>
-        <v>item.CustomerSienaView = r.FormValue("CustomerSienaView")</v>
+        <v>item.LegNo = r.FormValue("LegNo")</v>
       </c>
       <c r="AD7" t="str">
         <f t="shared" si="4"/>
-        <v>.CustomerSienaView</v>
+        <v>.LegNo</v>
       </c>
       <c r="AG7" t="str">
-        <f t="shared" ref="AG7:AG52" si="7">$I$3&amp;"."&amp;B7&amp;" = sql"&amp;B7&amp;".String"</f>
-        <v>sienaDealList.CustomerSienaView = sqlCustomerSienaView.String</v>
+        <f t="shared" ref="AG7:AG70" si="7">$I$3&amp;"."&amp;B7&amp;" = sql"&amp;B7&amp;".String"</f>
+        <v>sienaAccountTransactions.LegNo = sqlLegNo.String</v>
       </c>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>Status    string</v>
+        <v>MMLegNo    string</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="5"/>
-        <v>Status    string</v>
+        <v>MMLegNo    string</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>Status:    returnRecord.Status,</v>
+        <v>MMLegNo:    returnRecord.MMLegNo,</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="2"/>
-        <v>Status:    "",</v>
+        <v>MMLegNo:    "",</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.Status = Status.String</v>
+        <v>sienaAccountTransactions.MMLegNo = sqlACCTTXMMLegNo.String</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="3"/>
-        <v>item.Status = r.FormValue("Status")</v>
+        <v>item.MMLegNo = r.FormValue("MMLegNo")</v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="4"/>
-        <v>.Status</v>
+        <v>.MMLegNo</v>
       </c>
       <c r="AG8" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.Status = sqlStatus.String</v>
+        <v>sienaAccountTransactions.MMLegNo = sqlMMLegNo.String</v>
       </c>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>ValueDate    string</v>
+        <v>Narrative    string</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="5"/>
-        <v>ValueDate    string</v>
+        <v>Narrative    string</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>ValueDate:    returnRecord.ValueDate,</v>
+        <v>Narrative:    returnRecord.Narrative,</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="2"/>
-        <v>ValueDate:    "",</v>
+        <v>Narrative:    "",</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.ValueDate = ValueDate.String</v>
+        <v>sienaAccountTransactions.Narrative = sqlACCTTXNarrative.String</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="3"/>
-        <v>item.ValueDate = r.FormValue("ValueDate")</v>
+        <v>item.Narrative = r.FormValue("Narrative")</v>
       </c>
       <c r="AD9" t="str">
         <f t="shared" si="4"/>
-        <v>.ValueDate</v>
+        <v>.Narrative</v>
       </c>
       <c r="AG9" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.ValueDate = sqlValueDate.String</v>
+        <v>sienaAccountTransactions.Narrative = sqlNarrative.String</v>
       </c>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>MaturityDate    string</v>
+        <v>Amount    string</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="5"/>
-        <v>MaturityDate    string</v>
+        <v>Amount    string</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>MaturityDate:    returnRecord.MaturityDate,</v>
+        <v>Amount:    returnRecord.Amount,</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="2"/>
-        <v>MaturityDate:    "",</v>
+        <v>Amount:    "",</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.MaturityDate = MaturityDate.String</v>
+        <v>sienaAccountTransactions.Amount = sqlACCTTXAmount.String</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="3"/>
-        <v>item.MaturityDate = r.FormValue("MaturityDate")</v>
+        <v>item.Amount = r.FormValue("Amount")</v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="4"/>
-        <v>.MaturityDate</v>
+        <v>.Amount</v>
       </c>
       <c r="AG10" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.MaturityDate = sqlMaturityDate.String</v>
+        <v>sienaAccountTransactions.Amount = sqlAmount.String</v>
       </c>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>ContractNumber    string</v>
+        <v>StartInterestDate    string</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="5"/>
-        <v>ContractNumber    string</v>
+        <v>StartInterestDate    string</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
-        <v>ContractNumber:    returnRecord.ContractNumber,</v>
+        <v>StartInterestDate:    returnRecord.StartInterestDate,</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="2"/>
-        <v>ContractNumber:    "",</v>
+        <v>StartInterestDate:    "",</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.ContractNumber = ContractNumber.String</v>
+        <v>sienaAccountTransactions.StartInterestDate = sqlACCTTXStartInterestDate.String</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="3"/>
-        <v>item.ContractNumber = r.FormValue("ContractNumber")</v>
+        <v>item.StartInterestDate = r.FormValue("StartInterestDate")</v>
       </c>
       <c r="AD11" t="str">
         <f t="shared" si="4"/>
-        <v>.ContractNumber</v>
+        <v>.StartInterestDate</v>
       </c>
       <c r="AG11" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.ContractNumber = sqlContractNumber.String</v>
+        <v>sienaAccountTransactions.StartInterestDate = sqlStartInterestDate.String</v>
       </c>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>ExternalReference    string</v>
+        <v>EndInterestDate    string</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="5"/>
-        <v>ExternalReference    string</v>
+        <v>EndInterestDate    string</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
-        <v>ExternalReference:    returnRecord.ExternalReference,</v>
+        <v>EndInterestDate:    returnRecord.EndInterestDate,</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="2"/>
-        <v>ExternalReference:    "",</v>
+        <v>EndInterestDate:    "",</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.ExternalReference = ExternalReference.String</v>
+        <v>sienaAccountTransactions.EndInterestDate = sqlACCTTXEndInterestDate.String</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="3"/>
-        <v>item.ExternalReference = r.FormValue("ExternalReference")</v>
+        <v>item.EndInterestDate = r.FormValue("EndInterestDate")</v>
       </c>
       <c r="AD12" t="str">
         <f t="shared" si="4"/>
-        <v>.ExternalReference</v>
+        <v>.EndInterestDate</v>
       </c>
       <c r="AG12" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.ExternalReference = sqlExternalReference.String</v>
+        <v>sienaAccountTransactions.EndInterestDate = sqlEndInterestDate.String</v>
       </c>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>Book    string</v>
+        <v>Amortisation    string</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="5"/>
-        <v>Book    string</v>
+        <v>Amortisation    string</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
-        <v>Book:    returnRecord.Book,</v>
+        <v>Amortisation:    returnRecord.Amortisation,</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
-        <v>Book:    "",</v>
+        <v>Amortisation:    "",</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.Book = Book.String</v>
+        <v>sienaAccountTransactions.Amortisation = sqlACCTTXAmortisation.String</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="3"/>
-        <v>item.Book = r.FormValue("Book")</v>
+        <v>item.Amortisation = r.FormValue("Amortisation")</v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="4"/>
-        <v>.Book</v>
+        <v>.Amortisation</v>
       </c>
       <c r="AG13" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.Book = sqlBook.String</v>
+        <v>sienaAccountTransactions.Amortisation = sqlAmortisation.String</v>
       </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>MandatedUser    string</v>
+        <v>InterestAmount    string</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="5"/>
-        <v>MandatedUser    string</v>
+        <v>InterestAmount    string</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
-        <v>MandatedUser:    returnRecord.MandatedUser,</v>
+        <v>InterestAmount:    returnRecord.InterestAmount,</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="2"/>
-        <v>MandatedUser:    "",</v>
+        <v>InterestAmount:    "",</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.MandatedUser = MandatedUser.String</v>
+        <v>sienaAccountTransactions.InterestAmount = sqlACCTTXInterestAmount.String</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="3"/>
-        <v>item.MandatedUser = r.FormValue("MandatedUser")</v>
+        <v>item.InterestAmount = r.FormValue("InterestAmount")</v>
       </c>
       <c r="AD14" t="str">
         <f t="shared" si="4"/>
-        <v>.MandatedUser</v>
+        <v>.InterestAmount</v>
       </c>
       <c r="AG14" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.MandatedUser = sqlMandatedUser.String</v>
+        <v>sienaAccountTransactions.InterestAmount = sqlInterestAmount.String</v>
       </c>
     </row>
     <row r="15" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>Portfolio    string</v>
+        <v>InterestAction    string</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="5"/>
-        <v>Portfolio    string</v>
+        <v>InterestAction    string</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>Portfolio:    returnRecord.Portfolio,</v>
+        <v>InterestAction:    returnRecord.InterestAction,</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="2"/>
-        <v>Portfolio:    "",</v>
+        <v>InterestAction:    "",</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.Portfolio = Portfolio.String</v>
+        <v>sienaAccountTransactions.InterestAction = sqlACCTTXInterestAction.String</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="3"/>
-        <v>item.Portfolio = r.FormValue("Portfolio")</v>
+        <v>item.InterestAction = r.FormValue("InterestAction")</v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="4"/>
-        <v>.Portfolio</v>
+        <v>.InterestAction</v>
       </c>
       <c r="AG15" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.Portfolio = sqlPortfolio.String</v>
+        <v>sienaAccountTransactions.InterestAction = sqlInterestAction.String</v>
       </c>
     </row>
     <row r="16" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>AgreementId    string</v>
+        <v>FixingDate    string</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="5"/>
-        <v>AgreementId    string</v>
+        <v>FixingDate    string</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>AgreementId:    returnRecord.AgreementId,</v>
+        <v>FixingDate:    returnRecord.FixingDate,</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="2"/>
-        <v>AgreementId:    "",</v>
+        <v>FixingDate:    "",</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.AgreementId = AgreementId.String</v>
+        <v>sienaAccountTransactions.FixingDate = sqlACCTTXFixingDate.String</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="3"/>
-        <v>item.AgreementId = r.FormValue("AgreementId")</v>
+        <v>item.FixingDate = r.FormValue("FixingDate")</v>
       </c>
       <c r="AD16" t="str">
         <f t="shared" si="4"/>
-        <v>.AgreementId</v>
+        <v>.FixingDate</v>
       </c>
       <c r="AG16" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.AgreementId = sqlAgreementId.String</v>
+        <v>sienaAccountTransactions.FixingDate = sqlFixingDate.String</v>
       </c>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>BackOfficeRefNo    string</v>
+        <v>InterestCalculationDate    string</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="5"/>
-        <v>BackOfficeRefNo    string</v>
+        <v>InterestCalculationDate    string</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>BackOfficeRefNo:    returnRecord.BackOfficeRefNo,</v>
+        <v>InterestCalculationDate:    returnRecord.InterestCalculationDate,</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="2"/>
-        <v>BackOfficeRefNo:    "",</v>
+        <v>InterestCalculationDate:    "",</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.BackOfficeRefNo = BackOfficeRefNo.String</v>
+        <v>sienaAccountTransactions.InterestCalculationDate = sqlACCTTXInterestCalculationDate.String</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="3"/>
-        <v>item.BackOfficeRefNo = r.FormValue("BackOfficeRefNo")</v>
+        <v>item.InterestCalculationDate = r.FormValue("InterestCalculationDate")</v>
       </c>
       <c r="AD17" t="str">
         <f t="shared" si="4"/>
-        <v>.BackOfficeRefNo</v>
+        <v>.InterestCalculationDate</v>
       </c>
       <c r="AG17" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.BackOfficeRefNo = sqlBackOfficeRefNo.String</v>
+        <v>sienaAccountTransactions.InterestCalculationDate = sqlInterestCalculationDate.String</v>
       </c>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>ISIN    string</v>
+        <v>AmendmentAmount    string</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="5"/>
-        <v>ISIN    string</v>
+        <v>AmendmentAmount    string</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
-        <v>ISIN:    returnRecord.ISIN,</v>
+        <v>AmendmentAmount:    returnRecord.AmendmentAmount,</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="2"/>
-        <v>ISIN:    "",</v>
+        <v>AmendmentAmount:    "",</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.ISIN = ISIN.String</v>
+        <v>sienaAccountTransactions.AmendmentAmount = sqlACCTTXAmendmentAmount.String</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="3"/>
-        <v>item.ISIN = r.FormValue("ISIN")</v>
+        <v>item.AmendmentAmount = r.FormValue("AmendmentAmount")</v>
       </c>
       <c r="AD18" t="str">
         <f t="shared" si="4"/>
-        <v>.ISIN</v>
+        <v>.AmendmentAmount</v>
       </c>
       <c r="AG18" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.ISIN = sqlISIN.String</v>
+        <v>sienaAccountTransactions.AmendmentAmount = sqlAmendmentAmount.String</v>
       </c>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>UTI    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="5"/>
-        <v>UTI    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>UTI:    returnRecord.UTI,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="2"/>
-        <v>UTI:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.UTI = UTI.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="3"/>
-        <v>item.UTI = r.FormValue("UTI")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD19" t="str">
         <f t="shared" si="4"/>
-        <v>.UTI</v>
+        <v>.</v>
       </c>
       <c r="AG19" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.UTI = sqlUTI.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>BookName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="5"/>
-        <v>BookName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
-        <v>BookName:    returnRecord.BookName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="2"/>
-        <v>BookName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.BookName = BookName.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="3"/>
-        <v>item.BookName = r.FormValue("BookName")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD20" t="str">
         <f t="shared" si="4"/>
-        <v>.BookName</v>
+        <v>.</v>
       </c>
       <c r="AG20" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.BookName = sqlBookName.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B21" s="1"/>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>Centre    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="5"/>
-        <v>Centre    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
-        <v>Centre:    returnRecord.Centre,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="2"/>
-        <v>Centre:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.Centre = Centre.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="3"/>
-        <v>item.Centre = r.FormValue("Centre")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD21" t="str">
         <f t="shared" si="4"/>
-        <v>.Centre</v>
+        <v>.</v>
       </c>
       <c r="AG21" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.Centre = sqlCentre.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B22" s="1"/>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>Firm    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="5"/>
-        <v>Firm    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
-        <v>Firm:    returnRecord.Firm,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="2"/>
-        <v>Firm:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.Firm = Firm.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="3"/>
-        <v>item.Firm = r.FormValue("Firm")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD22" t="str">
         <f t="shared" si="4"/>
-        <v>.Firm</v>
+        <v>.</v>
       </c>
       <c r="AG22" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.Firm = sqlFirm.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>DealTypeShortName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="5"/>
-        <v>DealTypeShortName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
-        <v>DealTypeShortName:    returnRecord.DealTypeShortName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="2"/>
-        <v>DealTypeShortName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.DealTypeShortName = DealTypeShortName.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V23" t="str">
         <f t="shared" si="3"/>
-        <v>item.DealTypeShortName = r.FormValue("DealTypeShortName")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD23" t="str">
         <f t="shared" si="4"/>
-        <v>.DealTypeShortName</v>
+        <v>.</v>
       </c>
       <c r="AG23" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.DealTypeShortName = sqlDealTypeShortName.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B24" s="1"/>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>FullDealType    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="5"/>
-        <v>FullDealType    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
-        <v>FullDealType:    returnRecord.FullDealType,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="2"/>
-        <v>FullDealType:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.FullDealType = FullDealType.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V24" t="str">
         <f t="shared" si="3"/>
-        <v>item.FullDealType = r.FormValue("FullDealType")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD24" t="str">
         <f t="shared" si="4"/>
-        <v>.FullDealType</v>
+        <v>.</v>
       </c>
       <c r="AG24" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.FullDealType = sqlFullDealType.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B25" s="1"/>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>TradeDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="5"/>
-        <v>TradeDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
-        <v>TradeDate:    returnRecord.TradeDate,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="2"/>
-        <v>TradeDate:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.TradeDate = TradeDate.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V25" t="str">
         <f t="shared" si="3"/>
-        <v>item.TradeDate = r.FormValue("TradeDate")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD25" t="str">
         <f t="shared" si="4"/>
-        <v>.TradeDate</v>
+        <v>.</v>
       </c>
       <c r="AG25" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.TradeDate = sqlTradeDate.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="B26" s="1"/>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>DealtCcy    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="5"/>
-        <v>DealtCcy    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
-        <v>DealtCcy:    returnRecord.DealtCcy,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="2"/>
-        <v>DealtCcy:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.DealtCcy = DealtCcy.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V26" t="str">
         <f t="shared" si="3"/>
-        <v>item.DealtCcy = r.FormValue("DealtCcy")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD26" t="str">
         <f t="shared" si="4"/>
-        <v>.DealtCcy</v>
+        <v>.</v>
       </c>
       <c r="AG26" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.DealtCcy = sqlDealtCcy.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>DealtAmount    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="5"/>
-        <v>DealtAmount    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
-        <v>DealtAmount:    returnRecord.DealtAmount,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="2"/>
-        <v>DealtAmount:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.DealtAmount = DealtAmount.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V27" t="str">
         <f t="shared" si="3"/>
-        <v>item.DealtAmount = r.FormValue("DealtAmount")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD27" t="str">
         <f t="shared" si="4"/>
-        <v>.DealtAmount</v>
+        <v>.</v>
       </c>
       <c r="AG27" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.DealtAmount = sqlDealtAmount.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B28" s="1"/>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>AgainstAmount    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="5"/>
-        <v>AgainstAmount    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
-        <v>AgainstAmount:    returnRecord.AgainstAmount,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="2"/>
-        <v>AgainstAmount:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.AgainstAmount = AgainstAmount.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V28" t="str">
         <f t="shared" si="3"/>
-        <v>item.AgainstAmount = r.FormValue("AgainstAmount")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD28" t="str">
         <f t="shared" si="4"/>
-        <v>.AgainstAmount</v>
+        <v>.</v>
       </c>
       <c r="AG28" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.AgainstAmount = sqlAgainstAmount.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B29" s="1"/>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>AgainstCcy    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="5"/>
-        <v>AgainstCcy    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
-        <v>AgainstCcy:    returnRecord.AgainstCcy,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="2"/>
-        <v>AgainstCcy:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.AgainstCcy = AgainstCcy.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V29" t="str">
         <f t="shared" si="3"/>
-        <v>item.AgainstCcy = r.FormValue("AgainstCcy")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD29" t="str">
         <f t="shared" si="4"/>
-        <v>.AgainstCcy</v>
+        <v>.</v>
       </c>
       <c r="AG29" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.AgainstCcy = sqlAgainstCcy.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="30" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>AllInRate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="5"/>
-        <v>AllInRate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
-        <v>AllInRate:    returnRecord.AllInRate,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="2"/>
-        <v>AllInRate:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.AllInRate = AllInRate.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V30" t="str">
         <f t="shared" si="3"/>
-        <v>item.AllInRate = r.FormValue("AllInRate")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD30" t="str">
         <f t="shared" si="4"/>
-        <v>.AllInRate</v>
+        <v>.</v>
       </c>
       <c r="AG30" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.AllInRate = sqlAllInRate.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B31" s="1"/>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>MktRate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="5"/>
-        <v>MktRate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
-        <v>MktRate:    returnRecord.MktRate,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="2"/>
-        <v>MktRate:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.MktRate = MktRate.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V31" t="str">
         <f t="shared" si="3"/>
-        <v>item.MktRate = r.FormValue("MktRate")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD31" t="str">
         <f t="shared" si="4"/>
-        <v>.MktRate</v>
+        <v>.</v>
       </c>
       <c r="AG31" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.MktRate = sqlMktRate.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B32" s="1"/>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>SettleCcy    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="5"/>
-        <v>SettleCcy    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
-        <v>SettleCcy:    returnRecord.SettleCcy,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="2"/>
-        <v>SettleCcy:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.SettleCcy = SettleCcy.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V32" t="str">
         <f t="shared" si="3"/>
-        <v>item.SettleCcy = r.FormValue("SettleCcy")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD32" t="str">
         <f t="shared" si="4"/>
-        <v>.SettleCcy</v>
+        <v>.</v>
       </c>
       <c r="AG32" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.SettleCcy = sqlSettleCcy.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="33" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="B33" s="1"/>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>Direction    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="5"/>
-        <v>Direction    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
-        <v>Direction:    returnRecord.Direction,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="2"/>
-        <v>Direction:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.Direction = Direction.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V33" t="str">
         <f t="shared" si="3"/>
-        <v>item.Direction = r.FormValue("Direction")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD33" t="str">
         <f t="shared" si="4"/>
-        <v>.Direction</v>
+        <v>.</v>
       </c>
       <c r="AG33" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.Direction = sqlDirection.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="34" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="B34" s="1"/>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>NpvRate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="5"/>
-        <v>NpvRate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
-        <v>NpvRate:    returnRecord.NpvRate,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="2"/>
-        <v>NpvRate:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.NpvRate = NpvRate.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V34" t="str">
         <f t="shared" si="3"/>
-        <v>item.NpvRate = r.FormValue("NpvRate")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD34" t="str">
         <f t="shared" si="4"/>
-        <v>.NpvRate</v>
+        <v>.</v>
       </c>
       <c r="AG34" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.NpvRate = sqlNpvRate.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="35" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="B35" s="1"/>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>OriginUser    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="5"/>
-        <v>OriginUser    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
-        <v>OriginUser:    returnRecord.OriginUser,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="2"/>
-        <v>OriginUser:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.OriginUser = OriginUser.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V35" t="str">
         <f t="shared" si="3"/>
-        <v>item.OriginUser = r.FormValue("OriginUser")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD35" t="str">
         <f t="shared" si="4"/>
-        <v>.OriginUser</v>
+        <v>.</v>
       </c>
       <c r="AG35" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.OriginUser = sqlOriginUser.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="36" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B36" s="1"/>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>PayInstruction    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="5"/>
-        <v>PayInstruction    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
-        <v>PayInstruction:    returnRecord.PayInstruction,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="2"/>
-        <v>PayInstruction:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.PayInstruction = PayInstruction.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V36" t="str">
         <f t="shared" si="3"/>
-        <v>item.PayInstruction = r.FormValue("PayInstruction")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD36" t="str">
         <f t="shared" si="4"/>
-        <v>.PayInstruction</v>
+        <v>.</v>
       </c>
       <c r="AG36" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.PayInstruction = sqlPayInstruction.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="37" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="B37" s="1"/>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>ReceiptInstruction    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="5"/>
-        <v>ReceiptInstruction    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
-        <v>ReceiptInstruction:    returnRecord.ReceiptInstruction,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="2"/>
-        <v>ReceiptInstruction:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.ReceiptInstruction = ReceiptInstruction.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V37" t="str">
         <f t="shared" si="3"/>
-        <v>item.ReceiptInstruction = r.FormValue("ReceiptInstruction")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD37" t="str">
         <f t="shared" si="4"/>
-        <v>.ReceiptInstruction</v>
+        <v>.</v>
       </c>
       <c r="AG37" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.ReceiptInstruction = sqlReceiptInstruction.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="38" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="B38" s="1"/>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>NIName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="5"/>
-        <v>NIName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
-        <v>NIName:    returnRecord.NIName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="2"/>
-        <v>NIName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.NIName = NIName.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V38" t="str">
         <f t="shared" si="3"/>
-        <v>item.NIName = r.FormValue("NIName")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD38" t="str">
         <f t="shared" si="4"/>
-        <v>.NIName</v>
+        <v>.</v>
       </c>
       <c r="AG38" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.NIName = sqlNIName.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="39" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>CCYPair    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="5"/>
-        <v>CCYPair    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
-        <v>CCYPair:    returnRecord.CCYPair,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="2"/>
-        <v>CCYPair:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" si="6"/>
-        <v>sienaDealList.CCYPair = CCYPair.String</v>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V39" t="str">
         <f t="shared" si="3"/>
-        <v>item.CCYPair = r.FormValue("CCYPair")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD39" t="str">
         <f t="shared" si="4"/>
-        <v>.CCYPair</v>
+        <v>.</v>
       </c>
       <c r="AG39" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.CCYPair = sqlCCYPair.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="40" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="B40" s="1"/>
       <c r="D40" t="str">
         <f t="shared" ref="D40:D62" si="8">B40&amp;"    string"</f>
-        <v>Instrument    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" ref="E40:E62" si="9">D40</f>
-        <v>Instrument    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" ref="G40:G62" si="10">B40&amp;":    "&amp;$F$4&amp;B40&amp;","</f>
-        <v>Instrument:    returnRecord.Instrument,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" ref="H40:H62" si="11">B40&amp;":    """""&amp;","</f>
-        <v>Instrument:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L40" t="str">
-        <f t="shared" ref="L40:L62" si="12">$I$3&amp;"."&amp;B40&amp;" = "&amp;B40&amp;".String"</f>
-        <v>sienaDealList.Instrument = Instrument.String</v>
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
       </c>
       <c r="V40" t="str">
-        <f t="shared" ref="V40:V62" si="13">"item."&amp;B40&amp;" = r.FormValue("""&amp;B40&amp;""")"</f>
-        <v>item.Instrument = r.FormValue("Instrument")</v>
+        <f t="shared" ref="V40:V62" si="12">"item."&amp;B40&amp;" = r.FormValue("""&amp;B40&amp;""")"</f>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD40" t="str">
-        <f t="shared" ref="AD40:AD62" si="14">"."&amp;B40</f>
-        <v>.Instrument</v>
+        <f t="shared" ref="AD40:AD62" si="13">"."&amp;B40</f>
+        <v>.</v>
       </c>
       <c r="AG40" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.Instrument = sqlInstrument.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="41" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="B41" s="1"/>
       <c r="D41" t="str">
         <f t="shared" si="8"/>
-        <v>PortfolioName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="9"/>
-        <v>PortfolioName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="10"/>
-        <v>PortfolioName:    returnRecord.PortfolioName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="11"/>
-        <v>PortfolioName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L41" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V41" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList.PortfolioName = PortfolioName.String</v>
-      </c>
-      <c r="V41" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD41" t="str">
         <f t="shared" si="13"/>
-        <v>item.PortfolioName = r.FormValue("PortfolioName")</v>
-      </c>
-      <c r="AD41" t="str">
-        <f t="shared" si="14"/>
-        <v>.PortfolioName</v>
+        <v>.</v>
       </c>
       <c r="AG41" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.PortfolioName = sqlPortfolioName.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="42" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="B42" s="1"/>
       <c r="D42" t="str">
         <f t="shared" si="8"/>
-        <v>RVDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="9"/>
-        <v>RVDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="10"/>
-        <v>RVDate:    returnRecord.RVDate,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="11"/>
-        <v>RVDate:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L42" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V42" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList.RVDate = RVDate.String</v>
-      </c>
-      <c r="V42" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD42" t="str">
         <f t="shared" si="13"/>
-        <v>item.RVDate = r.FormValue("RVDate")</v>
-      </c>
-      <c r="AD42" t="str">
-        <f t="shared" si="14"/>
-        <v>.RVDate</v>
+        <v>.</v>
       </c>
       <c r="AG42" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.RVDate = sqlRVDate.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="43" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="B43" s="1"/>
       <c r="D43" t="str">
         <f t="shared" si="8"/>
-        <v>RVMTM    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="9"/>
-        <v>RVMTM    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="10"/>
-        <v>RVMTM:    returnRecord.RVMTM,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="11"/>
-        <v>RVMTM:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L43" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V43" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList.RVMTM = RVMTM.String</v>
-      </c>
-      <c r="V43" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD43" t="str">
         <f t="shared" si="13"/>
-        <v>item.RVMTM = r.FormValue("RVMTM")</v>
-      </c>
-      <c r="AD43" t="str">
-        <f t="shared" si="14"/>
-        <v>.RVMTM</v>
+        <v>.</v>
       </c>
       <c r="AG43" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.RVMTM = sqlRVMTM.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="44" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="B44" s="1"/>
       <c r="D44" t="str">
         <f t="shared" si="8"/>
-        <v>CounterBook    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="9"/>
-        <v>CounterBook    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="10"/>
-        <v>CounterBook:    returnRecord.CounterBook,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="11"/>
-        <v>CounterBook:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L44" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V44" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList.CounterBook = CounterBook.String</v>
-      </c>
-      <c r="V44" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD44" t="str">
         <f t="shared" si="13"/>
-        <v>item.CounterBook = r.FormValue("CounterBook")</v>
-      </c>
-      <c r="AD44" t="str">
-        <f t="shared" si="14"/>
-        <v>.CounterBook</v>
+        <v>.</v>
       </c>
       <c r="AG44" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.CounterBook = sqlCounterBook.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="45" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="B45" s="1"/>
       <c r="D45" t="str">
         <f t="shared" si="8"/>
-        <v>CounterBookName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="9"/>
-        <v>CounterBookName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="10"/>
-        <v>CounterBookName:    returnRecord.CounterBookName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="11"/>
-        <v>CounterBookName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L45" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V45" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList.CounterBookName = CounterBookName.String</v>
-      </c>
-      <c r="V45" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD45" t="str">
         <f t="shared" si="13"/>
-        <v>item.CounterBookName = r.FormValue("CounterBookName")</v>
-      </c>
-      <c r="AD45" t="str">
-        <f t="shared" si="14"/>
-        <v>.CounterBookName</v>
+        <v>.</v>
       </c>
       <c r="AG45" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.CounterBookName = sqlCounterBookName.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="46" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="B46" s="1"/>
       <c r="D46" t="str">
         <f t="shared" si="8"/>
-        <v>Party    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="9"/>
-        <v>Party    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="10"/>
-        <v>Party:    returnRecord.Party,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="11"/>
-        <v>Party:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L46" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V46" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList.Party = Party.String</v>
-      </c>
-      <c r="V46" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD46" t="str">
         <f t="shared" si="13"/>
-        <v>item.Party = r.FormValue("Party")</v>
-      </c>
-      <c r="AD46" t="str">
-        <f t="shared" si="14"/>
-        <v>.Party</v>
+        <v>.</v>
       </c>
       <c r="AG46" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.Party = sqlParty.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="47" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="B47" s="1"/>
       <c r="D47" t="str">
         <f t="shared" si="8"/>
-        <v>PartyName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="9"/>
-        <v>PartyName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="10"/>
-        <v>PartyName:    returnRecord.PartyName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="11"/>
-        <v>PartyName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L47" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V47" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList.PartyName = PartyName.String</v>
-      </c>
-      <c r="V47" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD47" t="str">
         <f t="shared" si="13"/>
-        <v>item.PartyName = r.FormValue("PartyName")</v>
-      </c>
-      <c r="AD47" t="str">
-        <f t="shared" si="14"/>
-        <v>.PartyName</v>
+        <v>.</v>
       </c>
       <c r="AG47" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList.PartyName = sqlPartyName.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="48" spans="2:33" x14ac:dyDescent="0.2">
@@ -2241,20 +2102,20 @@
         <v>:    "",</v>
       </c>
       <c r="L48" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V48" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V48" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD48" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD48" t="str">
-        <f t="shared" si="14"/>
         <v>.</v>
       </c>
       <c r="AG48" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList. = sql.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="49" spans="2:33" x14ac:dyDescent="0.2">
@@ -2276,20 +2137,20 @@
         <v>:    "",</v>
       </c>
       <c r="L49" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V49" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V49" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD49" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD49" t="str">
-        <f t="shared" si="14"/>
         <v>.</v>
       </c>
       <c r="AG49" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList. = sql.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="50" spans="2:33" x14ac:dyDescent="0.2">
@@ -2311,20 +2172,20 @@
         <v>:    "",</v>
       </c>
       <c r="L50" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V50" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V50" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD50" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD50" t="str">
-        <f t="shared" si="14"/>
         <v>.</v>
       </c>
       <c r="AG50" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList. = sql.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="51" spans="2:33" x14ac:dyDescent="0.2">
@@ -2346,20 +2207,20 @@
         <v>:    "",</v>
       </c>
       <c r="L51" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V51" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V51" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD51" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD51" t="str">
-        <f t="shared" si="14"/>
         <v>.</v>
       </c>
       <c r="AG51" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList. = sql.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="52" spans="2:33" x14ac:dyDescent="0.2">
@@ -2381,20 +2242,20 @@
         <v>:    "",</v>
       </c>
       <c r="L52" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V52" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V52" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD52" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD52" t="str">
-        <f t="shared" si="14"/>
         <v>.</v>
       </c>
       <c r="AG52" t="str">
         <f t="shared" si="7"/>
-        <v>sienaDealList. = sql.String</v>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="53" spans="2:33" x14ac:dyDescent="0.2">
@@ -2416,16 +2277,20 @@
         <v>:    "",</v>
       </c>
       <c r="L53" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V53" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V53" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD53" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD53" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG53" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="54" spans="2:33" x14ac:dyDescent="0.2">
@@ -2447,16 +2312,20 @@
         <v>:    "",</v>
       </c>
       <c r="L54" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V54" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V54" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD54" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD54" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG54" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="55" spans="2:33" x14ac:dyDescent="0.2">
@@ -2478,16 +2347,20 @@
         <v>:    "",</v>
       </c>
       <c r="L55" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V55" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V55" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD55" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD55" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG55" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="56" spans="2:33" x14ac:dyDescent="0.2">
@@ -2509,16 +2382,20 @@
         <v>:    "",</v>
       </c>
       <c r="L56" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V56" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V56" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD56" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD56" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG56" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="57" spans="2:33" x14ac:dyDescent="0.2">
@@ -2540,16 +2417,20 @@
         <v>:    "",</v>
       </c>
       <c r="L57" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V57" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V57" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD57" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD57" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG57" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="58" spans="2:33" x14ac:dyDescent="0.2">
@@ -2571,16 +2452,20 @@
         <v>:    "",</v>
       </c>
       <c r="L58" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V58" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V58" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD58" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD58" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG58" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="59" spans="2:33" x14ac:dyDescent="0.2">
@@ -2602,16 +2487,20 @@
         <v>:    "",</v>
       </c>
       <c r="L59" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V59" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V59" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD59" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD59" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG59" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="60" spans="2:33" x14ac:dyDescent="0.2">
@@ -2633,16 +2522,20 @@
         <v>:    "",</v>
       </c>
       <c r="L60" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V60" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V60" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD60" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD60" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG60" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="61" spans="2:33" x14ac:dyDescent="0.2">
@@ -2664,16 +2557,20 @@
         <v>:    "",</v>
       </c>
       <c r="L61" t="str">
+        <f t="shared" si="6"/>
+        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+      </c>
+      <c r="V61" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V61" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD61" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD61" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG61" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="62" spans="2:33" x14ac:dyDescent="0.2">
@@ -2695,16 +2592,20 @@
         <v>:    "",</v>
       </c>
       <c r="L62" t="str">
+        <f t="shared" ref="L40:L62" si="14">$I$3&amp;"."&amp;B62&amp;" = "&amp;B62&amp;".String"</f>
+        <v>sienaAccountTransactions. = .String</v>
+      </c>
+      <c r="V62" t="str">
         <f t="shared" si="12"/>
-        <v>sienaDealList. = .String</v>
-      </c>
-      <c r="V62" t="str">
+        <v>item. = r.FormValue("")</v>
+      </c>
+      <c r="AD62" t="str">
         <f t="shared" si="13"/>
-        <v>item. = r.FormValue("")</v>
-      </c>
-      <c r="AD62" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
+        <v>.</v>
+      </c>
+      <c r="AG62" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="63" spans="2:33" x14ac:dyDescent="0.2">
@@ -2727,7 +2628,7 @@
       </c>
       <c r="L63" t="str">
         <f t="shared" ref="L63:L74" si="19">$I$3&amp;"."&amp;B63&amp;" = "&amp;B63&amp;".String"</f>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V63" t="str">
         <f t="shared" ref="V63:V74" si="20">"item."&amp;B63&amp;" = r.FormValue("""&amp;B63&amp;""")"</f>
@@ -2736,6 +2637,10 @@
       <c r="AD63" t="str">
         <f t="shared" ref="AD63:AD74" si="21">"."&amp;B63</f>
         <v>.</v>
+      </c>
+      <c r="AG63" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
     <row r="64" spans="2:33" x14ac:dyDescent="0.2">
@@ -2758,7 +2663,7 @@
       </c>
       <c r="L64" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V64" t="str">
         <f t="shared" si="20"/>
@@ -2768,8 +2673,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="65" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG64" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="65" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B65" s="1"/>
       <c r="D65" t="str">
         <f t="shared" si="15"/>
@@ -2789,7 +2698,7 @@
       </c>
       <c r="L65" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V65" t="str">
         <f t="shared" si="20"/>
@@ -2799,8 +2708,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="66" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG65" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="66" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B66" s="1"/>
       <c r="D66" t="str">
         <f t="shared" si="15"/>
@@ -2820,7 +2733,7 @@
       </c>
       <c r="L66" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V66" t="str">
         <f t="shared" si="20"/>
@@ -2830,8 +2743,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="67" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG66" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="67" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B67" s="1"/>
       <c r="D67" t="str">
         <f t="shared" si="15"/>
@@ -2851,7 +2768,7 @@
       </c>
       <c r="L67" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V67" t="str">
         <f t="shared" si="20"/>
@@ -2861,8 +2778,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="68" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG67" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="68" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B68" s="1"/>
       <c r="D68" t="str">
         <f t="shared" si="15"/>
@@ -2882,7 +2803,7 @@
       </c>
       <c r="L68" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V68" t="str">
         <f t="shared" si="20"/>
@@ -2892,8 +2813,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="69" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG68" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="69" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B69" s="1"/>
       <c r="D69" t="str">
         <f t="shared" si="15"/>
@@ -2913,7 +2838,7 @@
       </c>
       <c r="L69" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V69" t="str">
         <f t="shared" si="20"/>
@@ -2923,8 +2848,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="70" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG69" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="70" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B70" s="1"/>
       <c r="D70" t="str">
         <f t="shared" si="15"/>
@@ -2944,7 +2873,7 @@
       </c>
       <c r="L70" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V70" t="str">
         <f t="shared" si="20"/>
@@ -2954,8 +2883,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="71" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG70" t="str">
+        <f t="shared" si="7"/>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="71" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B71" s="1"/>
       <c r="D71" t="str">
         <f t="shared" si="15"/>
@@ -2975,7 +2908,7 @@
       </c>
       <c r="L71" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V71" t="str">
         <f t="shared" si="20"/>
@@ -2985,8 +2918,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="72" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG71" t="str">
+        <f t="shared" ref="AG71:AG74" si="22">$I$3&amp;"."&amp;B71&amp;" = sql"&amp;B71&amp;".String"</f>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="72" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B72" s="1"/>
       <c r="D72" t="str">
         <f t="shared" si="15"/>
@@ -3006,7 +2943,7 @@
       </c>
       <c r="L72" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V72" t="str">
         <f t="shared" si="20"/>
@@ -3016,8 +2953,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="73" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG72" t="str">
+        <f t="shared" si="22"/>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="73" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B73" s="1"/>
       <c r="D73" t="str">
         <f t="shared" si="15"/>
@@ -3037,7 +2978,7 @@
       </c>
       <c r="L73" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V73" t="str">
         <f t="shared" si="20"/>
@@ -3047,8 +2988,12 @@
         <f t="shared" si="21"/>
         <v>.</v>
       </c>
-    </row>
-    <row r="74" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG73" t="str">
+        <f t="shared" si="22"/>
+        <v>sienaAccountTransactions. = sql.String</v>
+      </c>
+    </row>
+    <row r="74" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B74" s="1"/>
       <c r="D74" t="str">
         <f t="shared" si="15"/>
@@ -3068,7 +3013,7 @@
       </c>
       <c r="L74" t="str">
         <f t="shared" si="19"/>
-        <v>sienaDealList. = .String</v>
+        <v>sienaAccountTransactions. = .String</v>
       </c>
       <c r="V74" t="str">
         <f t="shared" si="20"/>
@@ -3077,6 +3022,10 @@
       <c r="AD74" t="str">
         <f t="shared" si="21"/>
         <v>.</v>
+      </c>
+      <c r="AG74" t="str">
+        <f t="shared" si="22"/>
+        <v>sienaAccountTransactions. = sql.String</v>
       </c>
     </row>
   </sheetData>
@@ -3086,19 +3035,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90230AA-F0B1-6C49-B8FC-2C26A6B44982}">
-  <dimension ref="B6:BK15"/>
+  <dimension ref="A3:BK15"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AR15" sqref="C15:AR15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="19" max="20" width="24.5" customWidth="1"/>
+    <col min="44" max="44" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:63" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="C3" t="str">
+        <f>UPPER('GO Struct Bits'!B2)</f>
+        <v>ACCTTX</v>
+      </c>
+    </row>
+    <row r="6" spans="1:63" x14ac:dyDescent="0.2">
       <c r="B6" cm="1">
         <f t="array" ref="B6:AU6">TRANSPOSE('GO Struct Bits'!B5:B50)</f>
         <v>0</v>
@@ -3107,127 +3064,127 @@
         <v>SienaReference</v>
       </c>
       <c r="D6" t="str">
-        <v>CustomerSienaView</v>
+        <v>LegNo</v>
       </c>
       <c r="E6" t="str">
-        <v>Status</v>
+        <v>MMLegNo</v>
       </c>
       <c r="F6" t="str">
-        <v>ValueDate</v>
+        <v>Narrative</v>
       </c>
       <c r="G6" t="str">
-        <v>MaturityDate</v>
+        <v>Amount</v>
       </c>
       <c r="H6" t="str">
-        <v>ContractNumber</v>
+        <v>StartInterestDate</v>
       </c>
       <c r="I6" t="str">
-        <v>ExternalReference</v>
+        <v>EndInterestDate</v>
       </c>
       <c r="J6" t="str">
-        <v>Book</v>
+        <v>Amortisation</v>
       </c>
       <c r="K6" t="str">
-        <v>MandatedUser</v>
+        <v>InterestAmount</v>
       </c>
       <c r="L6" t="str">
-        <v>Portfolio</v>
+        <v>InterestAction</v>
       </c>
       <c r="M6" t="str">
-        <v>AgreementId</v>
+        <v>FixingDate</v>
       </c>
       <c r="N6" t="str">
-        <v>BackOfficeRefNo</v>
+        <v>InterestCalculationDate</v>
       </c>
       <c r="O6" t="str">
-        <v>ISIN</v>
-      </c>
-      <c r="P6" t="str">
-        <v>UTI</v>
-      </c>
-      <c r="Q6" t="str">
-        <v>BookName</v>
-      </c>
-      <c r="R6" t="str">
-        <v>Centre</v>
-      </c>
-      <c r="S6" t="str">
-        <v>Firm</v>
-      </c>
-      <c r="T6" t="str">
-        <v>DealTypeShortName</v>
-      </c>
-      <c r="U6" t="str">
-        <v>FullDealType</v>
-      </c>
-      <c r="V6" t="str">
-        <v>TradeDate</v>
-      </c>
-      <c r="W6" t="str">
-        <v>DealtCcy</v>
-      </c>
-      <c r="X6" t="str">
-        <v>DealtAmount</v>
-      </c>
-      <c r="Y6" t="str">
-        <v>AgainstAmount</v>
-      </c>
-      <c r="Z6" t="str">
-        <v>AgainstCcy</v>
-      </c>
-      <c r="AA6" t="str">
-        <v>AllInRate</v>
-      </c>
-      <c r="AB6" t="str">
-        <v>MktRate</v>
-      </c>
-      <c r="AC6" t="str">
-        <v>SettleCcy</v>
-      </c>
-      <c r="AD6" t="str">
-        <v>Direction</v>
-      </c>
-      <c r="AE6" t="str">
-        <v>NpvRate</v>
-      </c>
-      <c r="AF6" t="str">
-        <v>OriginUser</v>
-      </c>
-      <c r="AG6" t="str">
-        <v>PayInstruction</v>
-      </c>
-      <c r="AH6" t="str">
-        <v>ReceiptInstruction</v>
-      </c>
-      <c r="AI6" t="str">
-        <v>NIName</v>
-      </c>
-      <c r="AJ6" t="str">
-        <v>CCYPair</v>
-      </c>
-      <c r="AK6" t="str">
-        <v>Instrument</v>
-      </c>
-      <c r="AL6" t="str">
-        <v>PortfolioName</v>
-      </c>
-      <c r="AM6" t="str">
-        <v>RVDate</v>
-      </c>
-      <c r="AN6" t="str">
-        <v>RVMTM</v>
-      </c>
-      <c r="AO6" t="str">
-        <v>CounterBook</v>
-      </c>
-      <c r="AP6" t="str">
-        <v>CounterBookName</v>
-      </c>
-      <c r="AQ6" t="str">
-        <v>Party</v>
-      </c>
-      <c r="AR6" t="str">
-        <v>PartyName</v>
+        <v>AmendmentAmount</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
       </c>
       <c r="AS6">
         <v>0</v>
@@ -3239,9 +3196,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:63" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>1</v>
+    <row r="8" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"var siena"&amp;'GO Struct Bits'!B4&amp;"SQL"</f>
+        <v>var sienaAccountTransactionsSQL</v>
       </c>
       <c r="C8" t="str">
         <f>C6&amp;", "</f>
@@ -3249,167 +3210,167 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" ref="D8:BK8" si="0">D6&amp;", "</f>
-        <v xml:space="preserve">CustomerSienaView, </v>
+        <v xml:space="preserve">LegNo, </v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Status, </v>
+        <v xml:space="preserve">MMLegNo, </v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ValueDate, </v>
+        <v xml:space="preserve">Narrative, </v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">MaturityDate, </v>
+        <v xml:space="preserve">Amount, </v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ContractNumber, </v>
+        <v xml:space="preserve">StartInterestDate, </v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ExternalReference, </v>
+        <v xml:space="preserve">EndInterestDate, </v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Book, </v>
+        <v xml:space="preserve">Amortisation, </v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">MandatedUser, </v>
+        <v xml:space="preserve">InterestAmount, </v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Portfolio, </v>
+        <v xml:space="preserve">InterestAction, </v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">AgreementId, </v>
+        <v xml:space="preserve">FixingDate, </v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">BackOfficeRefNo, </v>
+        <v xml:space="preserve">InterestCalculationDate, </v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ISIN, </v>
+        <v xml:space="preserve">AmendmentAmount, </v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">UTI, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">BookName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Centre, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Firm, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DealTypeShortName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">FullDealType, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">TradeDate, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DealtCcy, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="X8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DealtAmount, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">AgainstAmount, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">AgainstCcy, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">AllInRate, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">MktRate, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AC8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SettleCcy, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Direction, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AE8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">NpvRate, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AF8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">OriginUser, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AG8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PayInstruction, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AH8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ReceiptInstruction, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AI8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">NIName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AJ8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CCYPair, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AK8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Instrument, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AL8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PortfolioName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AM8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">RVDate, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AN8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">RVMTM, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AO8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CounterBook, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AP8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CounterBookName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AQ8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Party, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AR8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PartyName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AS8" t="str">
         <f t="shared" si="0"/>
@@ -3488,174 +3449,174 @@
         <v xml:space="preserve">, </v>
       </c>
     </row>
-    <row r="10" spans="2:63" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C10" t="str">
         <f>"&amp;"&amp;C8</f>
         <v xml:space="preserve">&amp;SienaReference, </v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ref="D10:BK10" si="1">"&amp;"&amp;D8</f>
-        <v xml:space="preserve">&amp;CustomerSienaView, </v>
+        <v xml:space="preserve">&amp;LegNo, </v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Status, </v>
+        <v xml:space="preserve">&amp;MMLegNo, </v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ValueDate, </v>
+        <v xml:space="preserve">&amp;Narrative, </v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;MaturityDate, </v>
+        <v xml:space="preserve">&amp;Amount, </v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ContractNumber, </v>
+        <v xml:space="preserve">&amp;StartInterestDate, </v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ExternalReference, </v>
+        <v xml:space="preserve">&amp;EndInterestDate, </v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Book, </v>
+        <v xml:space="preserve">&amp;Amortisation, </v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;MandatedUser, </v>
+        <v xml:space="preserve">&amp;InterestAmount, </v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Portfolio, </v>
+        <v xml:space="preserve">&amp;InterestAction, </v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;AgreementId, </v>
+        <v xml:space="preserve">&amp;FixingDate, </v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;BackOfficeRefNo, </v>
+        <v xml:space="preserve">&amp;InterestCalculationDate, </v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ISIN, </v>
+        <v xml:space="preserve">&amp;AmendmentAmount, </v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;UTI, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;BookName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="R10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Centre, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Firm, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="T10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;DealTypeShortName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="U10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;FullDealType, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;TradeDate, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;DealtCcy, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;DealtAmount, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;AgainstAmount, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;AgainstCcy, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;AllInRate, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;MktRate, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AC10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;SettleCcy, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Direction, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AE10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;NpvRate, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AF10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;OriginUser, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AG10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;PayInstruction, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AH10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ReceiptInstruction, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AI10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;NIName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AJ10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;CCYPair, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AK10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Instrument, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AL10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;PortfolioName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AM10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;RVDate, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AN10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;RVMTM, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AO10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;CounterBook, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AP10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;CounterBookName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AQ10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Party, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AR10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;PartyName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AS10" t="str">
         <f t="shared" si="1"/>
@@ -3734,344 +3695,372 @@
         <v xml:space="preserve">&amp;, </v>
       </c>
     </row>
-    <row r="13" spans="2:63" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C13" t="str">
-        <f>"sql"&amp;C8</f>
-        <v xml:space="preserve">sqlSienaReference, </v>
+        <f>"sql"&amp;$C$3&amp;""&amp;C8</f>
+        <v xml:space="preserve">sqlACCTTXSienaReference, </v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ref="D13:AR13" si="2">"sql"&amp;D8</f>
-        <v xml:space="preserve">sqlCustomerSienaView, </v>
+        <f t="shared" ref="D13:AY13" si="2">"sql"&amp;$C$3&amp;""&amp;D8</f>
+        <v xml:space="preserve">sqlACCTTXLegNo, </v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlStatus, </v>
+        <v xml:space="preserve">sqlACCTTXMMLegNo, </v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlValueDate, </v>
+        <v xml:space="preserve">sqlACCTTXNarrative, </v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlMaturityDate, </v>
+        <v xml:space="preserve">sqlACCTTXAmount, </v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlContractNumber, </v>
+        <v xml:space="preserve">sqlACCTTXStartInterestDate, </v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlExternalReference, </v>
+        <v xml:space="preserve">sqlACCTTXEndInterestDate, </v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlBook, </v>
+        <v xml:space="preserve">sqlACCTTXAmortisation, </v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlMandatedUser, </v>
+        <v xml:space="preserve">sqlACCTTXInterestAmount, </v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlPortfolio, </v>
+        <v xml:space="preserve">sqlACCTTXInterestAction, </v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlAgreementId, </v>
+        <v xml:space="preserve">sqlACCTTXFixingDate, </v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlBackOfficeRefNo, </v>
+        <v xml:space="preserve">sqlACCTTXInterestCalculationDate, </v>
       </c>
       <c r="O13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlISIN, </v>
+        <v xml:space="preserve">sqlACCTTXAmendmentAmount, </v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlUTI, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlBookName, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCentre, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlFirm, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlDealTypeShortName, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlFullDealType, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlTradeDate, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlDealtCcy, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlDealtAmount, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlAgainstAmount, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlAgainstCcy, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlAllInRate, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlMktRate, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AC13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlSettleCcy, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlDirection, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlNpvRate, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AF13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlOriginUser, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AG13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlPayInstruction, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AH13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlReceiptInstruction, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AI13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlNIName, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AJ13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCCYPair, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AK13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlInstrument, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AL13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlPortfolioName, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AM13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlRVDate, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AN13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlRVMTM, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AO13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCounterBook, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AP13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCounterBookName, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AQ13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlParty, </v>
+        <v xml:space="preserve">sqlACCTTX0, </v>
       </c>
       <c r="AR13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlPartyName, </v>
-      </c>
-    </row>
-    <row r="15" spans="2:63" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">sqlACCTTX0, </v>
+      </c>
+      <c r="AS13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">sqlACCTTX0, </v>
+      </c>
+      <c r="AT13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">sqlACCTTX0, </v>
+      </c>
+      <c r="AU13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">sqlACCTTX0, </v>
+      </c>
+      <c r="AV13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">sqlACCTTX, </v>
+      </c>
+      <c r="AW13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">sqlACCTTX, </v>
+      </c>
+      <c r="AX13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">sqlACCTTX, </v>
+      </c>
+      <c r="AY13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">sqlACCTTX, </v>
+      </c>
+    </row>
+    <row r="15" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C15" t="str">
         <f>"&amp;"&amp;C13</f>
-        <v xml:space="preserve">&amp;sqlSienaReference, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXSienaReference, </v>
       </c>
       <c r="D15" t="str">
         <f t="shared" ref="D15:AR15" si="3">"&amp;"&amp;D13</f>
-        <v xml:space="preserve">&amp;sqlCustomerSienaView, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXLegNo, </v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlStatus, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXMMLegNo, </v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlValueDate, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXNarrative, </v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlMaturityDate, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXAmount, </v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlContractNumber, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXStartInterestDate, </v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlExternalReference, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXEndInterestDate, </v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlBook, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXAmortisation, </v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlMandatedUser, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXInterestAmount, </v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlPortfolio, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXInterestAction, </v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlAgreementId, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXFixingDate, </v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlBackOfficeRefNo, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXInterestCalculationDate, </v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlISIN, </v>
+        <v xml:space="preserve">&amp;sqlACCTTXAmendmentAmount, </v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlUTI, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlBookName, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCentre, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlFirm, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlDealTypeShortName, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlFullDealType, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlTradeDate, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlDealtCcy, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlDealtAmount, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlAgainstAmount, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlAgainstCcy, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlAllInRate, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlMktRate, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AC15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlSettleCcy, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlDirection, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AE15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlNpvRate, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AF15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlOriginUser, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AG15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlPayInstruction, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AH15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlReceiptInstruction, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AI15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlNIName, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AJ15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCCYPair, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AK15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlInstrument, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AL15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlPortfolioName, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AM15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlRVDate, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AN15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlRVMTM, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AO15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCounterBook, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AP15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCounterBookName, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AQ15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlParty, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
       <c r="AR15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlPartyName, </v>
+        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on roles based navigation and pages
</commit_message>
<xml_diff>
--- a/design/sienaDataArraysBuilder.xlsx
+++ b/design/sienaDataArraysBuilder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matttownsend/go/mwt-go-dev/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA2F37-671D-8B41-B3EA-29939BE584C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41EFCA0-DD22-964A-A3D1-EE0916C610B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38120" yWindow="-4940" windowWidth="34980" windowHeight="18940" xr2:uid="{8265F428-BA81-814D-9171-A3F66298AE69}"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="26320" windowHeight="18000" activeTab="1" xr2:uid="{8265F428-BA81-814D-9171-A3F66298AE69}"/>
   </bookViews>
   <sheets>
     <sheet name="GO Struct Bits" sheetId="1" r:id="rId1"/>
@@ -58,70 +58,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>returnRecord.</t>
   </si>
   <si>
+    <t>var</t>
+  </si>
+  <si>
     <t>getSienaCounterpartyList</t>
   </si>
   <si>
-    <t>SienaReference</t>
-  </si>
-  <si>
     <t xml:space="preserve">getSiena…List </t>
   </si>
   <si>
+    <t>SortCode</t>
+  </si>
+  <si>
     <t>&gt;&gt;&gt;</t>
   </si>
   <si>
-    <t>LegNo</t>
-  </si>
-  <si>
-    <t>MMLegNo</t>
-  </si>
-  <si>
-    <t>Narrative</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>StartInterestDate</t>
-  </si>
-  <si>
-    <t>EndInterestDate</t>
-  </si>
-  <si>
-    <t>Amortisation</t>
-  </si>
-  <si>
-    <t>InterestAmount</t>
-  </si>
-  <si>
-    <t>InterestAction</t>
-  </si>
-  <si>
-    <t>FixingDate</t>
-  </si>
-  <si>
-    <t>InterestCalculationDate</t>
-  </si>
-  <si>
-    <t>AmendmentAmount</t>
-  </si>
-  <si>
-    <t>AccountTransactions</t>
-  </si>
-  <si>
-    <t>ACCTTX</t>
+    <t>http://mstat152.co.uk/service.php?s=click&amp;mm=2CHO03600120001475081010570039100000261500002781533&amp;lid=6187</t>
+  </si>
+  <si>
+    <t>ROWS&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>NameCentre</t>
+  </si>
+  <si>
+    <t>NameFirm</t>
+  </si>
+  <si>
+    <t>BICCode</t>
+  </si>
+  <si>
+    <t>ContactIndicator</t>
+  </si>
+  <si>
+    <t>CoverTrade</t>
+  </si>
+  <si>
+    <t>CustomerCategory</t>
+  </si>
+  <si>
+    <t>FSCSInclusive</t>
+  </si>
+  <si>
+    <t>FeeFactor</t>
+  </si>
+  <si>
+    <t>InactiveStatus</t>
+  </si>
+  <si>
+    <t>Indemnity</t>
+  </si>
+  <si>
+    <t>KnowYourCustomerStatus</t>
+  </si>
+  <si>
+    <t>LERLimitCarveOut</t>
+  </si>
+  <si>
+    <t>LastAmended</t>
+  </si>
+  <si>
+    <t>LastLogin</t>
+  </si>
+  <si>
+    <t>LossGivenDefault</t>
+  </si>
+  <si>
+    <t>MIC</t>
+  </si>
+  <si>
+    <t>ProtectedDepositor</t>
+  </si>
+  <si>
+    <t>RPTCurrency</t>
+  </si>
+  <si>
+    <t>RateTimeout</t>
+  </si>
+  <si>
+    <t>RateValidation</t>
+  </si>
+  <si>
+    <t>Registered</t>
+  </si>
+  <si>
+    <t>RegulatoryCategory</t>
+  </si>
+  <si>
+    <t>SecuredSettlement</t>
+  </si>
+  <si>
+    <t>SettlementLimitCarveOut</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>TrainingCode</t>
+  </si>
+  <si>
+    <t>TrainingReceived</t>
+  </si>
+  <si>
+    <t>Unencumbered</t>
+  </si>
+  <si>
+    <t>LEIExpiryDate</t>
+  </si>
+  <si>
+    <t>MIFIDReviewDate</t>
+  </si>
+  <si>
+    <t>GDPRReviewDate</t>
+  </si>
+  <si>
+    <t>DelegatedReporting</t>
+  </si>
+  <si>
+    <t>BOReconcile</t>
+  </si>
+  <si>
+    <t>MIFIDReportableDealsAllowed</t>
+  </si>
+  <si>
+    <t>SignedInvestmentAgreement</t>
+  </si>
+  <si>
+    <t>AppropriatenessAssessment</t>
+  </si>
+  <si>
+    <t>FinancialCounterparty</t>
+  </si>
+  <si>
+    <t>Collateralisation</t>
+  </si>
+  <si>
+    <t>PortfolioCode</t>
+  </si>
+  <si>
+    <t>ReconciliationLetterFrequency</t>
+  </si>
+  <si>
+    <t>DirectDealing</t>
+  </si>
+  <si>
+    <t>CounterpartyExtensions</t>
+  </si>
+  <si>
+    <t>CPEX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,6 +243,14 @@
     <font>
       <sz val="12"/>
       <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,19 +298,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -522,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4CE648-3973-0F42-A3A6-4E494BE264E6}">
   <dimension ref="B2:AG74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,40 +655,40 @@
   <sheetData>
     <row r="2" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D2" t="str">
         <f>"siena"&amp;B4&amp;".go"</f>
-        <v>sienaAccountTransactions.go</v>
+        <v>sienaCounterpartyExtensions.go</v>
       </c>
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.2">
       <c r="I3" t="str">
         <f>"siena"&amp;B4</f>
-        <v>sienaAccountTransactions</v>
+        <v>sienaCounterpartyExtensions</v>
       </c>
     </row>
     <row r="4" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>"siena"&amp;B4&amp;"Page"</f>
-        <v>sienaAccountTransactionsPage</v>
+        <v>sienaCounterpartyExtensionsPage</v>
       </c>
       <c r="E4" s="2" t="str">
         <f>"siena"&amp;B4&amp;"Item"</f>
-        <v>sienaAccountTransactionsItem</v>
+        <v>sienaCounterpartyExtensionsItem</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="str">
         <f>"newSiena"&amp;B4&amp;"Handler"</f>
-        <v>newSienaAccountTransactionsHandler</v>
+        <v>newSienaCounterpartyExtensionsHandler</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG4" t="s">
         <v>3</v>
@@ -589,1498 +696,1556 @@
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ref="D6:D39" si="0">B6&amp;"    string"</f>
-        <v>SienaReference    string</v>
+        <v>NameFirm    string</v>
       </c>
       <c r="E6" t="str">
         <f>D6</f>
-        <v>SienaReference    string</v>
+        <v>NameFirm    string</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ref="G6:G39" si="1">B6&amp;":    "&amp;$F$4&amp;B6&amp;","</f>
-        <v>SienaReference:    returnRecord.SienaReference,</v>
+        <v>NameFirm:    returnRecord.NameFirm,</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" ref="H6:H39" si="2">B6&amp;":    """""&amp;","</f>
-        <v>SienaReference:    "",</v>
+        <v>NameFirm:    "",</v>
       </c>
       <c r="L6" t="str">
         <f>$I$3&amp;"."&amp;B6&amp;" = sql"&amp;$B$2&amp;B6&amp;".String"</f>
-        <v>sienaAccountTransactions.SienaReference = sqlACCTTXSienaReference.String</v>
+        <v>sienaCounterpartyExtensions.NameFirm = sqlCPEXNameFirm.String</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" ref="V6:V39" si="3">"item."&amp;B6&amp;" = r.FormValue("""&amp;B6&amp;""")"</f>
-        <v>item.SienaReference = r.FormValue("SienaReference")</v>
+        <v>item.NameFirm = r.FormValue("NameFirm")</v>
       </c>
       <c r="AD6" t="str">
         <f t="shared" ref="AD6:AD39" si="4">"."&amp;B6</f>
-        <v>.SienaReference</v>
+        <v>.NameFirm</v>
       </c>
       <c r="AG6" t="str">
         <f>$I$3&amp;"."&amp;B6&amp;" = sql"&amp;B6&amp;".String"</f>
-        <v>sienaAccountTransactions.SienaReference = sqlSienaReference.String</v>
+        <v>sienaCounterpartyExtensions.NameFirm = sqlNameFirm.String</v>
       </c>
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>LegNo    string</v>
+        <v>NameCentre    string</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" ref="E7:E39" si="5">D7</f>
-        <v>LegNo    string</v>
+        <v>NameCentre    string</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>LegNo:    returnRecord.LegNo,</v>
+        <v>NameCentre:    returnRecord.NameCentre,</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="2"/>
-        <v>LegNo:    "",</v>
+        <v>NameCentre:    "",</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ref="L7:L61" si="6">$I$3&amp;"."&amp;B7&amp;" = sql"&amp;$B$2&amp;B7&amp;".String"</f>
-        <v>sienaAccountTransactions.LegNo = sqlACCTTXLegNo.String</v>
+        <v>sienaCounterpartyExtensions.NameCentre = sqlCPEXNameCentre.String</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="3"/>
-        <v>item.LegNo = r.FormValue("LegNo")</v>
+        <v>item.NameCentre = r.FormValue("NameCentre")</v>
       </c>
       <c r="AD7" t="str">
         <f t="shared" si="4"/>
-        <v>.LegNo</v>
+        <v>.NameCentre</v>
       </c>
       <c r="AG7" t="str">
         <f t="shared" ref="AG7:AG70" si="7">$I$3&amp;"."&amp;B7&amp;" = sql"&amp;B7&amp;".String"</f>
-        <v>sienaAccountTransactions.LegNo = sqlLegNo.String</v>
+        <v>sienaCounterpartyExtensions.NameCentre = sqlNameCentre.String</v>
       </c>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>MMLegNo    string</v>
+        <v>BICCode    string</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="5"/>
-        <v>MMLegNo    string</v>
+        <v>BICCode    string</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>MMLegNo:    returnRecord.MMLegNo,</v>
+        <v>BICCode:    returnRecord.BICCode,</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="2"/>
-        <v>MMLegNo:    "",</v>
+        <v>BICCode:    "",</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.MMLegNo = sqlACCTTXMMLegNo.String</v>
+        <v>sienaCounterpartyExtensions.BICCode = sqlCPEXBICCode.String</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="3"/>
-        <v>item.MMLegNo = r.FormValue("MMLegNo")</v>
+        <v>item.BICCode = r.FormValue("BICCode")</v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="4"/>
-        <v>.MMLegNo</v>
+        <v>.BICCode</v>
       </c>
       <c r="AG8" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.MMLegNo = sqlMMLegNo.String</v>
+        <v>sienaCounterpartyExtensions.BICCode = sqlBICCode.String</v>
       </c>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>Narrative    string</v>
+        <v>ContactIndicator    string</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="5"/>
-        <v>Narrative    string</v>
+        <v>ContactIndicator    string</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>Narrative:    returnRecord.Narrative,</v>
+        <v>ContactIndicator:    returnRecord.ContactIndicator,</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="2"/>
-        <v>Narrative:    "",</v>
+        <v>ContactIndicator:    "",</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.Narrative = sqlACCTTXNarrative.String</v>
+        <v>sienaCounterpartyExtensions.ContactIndicator = sqlCPEXContactIndicator.String</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="3"/>
-        <v>item.Narrative = r.FormValue("Narrative")</v>
+        <v>item.ContactIndicator = r.FormValue("ContactIndicator")</v>
       </c>
       <c r="AD9" t="str">
         <f t="shared" si="4"/>
-        <v>.Narrative</v>
+        <v>.ContactIndicator</v>
       </c>
       <c r="AG9" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.Narrative = sqlNarrative.String</v>
+        <v>sienaCounterpartyExtensions.ContactIndicator = sqlContactIndicator.String</v>
       </c>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>Amount    string</v>
+        <v>CoverTrade    string</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="5"/>
-        <v>Amount    string</v>
+        <v>CoverTrade    string</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>Amount:    returnRecord.Amount,</v>
+        <v>CoverTrade:    returnRecord.CoverTrade,</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="2"/>
-        <v>Amount:    "",</v>
+        <v>CoverTrade:    "",</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.Amount = sqlACCTTXAmount.String</v>
+        <v>sienaCounterpartyExtensions.CoverTrade = sqlCPEXCoverTrade.String</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="3"/>
-        <v>item.Amount = r.FormValue("Amount")</v>
+        <v>item.CoverTrade = r.FormValue("CoverTrade")</v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="4"/>
-        <v>.Amount</v>
+        <v>.CoverTrade</v>
       </c>
       <c r="AG10" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.Amount = sqlAmount.String</v>
+        <v>sienaCounterpartyExtensions.CoverTrade = sqlCoverTrade.String</v>
       </c>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>StartInterestDate    string</v>
+        <v>CustomerCategory    string</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="5"/>
-        <v>StartInterestDate    string</v>
+        <v>CustomerCategory    string</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
-        <v>StartInterestDate:    returnRecord.StartInterestDate,</v>
+        <v>CustomerCategory:    returnRecord.CustomerCategory,</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="2"/>
-        <v>StartInterestDate:    "",</v>
+        <v>CustomerCategory:    "",</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.StartInterestDate = sqlACCTTXStartInterestDate.String</v>
+        <v>sienaCounterpartyExtensions.CustomerCategory = sqlCPEXCustomerCategory.String</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="3"/>
-        <v>item.StartInterestDate = r.FormValue("StartInterestDate")</v>
+        <v>item.CustomerCategory = r.FormValue("CustomerCategory")</v>
       </c>
       <c r="AD11" t="str">
         <f t="shared" si="4"/>
-        <v>.StartInterestDate</v>
+        <v>.CustomerCategory</v>
       </c>
       <c r="AG11" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.StartInterestDate = sqlStartInterestDate.String</v>
+        <v>sienaCounterpartyExtensions.CustomerCategory = sqlCustomerCategory.String</v>
       </c>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>EndInterestDate    string</v>
+        <v>FSCSInclusive    string</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="5"/>
-        <v>EndInterestDate    string</v>
+        <v>FSCSInclusive    string</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
-        <v>EndInterestDate:    returnRecord.EndInterestDate,</v>
+        <v>FSCSInclusive:    returnRecord.FSCSInclusive,</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="2"/>
-        <v>EndInterestDate:    "",</v>
+        <v>FSCSInclusive:    "",</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.EndInterestDate = sqlACCTTXEndInterestDate.String</v>
+        <v>sienaCounterpartyExtensions.FSCSInclusive = sqlCPEXFSCSInclusive.String</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="3"/>
-        <v>item.EndInterestDate = r.FormValue("EndInterestDate")</v>
+        <v>item.FSCSInclusive = r.FormValue("FSCSInclusive")</v>
       </c>
       <c r="AD12" t="str">
         <f t="shared" si="4"/>
-        <v>.EndInterestDate</v>
+        <v>.FSCSInclusive</v>
       </c>
       <c r="AG12" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.EndInterestDate = sqlEndInterestDate.String</v>
+        <v>sienaCounterpartyExtensions.FSCSInclusive = sqlFSCSInclusive.String</v>
       </c>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>Amortisation    string</v>
+        <v>FeeFactor    string</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="5"/>
-        <v>Amortisation    string</v>
+        <v>FeeFactor    string</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
-        <v>Amortisation:    returnRecord.Amortisation,</v>
+        <v>FeeFactor:    returnRecord.FeeFactor,</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
-        <v>Amortisation:    "",</v>
+        <v>FeeFactor:    "",</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.Amortisation = sqlACCTTXAmortisation.String</v>
+        <v>sienaCounterpartyExtensions.FeeFactor = sqlCPEXFeeFactor.String</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="3"/>
-        <v>item.Amortisation = r.FormValue("Amortisation")</v>
+        <v>item.FeeFactor = r.FormValue("FeeFactor")</v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="4"/>
-        <v>.Amortisation</v>
+        <v>.FeeFactor</v>
       </c>
       <c r="AG13" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.Amortisation = sqlAmortisation.String</v>
+        <v>sienaCounterpartyExtensions.FeeFactor = sqlFeeFactor.String</v>
       </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>InterestAmount    string</v>
+        <v>InactiveStatus    string</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="5"/>
-        <v>InterestAmount    string</v>
+        <v>InactiveStatus    string</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
-        <v>InterestAmount:    returnRecord.InterestAmount,</v>
+        <v>InactiveStatus:    returnRecord.InactiveStatus,</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="2"/>
-        <v>InterestAmount:    "",</v>
+        <v>InactiveStatus:    "",</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.InterestAmount = sqlACCTTXInterestAmount.String</v>
+        <v>sienaCounterpartyExtensions.InactiveStatus = sqlCPEXInactiveStatus.String</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="3"/>
-        <v>item.InterestAmount = r.FormValue("InterestAmount")</v>
+        <v>item.InactiveStatus = r.FormValue("InactiveStatus")</v>
       </c>
       <c r="AD14" t="str">
         <f t="shared" si="4"/>
-        <v>.InterestAmount</v>
+        <v>.InactiveStatus</v>
       </c>
       <c r="AG14" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.InterestAmount = sqlInterestAmount.String</v>
+        <v>sienaCounterpartyExtensions.InactiveStatus = sqlInactiveStatus.String</v>
       </c>
     </row>
     <row r="15" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>InterestAction    string</v>
+        <v>Indemnity    string</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="5"/>
-        <v>InterestAction    string</v>
+        <v>Indemnity    string</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>InterestAction:    returnRecord.InterestAction,</v>
+        <v>Indemnity:    returnRecord.Indemnity,</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="2"/>
-        <v>InterestAction:    "",</v>
+        <v>Indemnity:    "",</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.InterestAction = sqlACCTTXInterestAction.String</v>
+        <v>sienaCounterpartyExtensions.Indemnity = sqlCPEXIndemnity.String</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="3"/>
-        <v>item.InterestAction = r.FormValue("InterestAction")</v>
+        <v>item.Indemnity = r.FormValue("Indemnity")</v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="4"/>
-        <v>.InterestAction</v>
+        <v>.Indemnity</v>
       </c>
       <c r="AG15" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.InterestAction = sqlInterestAction.String</v>
+        <v>sienaCounterpartyExtensions.Indemnity = sqlIndemnity.String</v>
       </c>
     </row>
     <row r="16" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>FixingDate    string</v>
+        <v>KnowYourCustomerStatus    string</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="5"/>
-        <v>FixingDate    string</v>
+        <v>KnowYourCustomerStatus    string</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>FixingDate:    returnRecord.FixingDate,</v>
+        <v>KnowYourCustomerStatus:    returnRecord.KnowYourCustomerStatus,</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="2"/>
-        <v>FixingDate:    "",</v>
+        <v>KnowYourCustomerStatus:    "",</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.FixingDate = sqlACCTTXFixingDate.String</v>
+        <v>sienaCounterpartyExtensions.KnowYourCustomerStatus = sqlCPEXKnowYourCustomerStatus.String</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="3"/>
-        <v>item.FixingDate = r.FormValue("FixingDate")</v>
+        <v>item.KnowYourCustomerStatus = r.FormValue("KnowYourCustomerStatus")</v>
       </c>
       <c r="AD16" t="str">
         <f t="shared" si="4"/>
-        <v>.FixingDate</v>
+        <v>.KnowYourCustomerStatus</v>
       </c>
       <c r="AG16" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.FixingDate = sqlFixingDate.String</v>
+        <v>sienaCounterpartyExtensions.KnowYourCustomerStatus = sqlKnowYourCustomerStatus.String</v>
       </c>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>InterestCalculationDate    string</v>
+        <v>LERLimitCarveOut    string</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="5"/>
-        <v>InterestCalculationDate    string</v>
+        <v>LERLimitCarveOut    string</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>InterestCalculationDate:    returnRecord.InterestCalculationDate,</v>
+        <v>LERLimitCarveOut:    returnRecord.LERLimitCarveOut,</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="2"/>
-        <v>InterestCalculationDate:    "",</v>
+        <v>LERLimitCarveOut:    "",</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.InterestCalculationDate = sqlACCTTXInterestCalculationDate.String</v>
+        <v>sienaCounterpartyExtensions.LERLimitCarveOut = sqlCPEXLERLimitCarveOut.String</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="3"/>
-        <v>item.InterestCalculationDate = r.FormValue("InterestCalculationDate")</v>
+        <v>item.LERLimitCarveOut = r.FormValue("LERLimitCarveOut")</v>
       </c>
       <c r="AD17" t="str">
         <f t="shared" si="4"/>
-        <v>.InterestCalculationDate</v>
+        <v>.LERLimitCarveOut</v>
       </c>
       <c r="AG17" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.InterestCalculationDate = sqlInterestCalculationDate.String</v>
+        <v>sienaCounterpartyExtensions.LERLimitCarveOut = sqlLERLimitCarveOut.String</v>
       </c>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>AmendmentAmount    string</v>
+        <v>LastAmended    string</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="5"/>
-        <v>AmendmentAmount    string</v>
+        <v>LastAmended    string</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
-        <v>AmendmentAmount:    returnRecord.AmendmentAmount,</v>
+        <v>LastAmended:    returnRecord.LastAmended,</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="2"/>
-        <v>AmendmentAmount:    "",</v>
+        <v>LastAmended:    "",</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions.AmendmentAmount = sqlACCTTXAmendmentAmount.String</v>
+        <v>sienaCounterpartyExtensions.LastAmended = sqlCPEXLastAmended.String</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="3"/>
-        <v>item.AmendmentAmount = r.FormValue("AmendmentAmount")</v>
+        <v>item.LastAmended = r.FormValue("LastAmended")</v>
       </c>
       <c r="AD18" t="str">
         <f t="shared" si="4"/>
-        <v>.AmendmentAmount</v>
+        <v>.LastAmended</v>
       </c>
       <c r="AG18" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions.AmendmentAmount = sqlAmendmentAmount.String</v>
+        <v>sienaCounterpartyExtensions.LastAmended = sqlLastAmended.String</v>
       </c>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>LastLogin    string</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>LastLogin    string</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>LastLogin:    returnRecord.LastLogin,</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>LastLogin:    "",</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.LastLogin = sqlCPEXLastLogin.String</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.LastLogin = r.FormValue("LastLogin")</v>
       </c>
       <c r="AD19" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.LastLogin</v>
       </c>
       <c r="AG19" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.LastLogin = sqlLastLogin.String</v>
       </c>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>LossGivenDefault    string</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>LossGivenDefault    string</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>LossGivenDefault:    returnRecord.LossGivenDefault,</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>LossGivenDefault:    "",</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.LossGivenDefault = sqlCPEXLossGivenDefault.String</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.LossGivenDefault = r.FormValue("LossGivenDefault")</v>
       </c>
       <c r="AD20" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.LossGivenDefault</v>
       </c>
       <c r="AG20" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.LossGivenDefault = sqlLossGivenDefault.String</v>
       </c>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>MIC    string</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>MIC    string</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>MIC:    returnRecord.MIC,</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>MIC:    "",</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.MIC = sqlCPEXMIC.String</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.MIC = r.FormValue("MIC")</v>
       </c>
       <c r="AD21" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.MIC</v>
       </c>
       <c r="AG21" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.MIC = sqlMIC.String</v>
       </c>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>ProtectedDepositor    string</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>ProtectedDepositor    string</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>ProtectedDepositor:    returnRecord.ProtectedDepositor,</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>ProtectedDepositor:    "",</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.ProtectedDepositor = sqlCPEXProtectedDepositor.String</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.ProtectedDepositor = r.FormValue("ProtectedDepositor")</v>
       </c>
       <c r="AD22" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.ProtectedDepositor</v>
       </c>
       <c r="AG22" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.ProtectedDepositor = sqlProtectedDepositor.String</v>
       </c>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>RPTCurrency    string</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>RPTCurrency    string</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>RPTCurrency:    returnRecord.RPTCurrency,</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>RPTCurrency:    "",</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.RPTCurrency = sqlCPEXRPTCurrency.String</v>
       </c>
       <c r="V23" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.RPTCurrency = r.FormValue("RPTCurrency")</v>
       </c>
       <c r="AD23" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.RPTCurrency</v>
       </c>
       <c r="AG23" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.RPTCurrency = sqlRPTCurrency.String</v>
       </c>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>RateTimeout    string</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>RateTimeout    string</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>RateTimeout:    returnRecord.RateTimeout,</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>RateTimeout:    "",</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.RateTimeout = sqlCPEXRateTimeout.String</v>
       </c>
       <c r="V24" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.RateTimeout = r.FormValue("RateTimeout")</v>
       </c>
       <c r="AD24" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.RateTimeout</v>
       </c>
       <c r="AG24" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.RateTimeout = sqlRateTimeout.String</v>
       </c>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>RateValidation    string</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>RateValidation    string</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>RateValidation:    returnRecord.RateValidation,</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>RateValidation:    "",</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.RateValidation = sqlCPEXRateValidation.String</v>
       </c>
       <c r="V25" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.RateValidation = r.FormValue("RateValidation")</v>
       </c>
       <c r="AD25" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.RateValidation</v>
       </c>
       <c r="AG25" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.RateValidation = sqlRateValidation.String</v>
       </c>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>Registered    string</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>Registered    string</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>Registered:    returnRecord.Registered,</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>Registered:    "",</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.Registered = sqlCPEXRegistered.String</v>
       </c>
       <c r="V26" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.Registered = r.FormValue("Registered")</v>
       </c>
       <c r="AD26" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.Registered</v>
       </c>
       <c r="AG26" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.Registered = sqlRegistered.String</v>
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>RegulatoryCategory    string</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>RegulatoryCategory    string</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>RegulatoryCategory:    returnRecord.RegulatoryCategory,</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>RegulatoryCategory:    "",</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.RegulatoryCategory = sqlCPEXRegulatoryCategory.String</v>
       </c>
       <c r="V27" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.RegulatoryCategory = r.FormValue("RegulatoryCategory")</v>
       </c>
       <c r="AD27" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.RegulatoryCategory</v>
       </c>
       <c r="AG27" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.RegulatoryCategory = sqlRegulatoryCategory.String</v>
       </c>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>SecuredSettlement    string</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>SecuredSettlement    string</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>SecuredSettlement:    returnRecord.SecuredSettlement,</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>SecuredSettlement:    "",</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.SecuredSettlement = sqlCPEXSecuredSettlement.String</v>
       </c>
       <c r="V28" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.SecuredSettlement = r.FormValue("SecuredSettlement")</v>
       </c>
       <c r="AD28" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.SecuredSettlement</v>
       </c>
       <c r="AG28" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.SecuredSettlement = sqlSecuredSettlement.String</v>
       </c>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>SettlementLimitCarveOut    string</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>SettlementLimitCarveOut    string</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>SettlementLimitCarveOut:    returnRecord.SettlementLimitCarveOut,</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>SettlementLimitCarveOut:    "",</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.SettlementLimitCarveOut = sqlCPEXSettlementLimitCarveOut.String</v>
       </c>
       <c r="V29" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.SettlementLimitCarveOut = r.FormValue("SettlementLimitCarveOut")</v>
       </c>
       <c r="AD29" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.SettlementLimitCarveOut</v>
       </c>
       <c r="AG29" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.SettlementLimitCarveOut = sqlSettlementLimitCarveOut.String</v>
       </c>
     </row>
     <row r="30" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>SortCode    string</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>SortCode    string</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>SortCode:    returnRecord.SortCode,</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>SortCode:    "",</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.SortCode = sqlCPEXSortCode.String</v>
       </c>
       <c r="V30" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.SortCode = r.FormValue("SortCode")</v>
       </c>
       <c r="AD30" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.SortCode</v>
       </c>
       <c r="AG30" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.SortCode = sqlSortCode.String</v>
       </c>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>Training    string</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>Training    string</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>Training:    returnRecord.Training,</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>Training:    "",</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.Training = sqlCPEXTraining.String</v>
       </c>
       <c r="V31" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.Training = r.FormValue("Training")</v>
       </c>
       <c r="AD31" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.Training</v>
       </c>
       <c r="AG31" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.Training = sqlTraining.String</v>
       </c>
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>TrainingCode    string</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>TrainingCode    string</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>TrainingCode:    returnRecord.TrainingCode,</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>TrainingCode:    "",</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.TrainingCode = sqlCPEXTrainingCode.String</v>
       </c>
       <c r="V32" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.TrainingCode = r.FormValue("TrainingCode")</v>
       </c>
       <c r="AD32" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.TrainingCode</v>
       </c>
       <c r="AG32" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.TrainingCode = sqlTrainingCode.String</v>
       </c>
     </row>
     <row r="33" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>TrainingReceived    string</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>TrainingReceived    string</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>TrainingReceived:    returnRecord.TrainingReceived,</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>TrainingReceived:    "",</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.TrainingReceived = sqlCPEXTrainingReceived.String</v>
       </c>
       <c r="V33" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.TrainingReceived = r.FormValue("TrainingReceived")</v>
       </c>
       <c r="AD33" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.TrainingReceived</v>
       </c>
       <c r="AG33" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.TrainingReceived = sqlTrainingReceived.String</v>
       </c>
     </row>
     <row r="34" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>Unencumbered    string</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>Unencumbered    string</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>Unencumbered:    returnRecord.Unencumbered,</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>Unencumbered:    "",</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.Unencumbered = sqlCPEXUnencumbered.String</v>
       </c>
       <c r="V34" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.Unencumbered = r.FormValue("Unencumbered")</v>
       </c>
       <c r="AD34" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.Unencumbered</v>
       </c>
       <c r="AG34" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.Unencumbered = sqlUnencumbered.String</v>
       </c>
     </row>
     <row r="35" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>LEIExpiryDate    string</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>LEIExpiryDate    string</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>LEIExpiryDate:    returnRecord.LEIExpiryDate,</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>LEIExpiryDate:    "",</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.LEIExpiryDate = sqlCPEXLEIExpiryDate.String</v>
       </c>
       <c r="V35" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.LEIExpiryDate = r.FormValue("LEIExpiryDate")</v>
       </c>
       <c r="AD35" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.LEIExpiryDate</v>
       </c>
       <c r="AG35" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.LEIExpiryDate = sqlLEIExpiryDate.String</v>
       </c>
     </row>
     <row r="36" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>MIFIDReviewDate    string</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>MIFIDReviewDate    string</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>MIFIDReviewDate:    returnRecord.MIFIDReviewDate,</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>MIFIDReviewDate:    "",</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.MIFIDReviewDate = sqlCPEXMIFIDReviewDate.String</v>
       </c>
       <c r="V36" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.MIFIDReviewDate = r.FormValue("MIFIDReviewDate")</v>
       </c>
       <c r="AD36" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.MIFIDReviewDate</v>
       </c>
       <c r="AG36" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.MIFIDReviewDate = sqlMIFIDReviewDate.String</v>
       </c>
     </row>
     <row r="37" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>GDPRReviewDate    string</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>GDPRReviewDate    string</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>GDPRReviewDate:    returnRecord.GDPRReviewDate,</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>GDPRReviewDate:    "",</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.GDPRReviewDate = sqlCPEXGDPRReviewDate.String</v>
       </c>
       <c r="V37" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.GDPRReviewDate = r.FormValue("GDPRReviewDate")</v>
       </c>
       <c r="AD37" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.GDPRReviewDate</v>
       </c>
       <c r="AG37" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.GDPRReviewDate = sqlGDPRReviewDate.String</v>
       </c>
     </row>
     <row r="38" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>DelegatedReporting    string</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>DelegatedReporting    string</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>DelegatedReporting:    returnRecord.DelegatedReporting,</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>DelegatedReporting:    "",</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.DelegatedReporting = sqlCPEXDelegatedReporting.String</v>
       </c>
       <c r="V38" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.DelegatedReporting = r.FormValue("DelegatedReporting")</v>
       </c>
       <c r="AD38" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.DelegatedReporting</v>
       </c>
       <c r="AG38" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.DelegatedReporting = sqlDelegatedReporting.String</v>
       </c>
     </row>
     <row r="39" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    string</v>
+        <v>BOReconcile    string</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    string</v>
+        <v>BOReconcile    string</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
-        <v>:    returnRecord.,</v>
+        <v>BOReconcile:    returnRecord.BOReconcile,</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="2"/>
-        <v>:    "",</v>
+        <v>BOReconcile:    "",</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.BOReconcile = sqlCPEXBOReconcile.String</v>
       </c>
       <c r="V39" t="str">
         <f t="shared" si="3"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.BOReconcile = r.FormValue("BOReconcile")</v>
       </c>
       <c r="AD39" t="str">
         <f t="shared" si="4"/>
-        <v>.</v>
+        <v>.BOReconcile</v>
       </c>
       <c r="AG39" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.BOReconcile = sqlBOReconcile.String</v>
       </c>
     </row>
     <row r="40" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D40" t="str">
         <f t="shared" ref="D40:D62" si="8">B40&amp;"    string"</f>
-        <v xml:space="preserve">    string</v>
+        <v>MIFIDReportableDealsAllowed    string</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" ref="E40:E62" si="9">D40</f>
-        <v xml:space="preserve">    string</v>
+        <v>MIFIDReportableDealsAllowed    string</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" ref="G40:G62" si="10">B40&amp;":    "&amp;$F$4&amp;B40&amp;","</f>
-        <v>:    returnRecord.,</v>
+        <v>MIFIDReportableDealsAllowed:    returnRecord.MIFIDReportableDealsAllowed,</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" ref="H40:H62" si="11">B40&amp;":    """""&amp;","</f>
-        <v>:    "",</v>
+        <v>MIFIDReportableDealsAllowed:    "",</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.MIFIDReportableDealsAllowed = sqlCPEXMIFIDReportableDealsAllowed.String</v>
       </c>
       <c r="V40" t="str">
         <f t="shared" ref="V40:V62" si="12">"item."&amp;B40&amp;" = r.FormValue("""&amp;B40&amp;""")"</f>
-        <v>item. = r.FormValue("")</v>
+        <v>item.MIFIDReportableDealsAllowed = r.FormValue("MIFIDReportableDealsAllowed")</v>
       </c>
       <c r="AD40" t="str">
         <f t="shared" ref="AD40:AD62" si="13">"."&amp;B40</f>
-        <v>.</v>
+        <v>.MIFIDReportableDealsAllowed</v>
       </c>
       <c r="AG40" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.MIFIDReportableDealsAllowed = sqlMIFIDReportableDealsAllowed.String</v>
       </c>
     </row>
     <row r="41" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D41" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">    string</v>
+        <v>SignedInvestmentAgreement    string</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">    string</v>
+        <v>SignedInvestmentAgreement    string</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="10"/>
-        <v>:    returnRecord.,</v>
+        <v>SignedInvestmentAgreement:    returnRecord.SignedInvestmentAgreement,</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="11"/>
-        <v>:    "",</v>
+        <v>SignedInvestmentAgreement:    "",</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.SignedInvestmentAgreement = sqlCPEXSignedInvestmentAgreement.String</v>
       </c>
       <c r="V41" t="str">
         <f t="shared" si="12"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.SignedInvestmentAgreement = r.FormValue("SignedInvestmentAgreement")</v>
       </c>
       <c r="AD41" t="str">
         <f t="shared" si="13"/>
-        <v>.</v>
+        <v>.SignedInvestmentAgreement</v>
       </c>
       <c r="AG41" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.SignedInvestmentAgreement = sqlSignedInvestmentAgreement.String</v>
       </c>
     </row>
     <row r="42" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D42" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">    string</v>
+        <v>AppropriatenessAssessment    string</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">    string</v>
+        <v>AppropriatenessAssessment    string</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="10"/>
-        <v>:    returnRecord.,</v>
+        <v>AppropriatenessAssessment:    returnRecord.AppropriatenessAssessment,</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="11"/>
-        <v>:    "",</v>
+        <v>AppropriatenessAssessment:    "",</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.AppropriatenessAssessment = sqlCPEXAppropriatenessAssessment.String</v>
       </c>
       <c r="V42" t="str">
         <f t="shared" si="12"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.AppropriatenessAssessment = r.FormValue("AppropriatenessAssessment")</v>
       </c>
       <c r="AD42" t="str">
         <f t="shared" si="13"/>
-        <v>.</v>
+        <v>.AppropriatenessAssessment</v>
       </c>
       <c r="AG42" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.AppropriatenessAssessment = sqlAppropriatenessAssessment.String</v>
       </c>
     </row>
     <row r="43" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D43" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">    string</v>
+        <v>FinancialCounterparty    string</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">    string</v>
+        <v>FinancialCounterparty    string</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="10"/>
-        <v>:    returnRecord.,</v>
+        <v>FinancialCounterparty:    returnRecord.FinancialCounterparty,</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="11"/>
-        <v>:    "",</v>
+        <v>FinancialCounterparty:    "",</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.FinancialCounterparty = sqlCPEXFinancialCounterparty.String</v>
       </c>
       <c r="V43" t="str">
         <f t="shared" si="12"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.FinancialCounterparty = r.FormValue("FinancialCounterparty")</v>
       </c>
       <c r="AD43" t="str">
         <f t="shared" si="13"/>
-        <v>.</v>
+        <v>.FinancialCounterparty</v>
       </c>
       <c r="AG43" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.FinancialCounterparty = sqlFinancialCounterparty.String</v>
       </c>
     </row>
     <row r="44" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D44" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">    string</v>
+        <v>Collateralisation    string</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">    string</v>
+        <v>Collateralisation    string</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="10"/>
-        <v>:    returnRecord.,</v>
+        <v>Collateralisation:    returnRecord.Collateralisation,</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="11"/>
-        <v>:    "",</v>
+        <v>Collateralisation:    "",</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.Collateralisation = sqlCPEXCollateralisation.String</v>
       </c>
       <c r="V44" t="str">
         <f t="shared" si="12"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.Collateralisation = r.FormValue("Collateralisation")</v>
       </c>
       <c r="AD44" t="str">
         <f t="shared" si="13"/>
-        <v>.</v>
+        <v>.Collateralisation</v>
       </c>
       <c r="AG44" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.Collateralisation = sqlCollateralisation.String</v>
       </c>
     </row>
     <row r="45" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D45" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">    string</v>
+        <v>PortfolioCode    string</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">    string</v>
+        <v>PortfolioCode    string</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="10"/>
-        <v>:    returnRecord.,</v>
+        <v>PortfolioCode:    returnRecord.PortfolioCode,</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="11"/>
-        <v>:    "",</v>
+        <v>PortfolioCode:    "",</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.PortfolioCode = sqlCPEXPortfolioCode.String</v>
       </c>
       <c r="V45" t="str">
         <f t="shared" si="12"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.PortfolioCode = r.FormValue("PortfolioCode")</v>
       </c>
       <c r="AD45" t="str">
         <f t="shared" si="13"/>
-        <v>.</v>
+        <v>.PortfolioCode</v>
       </c>
       <c r="AG45" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.PortfolioCode = sqlPortfolioCode.String</v>
       </c>
     </row>
     <row r="46" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="D46" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">    string</v>
+        <v>ReconciliationLetterFrequency    string</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">    string</v>
+        <v>ReconciliationLetterFrequency    string</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="10"/>
-        <v>:    returnRecord.,</v>
+        <v>ReconciliationLetterFrequency:    returnRecord.ReconciliationLetterFrequency,</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="11"/>
-        <v>:    "",</v>
+        <v>ReconciliationLetterFrequency:    "",</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.ReconciliationLetterFrequency = sqlCPEXReconciliationLetterFrequency.String</v>
       </c>
       <c r="V46" t="str">
         <f t="shared" si="12"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.ReconciliationLetterFrequency = r.FormValue("ReconciliationLetterFrequency")</v>
       </c>
       <c r="AD46" t="str">
         <f t="shared" si="13"/>
-        <v>.</v>
+        <v>.ReconciliationLetterFrequency</v>
       </c>
       <c r="AG46" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.ReconciliationLetterFrequency = sqlReconciliationLetterFrequency.String</v>
       </c>
     </row>
     <row r="47" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D47" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">    string</v>
+        <v>DirectDealing    string</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">    string</v>
+        <v>DirectDealing    string</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="10"/>
-        <v>:    returnRecord.,</v>
+        <v>DirectDealing:    returnRecord.DirectDealing,</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="11"/>
-        <v>:    "",</v>
+        <v>DirectDealing:    "",</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions.DirectDealing = sqlCPEXDirectDealing.String</v>
       </c>
       <c r="V47" t="str">
         <f t="shared" si="12"/>
-        <v>item. = r.FormValue("")</v>
+        <v>item.DirectDealing = r.FormValue("DirectDealing")</v>
       </c>
       <c r="AD47" t="str">
         <f t="shared" si="13"/>
-        <v>.</v>
+        <v>.DirectDealing</v>
       </c>
       <c r="AG47" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions.DirectDealing = sqlDirectDealing.String</v>
       </c>
     </row>
     <row r="48" spans="2:33" x14ac:dyDescent="0.2">
@@ -2103,7 +2268,7 @@
       </c>
       <c r="L48" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V48" t="str">
         <f t="shared" si="12"/>
@@ -2115,7 +2280,7 @@
       </c>
       <c r="AG48" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="49" spans="2:33" x14ac:dyDescent="0.2">
@@ -2138,7 +2303,7 @@
       </c>
       <c r="L49" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V49" t="str">
         <f t="shared" si="12"/>
@@ -2150,7 +2315,7 @@
       </c>
       <c r="AG49" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="50" spans="2:33" x14ac:dyDescent="0.2">
@@ -2173,7 +2338,7 @@
       </c>
       <c r="L50" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V50" t="str">
         <f t="shared" si="12"/>
@@ -2185,7 +2350,7 @@
       </c>
       <c r="AG50" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="51" spans="2:33" x14ac:dyDescent="0.2">
@@ -2208,7 +2373,7 @@
       </c>
       <c r="L51" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V51" t="str">
         <f t="shared" si="12"/>
@@ -2220,7 +2385,7 @@
       </c>
       <c r="AG51" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="52" spans="2:33" x14ac:dyDescent="0.2">
@@ -2243,7 +2408,7 @@
       </c>
       <c r="L52" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V52" t="str">
         <f t="shared" si="12"/>
@@ -2255,7 +2420,7 @@
       </c>
       <c r="AG52" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="53" spans="2:33" x14ac:dyDescent="0.2">
@@ -2278,7 +2443,7 @@
       </c>
       <c r="L53" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V53" t="str">
         <f t="shared" si="12"/>
@@ -2290,7 +2455,7 @@
       </c>
       <c r="AG53" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="54" spans="2:33" x14ac:dyDescent="0.2">
@@ -2313,7 +2478,7 @@
       </c>
       <c r="L54" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V54" t="str">
         <f t="shared" si="12"/>
@@ -2325,7 +2490,7 @@
       </c>
       <c r="AG54" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="55" spans="2:33" x14ac:dyDescent="0.2">
@@ -2348,7 +2513,7 @@
       </c>
       <c r="L55" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V55" t="str">
         <f t="shared" si="12"/>
@@ -2360,7 +2525,7 @@
       </c>
       <c r="AG55" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="56" spans="2:33" x14ac:dyDescent="0.2">
@@ -2383,7 +2548,7 @@
       </c>
       <c r="L56" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V56" t="str">
         <f t="shared" si="12"/>
@@ -2395,7 +2560,7 @@
       </c>
       <c r="AG56" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="57" spans="2:33" x14ac:dyDescent="0.2">
@@ -2418,7 +2583,7 @@
       </c>
       <c r="L57" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V57" t="str">
         <f t="shared" si="12"/>
@@ -2430,7 +2595,7 @@
       </c>
       <c r="AG57" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="58" spans="2:33" x14ac:dyDescent="0.2">
@@ -2453,7 +2618,7 @@
       </c>
       <c r="L58" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V58" t="str">
         <f t="shared" si="12"/>
@@ -2465,7 +2630,7 @@
       </c>
       <c r="AG58" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="59" spans="2:33" x14ac:dyDescent="0.2">
@@ -2488,7 +2653,7 @@
       </c>
       <c r="L59" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V59" t="str">
         <f t="shared" si="12"/>
@@ -2500,7 +2665,7 @@
       </c>
       <c r="AG59" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="60" spans="2:33" x14ac:dyDescent="0.2">
@@ -2523,7 +2688,7 @@
       </c>
       <c r="L60" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V60" t="str">
         <f t="shared" si="12"/>
@@ -2535,7 +2700,7 @@
       </c>
       <c r="AG60" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="61" spans="2:33" x14ac:dyDescent="0.2">
@@ -2558,7 +2723,7 @@
       </c>
       <c r="L61" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccountTransactions. = sqlACCTTX.String</v>
+        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
       </c>
       <c r="V61" t="str">
         <f t="shared" si="12"/>
@@ -2570,7 +2735,7 @@
       </c>
       <c r="AG61" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="62" spans="2:33" x14ac:dyDescent="0.2">
@@ -2593,7 +2758,7 @@
       </c>
       <c r="L62" t="str">
         <f t="shared" ref="L40:L62" si="14">$I$3&amp;"."&amp;B62&amp;" = "&amp;B62&amp;".String"</f>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V62" t="str">
         <f t="shared" si="12"/>
@@ -2605,7 +2770,7 @@
       </c>
       <c r="AG62" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="63" spans="2:33" x14ac:dyDescent="0.2">
@@ -2628,7 +2793,7 @@
       </c>
       <c r="L63" t="str">
         <f t="shared" ref="L63:L74" si="19">$I$3&amp;"."&amp;B63&amp;" = "&amp;B63&amp;".String"</f>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V63" t="str">
         <f t="shared" ref="V63:V74" si="20">"item."&amp;B63&amp;" = r.FormValue("""&amp;B63&amp;""")"</f>
@@ -2640,7 +2805,7 @@
       </c>
       <c r="AG63" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="64" spans="2:33" x14ac:dyDescent="0.2">
@@ -2663,7 +2828,7 @@
       </c>
       <c r="L64" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V64" t="str">
         <f t="shared" si="20"/>
@@ -2675,7 +2840,7 @@
       </c>
       <c r="AG64" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="65" spans="2:33" x14ac:dyDescent="0.2">
@@ -2698,7 +2863,7 @@
       </c>
       <c r="L65" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V65" t="str">
         <f t="shared" si="20"/>
@@ -2710,7 +2875,7 @@
       </c>
       <c r="AG65" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="66" spans="2:33" x14ac:dyDescent="0.2">
@@ -2733,7 +2898,7 @@
       </c>
       <c r="L66" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V66" t="str">
         <f t="shared" si="20"/>
@@ -2745,7 +2910,7 @@
       </c>
       <c r="AG66" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="67" spans="2:33" x14ac:dyDescent="0.2">
@@ -2768,7 +2933,7 @@
       </c>
       <c r="L67" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V67" t="str">
         <f t="shared" si="20"/>
@@ -2780,7 +2945,7 @@
       </c>
       <c r="AG67" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="68" spans="2:33" x14ac:dyDescent="0.2">
@@ -2803,7 +2968,7 @@
       </c>
       <c r="L68" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V68" t="str">
         <f t="shared" si="20"/>
@@ -2815,7 +2980,7 @@
       </c>
       <c r="AG68" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="69" spans="2:33" x14ac:dyDescent="0.2">
@@ -2838,7 +3003,7 @@
       </c>
       <c r="L69" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V69" t="str">
         <f t="shared" si="20"/>
@@ -2850,7 +3015,7 @@
       </c>
       <c r="AG69" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="70" spans="2:33" x14ac:dyDescent="0.2">
@@ -2873,7 +3038,7 @@
       </c>
       <c r="L70" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V70" t="str">
         <f t="shared" si="20"/>
@@ -2885,7 +3050,7 @@
       </c>
       <c r="AG70" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="71" spans="2:33" x14ac:dyDescent="0.2">
@@ -2908,7 +3073,7 @@
       </c>
       <c r="L71" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V71" t="str">
         <f t="shared" si="20"/>
@@ -2920,7 +3085,7 @@
       </c>
       <c r="AG71" t="str">
         <f t="shared" ref="AG71:AG74" si="22">$I$3&amp;"."&amp;B71&amp;" = sql"&amp;B71&amp;".String"</f>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="72" spans="2:33" x14ac:dyDescent="0.2">
@@ -2943,7 +3108,7 @@
       </c>
       <c r="L72" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V72" t="str">
         <f t="shared" si="20"/>
@@ -2955,7 +3120,7 @@
       </c>
       <c r="AG72" t="str">
         <f t="shared" si="22"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="73" spans="2:33" x14ac:dyDescent="0.2">
@@ -2978,7 +3143,7 @@
       </c>
       <c r="L73" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V73" t="str">
         <f t="shared" si="20"/>
@@ -2990,7 +3155,7 @@
       </c>
       <c r="AG73" t="str">
         <f t="shared" si="22"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
     <row r="74" spans="2:33" x14ac:dyDescent="0.2">
@@ -3013,7 +3178,7 @@
       </c>
       <c r="L74" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccountTransactions. = .String</v>
+        <v>sienaCounterpartyExtensions. = .String</v>
       </c>
       <c r="V74" t="str">
         <f t="shared" si="20"/>
@@ -3025,7 +3190,7 @@
       </c>
       <c r="AG74" t="str">
         <f t="shared" si="22"/>
-        <v>sienaAccountTransactions. = sql.String</v>
+        <v>sienaCounterpartyExtensions. = sql.String</v>
       </c>
     </row>
   </sheetData>
@@ -3035,24 +3200,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90230AA-F0B1-6C49-B8FC-2C26A6B44982}">
-  <dimension ref="A3:BK15"/>
+  <dimension ref="A2:BK15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:AR15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
     <col min="19" max="20" width="24.5" customWidth="1"/>
     <col min="44" max="44" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="G2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="3" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C3" t="str">
         <f>UPPER('GO Struct Bits'!B2)</f>
-        <v>ACCTTX</v>
+        <v>CPEX</v>
       </c>
     </row>
     <row r="6" spans="1:63" x14ac:dyDescent="0.2">
@@ -3061,130 +3231,130 @@
         <v>0</v>
       </c>
       <c r="C6" t="str">
-        <v>SienaReference</v>
+        <v>NameFirm</v>
       </c>
       <c r="D6" t="str">
-        <v>LegNo</v>
+        <v>NameCentre</v>
       </c>
       <c r="E6" t="str">
-        <v>MMLegNo</v>
+        <v>BICCode</v>
       </c>
       <c r="F6" t="str">
-        <v>Narrative</v>
+        <v>ContactIndicator</v>
       </c>
       <c r="G6" t="str">
-        <v>Amount</v>
+        <v>CoverTrade</v>
       </c>
       <c r="H6" t="str">
-        <v>StartInterestDate</v>
+        <v>CustomerCategory</v>
       </c>
       <c r="I6" t="str">
-        <v>EndInterestDate</v>
+        <v>FSCSInclusive</v>
       </c>
       <c r="J6" t="str">
-        <v>Amortisation</v>
+        <v>FeeFactor</v>
       </c>
       <c r="K6" t="str">
-        <v>InterestAmount</v>
+        <v>InactiveStatus</v>
       </c>
       <c r="L6" t="str">
-        <v>InterestAction</v>
+        <v>Indemnity</v>
       </c>
       <c r="M6" t="str">
-        <v>FixingDate</v>
+        <v>KnowYourCustomerStatus</v>
       </c>
       <c r="N6" t="str">
-        <v>InterestCalculationDate</v>
+        <v>LERLimitCarveOut</v>
       </c>
       <c r="O6" t="str">
-        <v>AmendmentAmount</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AH6">
-        <v>0</v>
-      </c>
-      <c r="AI6">
-        <v>0</v>
-      </c>
-      <c r="AJ6">
-        <v>0</v>
-      </c>
-      <c r="AK6">
-        <v>0</v>
-      </c>
-      <c r="AL6">
-        <v>0</v>
-      </c>
-      <c r="AM6">
-        <v>0</v>
-      </c>
-      <c r="AN6">
-        <v>0</v>
-      </c>
-      <c r="AO6">
-        <v>0</v>
-      </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-      <c r="AR6">
-        <v>0</v>
+        <v>LastAmended</v>
+      </c>
+      <c r="P6" t="str">
+        <v>LastLogin</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>LossGivenDefault</v>
+      </c>
+      <c r="R6" t="str">
+        <v>MIC</v>
+      </c>
+      <c r="S6" t="str">
+        <v>ProtectedDepositor</v>
+      </c>
+      <c r="T6" t="str">
+        <v>RPTCurrency</v>
+      </c>
+      <c r="U6" t="str">
+        <v>RateTimeout</v>
+      </c>
+      <c r="V6" t="str">
+        <v>RateValidation</v>
+      </c>
+      <c r="W6" t="str">
+        <v>Registered</v>
+      </c>
+      <c r="X6" t="str">
+        <v>RegulatoryCategory</v>
+      </c>
+      <c r="Y6" t="str">
+        <v>SecuredSettlement</v>
+      </c>
+      <c r="Z6" t="str">
+        <v>SettlementLimitCarveOut</v>
+      </c>
+      <c r="AA6" t="str">
+        <v>SortCode</v>
+      </c>
+      <c r="AB6" t="str">
+        <v>Training</v>
+      </c>
+      <c r="AC6" t="str">
+        <v>TrainingCode</v>
+      </c>
+      <c r="AD6" t="str">
+        <v>TrainingReceived</v>
+      </c>
+      <c r="AE6" t="str">
+        <v>Unencumbered</v>
+      </c>
+      <c r="AF6" t="str">
+        <v>LEIExpiryDate</v>
+      </c>
+      <c r="AG6" t="str">
+        <v>MIFIDReviewDate</v>
+      </c>
+      <c r="AH6" t="str">
+        <v>GDPRReviewDate</v>
+      </c>
+      <c r="AI6" t="str">
+        <v>DelegatedReporting</v>
+      </c>
+      <c r="AJ6" t="str">
+        <v>BOReconcile</v>
+      </c>
+      <c r="AK6" t="str">
+        <v>MIFIDReportableDealsAllowed</v>
+      </c>
+      <c r="AL6" t="str">
+        <v>SignedInvestmentAgreement</v>
+      </c>
+      <c r="AM6" t="str">
+        <v>AppropriatenessAssessment</v>
+      </c>
+      <c r="AN6" t="str">
+        <v>FinancialCounterparty</v>
+      </c>
+      <c r="AO6" t="str">
+        <v>Collateralisation</v>
+      </c>
+      <c r="AP6" t="str">
+        <v>PortfolioCode</v>
+      </c>
+      <c r="AQ6" t="str">
+        <v>ReconciliationLetterFrequency</v>
+      </c>
+      <c r="AR6" t="str">
+        <v>DirectDealing</v>
       </c>
       <c r="AS6">
         <v>0</v>
@@ -3198,179 +3368,179 @@
     </row>
     <row r="8" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="str">
         <f>"var siena"&amp;'GO Struct Bits'!B4&amp;"SQL"</f>
-        <v>var sienaAccountTransactionsSQL</v>
+        <v>var sienaCounterpartyExtensionsSQL</v>
       </c>
       <c r="C8" t="str">
         <f>C6&amp;", "</f>
-        <v xml:space="preserve">SienaReference, </v>
+        <v xml:space="preserve">NameFirm, </v>
       </c>
       <c r="D8" t="str">
         <f t="shared" ref="D8:BK8" si="0">D6&amp;", "</f>
-        <v xml:space="preserve">LegNo, </v>
+        <v xml:space="preserve">NameCentre, </v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">MMLegNo, </v>
+        <v xml:space="preserve">BICCode, </v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Narrative, </v>
+        <v xml:space="preserve">ContactIndicator, </v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Amount, </v>
+        <v xml:space="preserve">CoverTrade, </v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">StartInterestDate, </v>
+        <v xml:space="preserve">CustomerCategory, </v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EndInterestDate, </v>
+        <v xml:space="preserve">FSCSInclusive, </v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Amortisation, </v>
+        <v xml:space="preserve">FeeFactor, </v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">InterestAmount, </v>
+        <v xml:space="preserve">InactiveStatus, </v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">InterestAction, </v>
+        <v xml:space="preserve">Indemnity, </v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">FixingDate, </v>
+        <v xml:space="preserve">KnowYourCustomerStatus, </v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">InterestCalculationDate, </v>
+        <v xml:space="preserve">LERLimitCarveOut, </v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">AmendmentAmount, </v>
+        <v xml:space="preserve">LastAmended, </v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">LastLogin, </v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">LossGivenDefault, </v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">MIC, </v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">ProtectedDepositor, </v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">RPTCurrency, </v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">RateTimeout, </v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">RateValidation, </v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">Registered, </v>
       </c>
       <c r="X8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">RegulatoryCategory, </v>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">SecuredSettlement, </v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">SettlementLimitCarveOut, </v>
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">SortCode, </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">Training, </v>
       </c>
       <c r="AC8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">TrainingCode, </v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">TrainingReceived, </v>
       </c>
       <c r="AE8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">Unencumbered, </v>
       </c>
       <c r="AF8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">LEIExpiryDate, </v>
       </c>
       <c r="AG8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">MIFIDReviewDate, </v>
       </c>
       <c r="AH8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">GDPRReviewDate, </v>
       </c>
       <c r="AI8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">DelegatedReporting, </v>
       </c>
       <c r="AJ8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">BOReconcile, </v>
       </c>
       <c r="AK8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">MIFIDReportableDealsAllowed, </v>
       </c>
       <c r="AL8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">SignedInvestmentAgreement, </v>
       </c>
       <c r="AM8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">AppropriatenessAssessment, </v>
       </c>
       <c r="AN8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">FinancialCounterparty, </v>
       </c>
       <c r="AO8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">Collateralisation, </v>
       </c>
       <c r="AP8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">PortfolioCode, </v>
       </c>
       <c r="AQ8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">ReconciliationLetterFrequency, </v>
       </c>
       <c r="AR8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">0, </v>
+        <v xml:space="preserve">DirectDealing, </v>
       </c>
       <c r="AS8" t="str">
         <f t="shared" si="0"/>
@@ -3452,184 +3622,184 @@
     <row r="10" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C10" t="str">
         <f>"&amp;"&amp;C8</f>
-        <v xml:space="preserve">&amp;SienaReference, </v>
+        <v xml:space="preserve">&amp;NameFirm, </v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ref="D10:BK10" si="1">"&amp;"&amp;D8</f>
-        <v xml:space="preserve">&amp;LegNo, </v>
+        <v xml:space="preserve">&amp;NameCentre, </v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;MMLegNo, </v>
+        <v xml:space="preserve">&amp;BICCode, </v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Narrative, </v>
+        <v xml:space="preserve">&amp;ContactIndicator, </v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Amount, </v>
+        <v xml:space="preserve">&amp;CoverTrade, </v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;StartInterestDate, </v>
+        <v xml:space="preserve">&amp;CustomerCategory, </v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;EndInterestDate, </v>
+        <v xml:space="preserve">&amp;FSCSInclusive, </v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Amortisation, </v>
+        <v xml:space="preserve">&amp;FeeFactor, </v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;InterestAmount, </v>
+        <v xml:space="preserve">&amp;InactiveStatus, </v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;InterestAction, </v>
+        <v xml:space="preserve">&amp;Indemnity, </v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;FixingDate, </v>
+        <v xml:space="preserve">&amp;KnowYourCustomerStatus, </v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;InterestCalculationDate, </v>
+        <v xml:space="preserve">&amp;LERLimitCarveOut, </v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;AmendmentAmount, </v>
+        <v xml:space="preserve">&amp;LastAmended, </v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;LastLogin, </v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;LossGivenDefault, </v>
+      </c>
+      <c r="R10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;MIC, </v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;ProtectedDepositor, </v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;RPTCurrency, </v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;RateTimeout, </v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;RateValidation, </v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;Registered, </v>
+      </c>
+      <c r="X10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;RegulatoryCategory, </v>
+      </c>
+      <c r="Y10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;SecuredSettlement, </v>
+      </c>
+      <c r="Z10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;SettlementLimitCarveOut, </v>
+      </c>
+      <c r="AA10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;SortCode, </v>
+      </c>
+      <c r="AB10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;Training, </v>
+      </c>
+      <c r="AC10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;TrainingCode, </v>
+      </c>
+      <c r="AD10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;TrainingReceived, </v>
+      </c>
+      <c r="AE10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;Unencumbered, </v>
+      </c>
+      <c r="AF10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;LEIExpiryDate, </v>
+      </c>
+      <c r="AG10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;MIFIDReviewDate, </v>
+      </c>
+      <c r="AH10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;GDPRReviewDate, </v>
+      </c>
+      <c r="AI10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;DelegatedReporting, </v>
+      </c>
+      <c r="AJ10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;BOReconcile, </v>
+      </c>
+      <c r="AK10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;MIFIDReportableDealsAllowed, </v>
+      </c>
+      <c r="AL10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;SignedInvestmentAgreement, </v>
+      </c>
+      <c r="AM10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;AppropriatenessAssessment, </v>
+      </c>
+      <c r="AN10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;FinancialCounterparty, </v>
+      </c>
+      <c r="AO10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;Collateralisation, </v>
+      </c>
+      <c r="AP10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;PortfolioCode, </v>
+      </c>
+      <c r="AQ10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;ReconciliationLetterFrequency, </v>
+      </c>
+      <c r="AR10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">&amp;DirectDealing, </v>
+      </c>
+      <c r="AS10" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve">&amp;0, </v>
       </c>
-      <c r="Q10" t="str">
+      <c r="AT10" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">&amp;0, </v>
       </c>
-      <c r="R10" t="str">
+      <c r="AU10" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">&amp;0, </v>
       </c>
-      <c r="S10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="T10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="U10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="V10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="W10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="X10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="Y10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="Z10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AA10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AB10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AC10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AD10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AE10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AF10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AG10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AH10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AI10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AJ10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AK10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AL10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AM10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AN10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AO10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AP10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AQ10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AR10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AS10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AT10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
-      <c r="AU10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;0, </v>
-      </c>
       <c r="AV10" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">&amp;, </v>
@@ -3696,374 +3866,383 @@
       </c>
     </row>
     <row r="13" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
       <c r="C13" t="str">
         <f>"sql"&amp;$C$3&amp;""&amp;C8</f>
-        <v xml:space="preserve">sqlACCTTXSienaReference, </v>
+        <v xml:space="preserve">sqlCPEXNameFirm, </v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ref="D13:AY13" si="2">"sql"&amp;$C$3&amp;""&amp;D8</f>
-        <v xml:space="preserve">sqlACCTTXLegNo, </v>
+        <v xml:space="preserve">sqlCPEXNameCentre, </v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXMMLegNo, </v>
+        <v xml:space="preserve">sqlCPEXBICCode, </v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXNarrative, </v>
+        <v xml:space="preserve">sqlCPEXContactIndicator, </v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXAmount, </v>
+        <v xml:space="preserve">sqlCPEXCoverTrade, </v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXStartInterestDate, </v>
+        <v xml:space="preserve">sqlCPEXCustomerCategory, </v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXEndInterestDate, </v>
+        <v xml:space="preserve">sqlCPEXFSCSInclusive, </v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXAmortisation, </v>
+        <v xml:space="preserve">sqlCPEXFeeFactor, </v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXInterestAmount, </v>
+        <v xml:space="preserve">sqlCPEXInactiveStatus, </v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXInterestAction, </v>
+        <v xml:space="preserve">sqlCPEXIndemnity, </v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXFixingDate, </v>
+        <v xml:space="preserve">sqlCPEXKnowYourCustomerStatus, </v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXInterestCalculationDate, </v>
+        <v xml:space="preserve">sqlCPEXLERLimitCarveOut, </v>
       </c>
       <c r="O13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTXAmendmentAmount, </v>
+        <v xml:space="preserve">sqlCPEXLastAmended, </v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXLastLogin, </v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXLossGivenDefault, </v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXMIC, </v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXProtectedDepositor, </v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXRPTCurrency, </v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXRateTimeout, </v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXRateValidation, </v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXRegistered, </v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXRegulatoryCategory, </v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXSecuredSettlement, </v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXSettlementLimitCarveOut, </v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXSortCode, </v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXTraining, </v>
       </c>
       <c r="AC13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXTrainingCode, </v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXTrainingReceived, </v>
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXUnencumbered, </v>
       </c>
       <c r="AF13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXLEIExpiryDate, </v>
       </c>
       <c r="AG13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXMIFIDReviewDate, </v>
       </c>
       <c r="AH13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXGDPRReviewDate, </v>
       </c>
       <c r="AI13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXDelegatedReporting, </v>
       </c>
       <c r="AJ13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXBOReconcile, </v>
       </c>
       <c r="AK13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXMIFIDReportableDealsAllowed, </v>
       </c>
       <c r="AL13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXSignedInvestmentAgreement, </v>
       </c>
       <c r="AM13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXAppropriatenessAssessment, </v>
       </c>
       <c r="AN13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXFinancialCounterparty, </v>
       </c>
       <c r="AO13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXCollateralisation, </v>
       </c>
       <c r="AP13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXPortfolioCode, </v>
       </c>
       <c r="AQ13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXReconciliationLetterFrequency, </v>
       </c>
       <c r="AR13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEXDirectDealing, </v>
       </c>
       <c r="AS13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEX0, </v>
       </c>
       <c r="AT13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEX0, </v>
       </c>
       <c r="AU13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX0, </v>
+        <v xml:space="preserve">sqlCPEX0, </v>
       </c>
       <c r="AV13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX, </v>
+        <v xml:space="preserve">sqlCPEX, </v>
       </c>
       <c r="AW13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX, </v>
+        <v xml:space="preserve">sqlCPEX, </v>
       </c>
       <c r="AX13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX, </v>
+        <v xml:space="preserve">sqlCPEX, </v>
       </c>
       <c r="AY13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTTX, </v>
+        <v xml:space="preserve">sqlCPEX, </v>
       </c>
     </row>
     <row r="15" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
       <c r="C15" t="str">
         <f>"&amp;"&amp;C13</f>
-        <v xml:space="preserve">&amp;sqlACCTTXSienaReference, </v>
+        <v xml:space="preserve">&amp;sqlCPEXNameFirm, </v>
       </c>
       <c r="D15" t="str">
         <f t="shared" ref="D15:AR15" si="3">"&amp;"&amp;D13</f>
-        <v xml:space="preserve">&amp;sqlACCTTXLegNo, </v>
+        <v xml:space="preserve">&amp;sqlCPEXNameCentre, </v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXMMLegNo, </v>
+        <v xml:space="preserve">&amp;sqlCPEXBICCode, </v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXNarrative, </v>
+        <v xml:space="preserve">&amp;sqlCPEXContactIndicator, </v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXAmount, </v>
+        <v xml:space="preserve">&amp;sqlCPEXCoverTrade, </v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXStartInterestDate, </v>
+        <v xml:space="preserve">&amp;sqlCPEXCustomerCategory, </v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXEndInterestDate, </v>
+        <v xml:space="preserve">&amp;sqlCPEXFSCSInclusive, </v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXAmortisation, </v>
+        <v xml:space="preserve">&amp;sqlCPEXFeeFactor, </v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXInterestAmount, </v>
+        <v xml:space="preserve">&amp;sqlCPEXInactiveStatus, </v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXInterestAction, </v>
+        <v xml:space="preserve">&amp;sqlCPEXIndemnity, </v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXFixingDate, </v>
+        <v xml:space="preserve">&amp;sqlCPEXKnowYourCustomerStatus, </v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXInterestCalculationDate, </v>
+        <v xml:space="preserve">&amp;sqlCPEXLERLimitCarveOut, </v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTXAmendmentAmount, </v>
+        <v xml:space="preserve">&amp;sqlCPEXLastAmended, </v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXLastLogin, </v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXLossGivenDefault, </v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXMIC, </v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXProtectedDepositor, </v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXRPTCurrency, </v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXRateTimeout, </v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXRateValidation, </v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXRegistered, </v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXRegulatoryCategory, </v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXSecuredSettlement, </v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXSettlementLimitCarveOut, </v>
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXSortCode, </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXTraining, </v>
       </c>
       <c r="AC15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXTrainingCode, </v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXTrainingReceived, </v>
       </c>
       <c r="AE15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXUnencumbered, </v>
       </c>
       <c r="AF15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXLEIExpiryDate, </v>
       </c>
       <c r="AG15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXMIFIDReviewDate, </v>
       </c>
       <c r="AH15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXGDPRReviewDate, </v>
       </c>
       <c r="AI15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXDelegatedReporting, </v>
       </c>
       <c r="AJ15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXBOReconcile, </v>
       </c>
       <c r="AK15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXMIFIDReportableDealsAllowed, </v>
       </c>
       <c r="AL15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXSignedInvestmentAgreement, </v>
       </c>
       <c r="AM15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXAppropriatenessAssessment, </v>
       </c>
       <c r="AN15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXFinancialCounterparty, </v>
       </c>
       <c r="AO15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXCollateralisation, </v>
       </c>
       <c r="AP15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXPortfolioCode, </v>
       </c>
       <c r="AQ15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXReconciliationLetterFrequency, </v>
       </c>
       <c r="AR15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTTX0, </v>
+        <v xml:space="preserve">&amp;sqlCPEXDirectDealing, </v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{2A1EAD35-E338-E445-AD9F-610B039958ED}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Move action buttons to card-header
</commit_message>
<xml_diff>
--- a/design/sienaDataArraysBuilder.xlsx
+++ b/design/sienaDataArraysBuilder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matttownsend/go/mwt-go-dev/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41EFCA0-DD22-964A-A3D1-EE0916C610B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA68C24-E5A4-D44F-ABEB-645181ECE1F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="26320" windowHeight="18000" activeTab="1" xr2:uid="{8265F428-BA81-814D-9171-A3F66298AE69}"/>
+    <workbookView xWindow="-34660" yWindow="-3580" windowWidth="26320" windowHeight="18000" xr2:uid="{8265F428-BA81-814D-9171-A3F66298AE69}"/>
   </bookViews>
   <sheets>
     <sheet name="GO Struct Bits" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>returnRecord.</t>
   </si>
@@ -72,9 +72,6 @@
     <t xml:space="preserve">getSiena…List </t>
   </si>
   <si>
-    <t>SortCode</t>
-  </si>
-  <si>
     <t>&gt;&gt;&gt;</t>
   </si>
   <si>
@@ -84,133 +81,94 @@
     <t>ROWS&gt;&gt;&gt;&gt;</t>
   </si>
   <si>
-    <t>NameCentre</t>
+    <t>Account</t>
   </si>
   <si>
-    <t>NameFirm</t>
+    <t>ACCT</t>
   </si>
   <si>
-    <t>BICCode</t>
+    <t>SienaReference</t>
   </si>
   <si>
-    <t>ContactIndicator</t>
+    <t>CustomerSienaView</t>
   </si>
   <si>
-    <t>CoverTrade</t>
+    <t>SienaCommonRef</t>
   </si>
   <si>
-    <t>CustomerCategory</t>
+    <t>Status</t>
   </si>
   <si>
-    <t>FSCSInclusive</t>
+    <t>StartDate</t>
   </si>
   <si>
-    <t>FeeFactor</t>
+    <t>MaturityDate</t>
   </si>
   <si>
-    <t>InactiveStatus</t>
+    <t>ContractNumber</t>
   </si>
   <si>
-    <t>Indemnity</t>
+    <t>ExternalReference</t>
   </si>
   <si>
-    <t>KnowYourCustomerStatus</t>
+    <t>CCY</t>
   </si>
   <si>
-    <t>LERLimitCarveOut</t>
+    <t>Book</t>
   </si>
   <si>
-    <t>LastAmended</t>
+    <t>MandatedUser</t>
   </si>
   <si>
-    <t>LastLogin</t>
+    <t>BackOfficeNotes</t>
   </si>
   <si>
-    <t>LossGivenDefault</t>
+    <t>CashBalance</t>
   </si>
   <si>
-    <t>MIC</t>
+    <t>AccountNumber</t>
   </si>
   <si>
-    <t>ProtectedDepositor</t>
+    <t>AccountName</t>
   </si>
   <si>
-    <t>RPTCurrency</t>
+    <t>LedgerBalance</t>
   </si>
   <si>
-    <t>RateTimeout</t>
+    <t>Portfolio</t>
   </si>
   <si>
-    <t>RateValidation</t>
+    <t>AgreementId</t>
   </si>
   <si>
-    <t>Registered</t>
+    <t>BackOfficeRefNo</t>
   </si>
   <si>
-    <t>RegulatoryCategory</t>
+    <t>PaymentSystemSienaView</t>
   </si>
   <si>
-    <t>SecuredSettlement</t>
+    <t>ISIN</t>
   </si>
   <si>
-    <t>SettlementLimitCarveOut</t>
+    <t>UTI</t>
   </si>
   <si>
-    <t>Training</t>
+    <t>CCYName</t>
   </si>
   <si>
-    <t>TrainingCode</t>
+    <t>BookName</t>
   </si>
   <si>
-    <t>TrainingReceived</t>
+    <t>PortfolioName</t>
   </si>
   <si>
-    <t>Unencumbered</t>
+    <t>Centre</t>
   </si>
   <si>
-    <t>LEIExpiryDate</t>
+    <t>Firm</t>
   </si>
   <si>
-    <t>MIFIDReviewDate</t>
-  </si>
-  <si>
-    <t>GDPRReviewDate</t>
-  </si>
-  <si>
-    <t>DelegatedReporting</t>
-  </si>
-  <si>
-    <t>BOReconcile</t>
-  </si>
-  <si>
-    <t>MIFIDReportableDealsAllowed</t>
-  </si>
-  <si>
-    <t>SignedInvestmentAgreement</t>
-  </si>
-  <si>
-    <t>AppropriatenessAssessment</t>
-  </si>
-  <si>
-    <t>FinancialCounterparty</t>
-  </si>
-  <si>
-    <t>Collateralisation</t>
-  </si>
-  <si>
-    <t>PortfolioCode</t>
-  </si>
-  <si>
-    <t>ReconciliationLetterFrequency</t>
-  </si>
-  <si>
-    <t>DirectDealing</t>
-  </si>
-  <si>
-    <t>CounterpartyExtensions</t>
-  </si>
-  <si>
-    <t>CPEX</t>
+    <t>CCYDp</t>
   </si>
 </sst>
 </file>
@@ -629,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4CE648-3973-0F42-A3A6-4E494BE264E6}">
   <dimension ref="B2:AG74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:L47"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,37 +613,37 @@
   <sheetData>
     <row r="2" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="D2" t="str">
         <f>"siena"&amp;B4&amp;".go"</f>
-        <v>sienaCounterpartyExtensions.go</v>
+        <v>sienaAccount.go</v>
       </c>
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.2">
       <c r="I3" t="str">
         <f>"siena"&amp;B4</f>
-        <v>sienaCounterpartyExtensions</v>
+        <v>sienaAccount</v>
       </c>
     </row>
     <row r="4" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>"siena"&amp;B4&amp;"Page"</f>
-        <v>sienaCounterpartyExtensionsPage</v>
+        <v>sienaAccountPage</v>
       </c>
       <c r="E4" s="2" t="str">
         <f>"siena"&amp;B4&amp;"Item"</f>
-        <v>sienaCounterpartyExtensionsItem</v>
+        <v>sienaAccountItem</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="str">
         <f>"newSiena"&amp;B4&amp;"Handler"</f>
-        <v>newSienaCounterpartyExtensionsHandler</v>
+        <v>newSienaAccountHandler</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>2</v>
@@ -700,1552 +658,1524 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" ref="D6:D39" si="0">B6&amp;"    string"</f>
-        <v>NameFirm    string</v>
+        <v>SienaReference    string</v>
       </c>
       <c r="E6" t="str">
         <f>D6</f>
-        <v>NameFirm    string</v>
+        <v>SienaReference    string</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ref="G6:G39" si="1">B6&amp;":    "&amp;$F$4&amp;B6&amp;","</f>
-        <v>NameFirm:    returnRecord.NameFirm,</v>
+        <v>SienaReference:    returnRecord.SienaReference,</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" ref="H6:H39" si="2">B6&amp;":    """""&amp;","</f>
-        <v>NameFirm:    "",</v>
+        <v>SienaReference:    "",</v>
       </c>
       <c r="L6" t="str">
         <f>$I$3&amp;"."&amp;B6&amp;" = sql"&amp;$B$2&amp;B6&amp;".String"</f>
-        <v>sienaCounterpartyExtensions.NameFirm = sqlCPEXNameFirm.String</v>
+        <v>sienaAccount.SienaReference = sqlACCTSienaReference.String</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" ref="V6:V39" si="3">"item."&amp;B6&amp;" = r.FormValue("""&amp;B6&amp;""")"</f>
-        <v>item.NameFirm = r.FormValue("NameFirm")</v>
+        <v>item.SienaReference = r.FormValue("SienaReference")</v>
       </c>
       <c r="AD6" t="str">
         <f t="shared" ref="AD6:AD39" si="4">"."&amp;B6</f>
-        <v>.NameFirm</v>
+        <v>.SienaReference</v>
       </c>
       <c r="AG6" t="str">
         <f>$I$3&amp;"."&amp;B6&amp;" = sql"&amp;B6&amp;".String"</f>
-        <v>sienaCounterpartyExtensions.NameFirm = sqlNameFirm.String</v>
+        <v>sienaAccount.SienaReference = sqlSienaReference.String</v>
       </c>
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>NameCentre    string</v>
+        <v>CustomerSienaView    string</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" ref="E7:E39" si="5">D7</f>
-        <v>NameCentre    string</v>
+        <v>CustomerSienaView    string</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>NameCentre:    returnRecord.NameCentre,</v>
+        <v>CustomerSienaView:    returnRecord.CustomerSienaView,</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="2"/>
-        <v>NameCentre:    "",</v>
+        <v>CustomerSienaView:    "",</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ref="L7:L61" si="6">$I$3&amp;"."&amp;B7&amp;" = sql"&amp;$B$2&amp;B7&amp;".String"</f>
-        <v>sienaCounterpartyExtensions.NameCentre = sqlCPEXNameCentre.String</v>
+        <v>sienaAccount.CustomerSienaView = sqlACCTCustomerSienaView.String</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="3"/>
-        <v>item.NameCentre = r.FormValue("NameCentre")</v>
+        <v>item.CustomerSienaView = r.FormValue("CustomerSienaView")</v>
       </c>
       <c r="AD7" t="str">
         <f t="shared" si="4"/>
-        <v>.NameCentre</v>
+        <v>.CustomerSienaView</v>
       </c>
       <c r="AG7" t="str">
         <f t="shared" ref="AG7:AG70" si="7">$I$3&amp;"."&amp;B7&amp;" = sql"&amp;B7&amp;".String"</f>
-        <v>sienaCounterpartyExtensions.NameCentre = sqlNameCentre.String</v>
+        <v>sienaAccount.CustomerSienaView = sqlCustomerSienaView.String</v>
       </c>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>BICCode    string</v>
+        <v>SienaCommonRef    string</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="5"/>
-        <v>BICCode    string</v>
+        <v>SienaCommonRef    string</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>BICCode:    returnRecord.BICCode,</v>
+        <v>SienaCommonRef:    returnRecord.SienaCommonRef,</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="2"/>
-        <v>BICCode:    "",</v>
+        <v>SienaCommonRef:    "",</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.BICCode = sqlCPEXBICCode.String</v>
+        <v>sienaAccount.SienaCommonRef = sqlACCTSienaCommonRef.String</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="3"/>
-        <v>item.BICCode = r.FormValue("BICCode")</v>
+        <v>item.SienaCommonRef = r.FormValue("SienaCommonRef")</v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="4"/>
-        <v>.BICCode</v>
+        <v>.SienaCommonRef</v>
       </c>
       <c r="AG8" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.BICCode = sqlBICCode.String</v>
+        <v>sienaAccount.SienaCommonRef = sqlSienaCommonRef.String</v>
       </c>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>ContactIndicator    string</v>
+        <v>Status    string</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="5"/>
-        <v>ContactIndicator    string</v>
+        <v>Status    string</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>ContactIndicator:    returnRecord.ContactIndicator,</v>
+        <v>Status:    returnRecord.Status,</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="2"/>
-        <v>ContactIndicator:    "",</v>
+        <v>Status:    "",</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.ContactIndicator = sqlCPEXContactIndicator.String</v>
+        <v>sienaAccount.Status = sqlACCTStatus.String</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="3"/>
-        <v>item.ContactIndicator = r.FormValue("ContactIndicator")</v>
+        <v>item.Status = r.FormValue("Status")</v>
       </c>
       <c r="AD9" t="str">
         <f t="shared" si="4"/>
-        <v>.ContactIndicator</v>
+        <v>.Status</v>
       </c>
       <c r="AG9" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.ContactIndicator = sqlContactIndicator.String</v>
+        <v>sienaAccount.Status = sqlStatus.String</v>
       </c>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>CoverTrade    string</v>
+        <v>StartDate    string</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="5"/>
-        <v>CoverTrade    string</v>
+        <v>StartDate    string</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>CoverTrade:    returnRecord.CoverTrade,</v>
+        <v>StartDate:    returnRecord.StartDate,</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="2"/>
-        <v>CoverTrade:    "",</v>
+        <v>StartDate:    "",</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.CoverTrade = sqlCPEXCoverTrade.String</v>
+        <v>sienaAccount.StartDate = sqlACCTStartDate.String</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="3"/>
-        <v>item.CoverTrade = r.FormValue("CoverTrade")</v>
+        <v>item.StartDate = r.FormValue("StartDate")</v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="4"/>
-        <v>.CoverTrade</v>
+        <v>.StartDate</v>
       </c>
       <c r="AG10" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.CoverTrade = sqlCoverTrade.String</v>
+        <v>sienaAccount.StartDate = sqlStartDate.String</v>
       </c>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>CustomerCategory    string</v>
+        <v>MaturityDate    string</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="5"/>
-        <v>CustomerCategory    string</v>
+        <v>MaturityDate    string</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
-        <v>CustomerCategory:    returnRecord.CustomerCategory,</v>
+        <v>MaturityDate:    returnRecord.MaturityDate,</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="2"/>
-        <v>CustomerCategory:    "",</v>
+        <v>MaturityDate:    "",</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.CustomerCategory = sqlCPEXCustomerCategory.String</v>
+        <v>sienaAccount.MaturityDate = sqlACCTMaturityDate.String</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="3"/>
-        <v>item.CustomerCategory = r.FormValue("CustomerCategory")</v>
+        <v>item.MaturityDate = r.FormValue("MaturityDate")</v>
       </c>
       <c r="AD11" t="str">
         <f t="shared" si="4"/>
-        <v>.CustomerCategory</v>
+        <v>.MaturityDate</v>
       </c>
       <c r="AG11" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.CustomerCategory = sqlCustomerCategory.String</v>
+        <v>sienaAccount.MaturityDate = sqlMaturityDate.String</v>
       </c>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>FSCSInclusive    string</v>
+        <v>ContractNumber    string</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="5"/>
-        <v>FSCSInclusive    string</v>
+        <v>ContractNumber    string</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
-        <v>FSCSInclusive:    returnRecord.FSCSInclusive,</v>
+        <v>ContractNumber:    returnRecord.ContractNumber,</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="2"/>
-        <v>FSCSInclusive:    "",</v>
+        <v>ContractNumber:    "",</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.FSCSInclusive = sqlCPEXFSCSInclusive.String</v>
+        <v>sienaAccount.ContractNumber = sqlACCTContractNumber.String</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="3"/>
-        <v>item.FSCSInclusive = r.FormValue("FSCSInclusive")</v>
+        <v>item.ContractNumber = r.FormValue("ContractNumber")</v>
       </c>
       <c r="AD12" t="str">
         <f t="shared" si="4"/>
-        <v>.FSCSInclusive</v>
+        <v>.ContractNumber</v>
       </c>
       <c r="AG12" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.FSCSInclusive = sqlFSCSInclusive.String</v>
+        <v>sienaAccount.ContractNumber = sqlContractNumber.String</v>
       </c>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>FeeFactor    string</v>
+        <v>ExternalReference    string</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="5"/>
-        <v>FeeFactor    string</v>
+        <v>ExternalReference    string</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
-        <v>FeeFactor:    returnRecord.FeeFactor,</v>
+        <v>ExternalReference:    returnRecord.ExternalReference,</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
-        <v>FeeFactor:    "",</v>
+        <v>ExternalReference:    "",</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.FeeFactor = sqlCPEXFeeFactor.String</v>
+        <v>sienaAccount.ExternalReference = sqlACCTExternalReference.String</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="3"/>
-        <v>item.FeeFactor = r.FormValue("FeeFactor")</v>
+        <v>item.ExternalReference = r.FormValue("ExternalReference")</v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="4"/>
-        <v>.FeeFactor</v>
+        <v>.ExternalReference</v>
       </c>
       <c r="AG13" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.FeeFactor = sqlFeeFactor.String</v>
+        <v>sienaAccount.ExternalReference = sqlExternalReference.String</v>
       </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>InactiveStatus    string</v>
+        <v>CCY    string</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="5"/>
-        <v>InactiveStatus    string</v>
+        <v>CCY    string</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
-        <v>InactiveStatus:    returnRecord.InactiveStatus,</v>
+        <v>CCY:    returnRecord.CCY,</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="2"/>
-        <v>InactiveStatus:    "",</v>
+        <v>CCY:    "",</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.InactiveStatus = sqlCPEXInactiveStatus.String</v>
+        <v>sienaAccount.CCY = sqlACCTCCY.String</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="3"/>
-        <v>item.InactiveStatus = r.FormValue("InactiveStatus")</v>
+        <v>item.CCY = r.FormValue("CCY")</v>
       </c>
       <c r="AD14" t="str">
         <f t="shared" si="4"/>
-        <v>.InactiveStatus</v>
+        <v>.CCY</v>
       </c>
       <c r="AG14" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.InactiveStatus = sqlInactiveStatus.String</v>
+        <v>sienaAccount.CCY = sqlCCY.String</v>
       </c>
     </row>
     <row r="15" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>Indemnity    string</v>
+        <v>Book    string</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="5"/>
-        <v>Indemnity    string</v>
+        <v>Book    string</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>Indemnity:    returnRecord.Indemnity,</v>
+        <v>Book:    returnRecord.Book,</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="2"/>
-        <v>Indemnity:    "",</v>
+        <v>Book:    "",</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.Indemnity = sqlCPEXIndemnity.String</v>
+        <v>sienaAccount.Book = sqlACCTBook.String</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="3"/>
-        <v>item.Indemnity = r.FormValue("Indemnity")</v>
+        <v>item.Book = r.FormValue("Book")</v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="4"/>
-        <v>.Indemnity</v>
+        <v>.Book</v>
       </c>
       <c r="AG15" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.Indemnity = sqlIndemnity.String</v>
+        <v>sienaAccount.Book = sqlBook.String</v>
       </c>
     </row>
     <row r="16" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>KnowYourCustomerStatus    string</v>
+        <v>MandatedUser    string</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="5"/>
-        <v>KnowYourCustomerStatus    string</v>
+        <v>MandatedUser    string</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>KnowYourCustomerStatus:    returnRecord.KnowYourCustomerStatus,</v>
+        <v>MandatedUser:    returnRecord.MandatedUser,</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="2"/>
-        <v>KnowYourCustomerStatus:    "",</v>
+        <v>MandatedUser:    "",</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.KnowYourCustomerStatus = sqlCPEXKnowYourCustomerStatus.String</v>
+        <v>sienaAccount.MandatedUser = sqlACCTMandatedUser.String</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="3"/>
-        <v>item.KnowYourCustomerStatus = r.FormValue("KnowYourCustomerStatus")</v>
+        <v>item.MandatedUser = r.FormValue("MandatedUser")</v>
       </c>
       <c r="AD16" t="str">
         <f t="shared" si="4"/>
-        <v>.KnowYourCustomerStatus</v>
+        <v>.MandatedUser</v>
       </c>
       <c r="AG16" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.KnowYourCustomerStatus = sqlKnowYourCustomerStatus.String</v>
+        <v>sienaAccount.MandatedUser = sqlMandatedUser.String</v>
       </c>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>LERLimitCarveOut    string</v>
+        <v>BackOfficeNotes    string</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="5"/>
-        <v>LERLimitCarveOut    string</v>
+        <v>BackOfficeNotes    string</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>LERLimitCarveOut:    returnRecord.LERLimitCarveOut,</v>
+        <v>BackOfficeNotes:    returnRecord.BackOfficeNotes,</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="2"/>
-        <v>LERLimitCarveOut:    "",</v>
+        <v>BackOfficeNotes:    "",</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.LERLimitCarveOut = sqlCPEXLERLimitCarveOut.String</v>
+        <v>sienaAccount.BackOfficeNotes = sqlACCTBackOfficeNotes.String</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="3"/>
-        <v>item.LERLimitCarveOut = r.FormValue("LERLimitCarveOut")</v>
+        <v>item.BackOfficeNotes = r.FormValue("BackOfficeNotes")</v>
       </c>
       <c r="AD17" t="str">
         <f t="shared" si="4"/>
-        <v>.LERLimitCarveOut</v>
+        <v>.BackOfficeNotes</v>
       </c>
       <c r="AG17" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.LERLimitCarveOut = sqlLERLimitCarveOut.String</v>
+        <v>sienaAccount.BackOfficeNotes = sqlBackOfficeNotes.String</v>
       </c>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>LastAmended    string</v>
+        <v>CashBalance    string</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="5"/>
-        <v>LastAmended    string</v>
+        <v>CashBalance    string</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
-        <v>LastAmended:    returnRecord.LastAmended,</v>
+        <v>CashBalance:    returnRecord.CashBalance,</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="2"/>
-        <v>LastAmended:    "",</v>
+        <v>CashBalance:    "",</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.LastAmended = sqlCPEXLastAmended.String</v>
+        <v>sienaAccount.CashBalance = sqlACCTCashBalance.String</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="3"/>
-        <v>item.LastAmended = r.FormValue("LastAmended")</v>
+        <v>item.CashBalance = r.FormValue("CashBalance")</v>
       </c>
       <c r="AD18" t="str">
         <f t="shared" si="4"/>
-        <v>.LastAmended</v>
+        <v>.CashBalance</v>
       </c>
       <c r="AG18" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.LastAmended = sqlLastAmended.String</v>
+        <v>sienaAccount.CashBalance = sqlCashBalance.String</v>
       </c>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>LastLogin    string</v>
+        <v>AccountNumber    string</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="5"/>
-        <v>LastLogin    string</v>
+        <v>AccountNumber    string</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>LastLogin:    returnRecord.LastLogin,</v>
+        <v>AccountNumber:    returnRecord.AccountNumber,</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="2"/>
-        <v>LastLogin:    "",</v>
+        <v>AccountNumber:    "",</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.LastLogin = sqlCPEXLastLogin.String</v>
+        <v>sienaAccount.AccountNumber = sqlACCTAccountNumber.String</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="3"/>
-        <v>item.LastLogin = r.FormValue("LastLogin")</v>
+        <v>item.AccountNumber = r.FormValue("AccountNumber")</v>
       </c>
       <c r="AD19" t="str">
         <f t="shared" si="4"/>
-        <v>.LastLogin</v>
+        <v>.AccountNumber</v>
       </c>
       <c r="AG19" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.LastLogin = sqlLastLogin.String</v>
+        <v>sienaAccount.AccountNumber = sqlAccountNumber.String</v>
       </c>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>LossGivenDefault    string</v>
+        <v>AccountName    string</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="5"/>
-        <v>LossGivenDefault    string</v>
+        <v>AccountName    string</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
-        <v>LossGivenDefault:    returnRecord.LossGivenDefault,</v>
+        <v>AccountName:    returnRecord.AccountName,</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="2"/>
-        <v>LossGivenDefault:    "",</v>
+        <v>AccountName:    "",</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.LossGivenDefault = sqlCPEXLossGivenDefault.String</v>
+        <v>sienaAccount.AccountName = sqlACCTAccountName.String</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="3"/>
-        <v>item.LossGivenDefault = r.FormValue("LossGivenDefault")</v>
+        <v>item.AccountName = r.FormValue("AccountName")</v>
       </c>
       <c r="AD20" t="str">
         <f t="shared" si="4"/>
-        <v>.LossGivenDefault</v>
+        <v>.AccountName</v>
       </c>
       <c r="AG20" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.LossGivenDefault = sqlLossGivenDefault.String</v>
+        <v>sienaAccount.AccountName = sqlAccountName.String</v>
       </c>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>MIC    string</v>
+        <v>LedgerBalance    string</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="5"/>
-        <v>MIC    string</v>
+        <v>LedgerBalance    string</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
-        <v>MIC:    returnRecord.MIC,</v>
+        <v>LedgerBalance:    returnRecord.LedgerBalance,</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="2"/>
-        <v>MIC:    "",</v>
+        <v>LedgerBalance:    "",</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.MIC = sqlCPEXMIC.String</v>
+        <v>sienaAccount.LedgerBalance = sqlACCTLedgerBalance.String</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="3"/>
-        <v>item.MIC = r.FormValue("MIC")</v>
+        <v>item.LedgerBalance = r.FormValue("LedgerBalance")</v>
       </c>
       <c r="AD21" t="str">
         <f t="shared" si="4"/>
-        <v>.MIC</v>
+        <v>.LedgerBalance</v>
       </c>
       <c r="AG21" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.MIC = sqlMIC.String</v>
+        <v>sienaAccount.LedgerBalance = sqlLedgerBalance.String</v>
       </c>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>ProtectedDepositor    string</v>
+        <v>Portfolio    string</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="5"/>
-        <v>ProtectedDepositor    string</v>
+        <v>Portfolio    string</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
-        <v>ProtectedDepositor:    returnRecord.ProtectedDepositor,</v>
+        <v>Portfolio:    returnRecord.Portfolio,</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="2"/>
-        <v>ProtectedDepositor:    "",</v>
+        <v>Portfolio:    "",</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.ProtectedDepositor = sqlCPEXProtectedDepositor.String</v>
+        <v>sienaAccount.Portfolio = sqlACCTPortfolio.String</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="3"/>
-        <v>item.ProtectedDepositor = r.FormValue("ProtectedDepositor")</v>
+        <v>item.Portfolio = r.FormValue("Portfolio")</v>
       </c>
       <c r="AD22" t="str">
         <f t="shared" si="4"/>
-        <v>.ProtectedDepositor</v>
+        <v>.Portfolio</v>
       </c>
       <c r="AG22" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.ProtectedDepositor = sqlProtectedDepositor.String</v>
+        <v>sienaAccount.Portfolio = sqlPortfolio.String</v>
       </c>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>RPTCurrency    string</v>
+        <v>AgreementId    string</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="5"/>
-        <v>RPTCurrency    string</v>
+        <v>AgreementId    string</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
-        <v>RPTCurrency:    returnRecord.RPTCurrency,</v>
+        <v>AgreementId:    returnRecord.AgreementId,</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="2"/>
-        <v>RPTCurrency:    "",</v>
+        <v>AgreementId:    "",</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.RPTCurrency = sqlCPEXRPTCurrency.String</v>
+        <v>sienaAccount.AgreementId = sqlACCTAgreementId.String</v>
       </c>
       <c r="V23" t="str">
         <f t="shared" si="3"/>
-        <v>item.RPTCurrency = r.FormValue("RPTCurrency")</v>
+        <v>item.AgreementId = r.FormValue("AgreementId")</v>
       </c>
       <c r="AD23" t="str">
         <f t="shared" si="4"/>
-        <v>.RPTCurrency</v>
+        <v>.AgreementId</v>
       </c>
       <c r="AG23" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.RPTCurrency = sqlRPTCurrency.String</v>
+        <v>sienaAccount.AgreementId = sqlAgreementId.String</v>
       </c>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>RateTimeout    string</v>
+        <v>BackOfficeRefNo    string</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="5"/>
-        <v>RateTimeout    string</v>
+        <v>BackOfficeRefNo    string</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
-        <v>RateTimeout:    returnRecord.RateTimeout,</v>
+        <v>BackOfficeRefNo:    returnRecord.BackOfficeRefNo,</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="2"/>
-        <v>RateTimeout:    "",</v>
+        <v>BackOfficeRefNo:    "",</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.RateTimeout = sqlCPEXRateTimeout.String</v>
+        <v>sienaAccount.BackOfficeRefNo = sqlACCTBackOfficeRefNo.String</v>
       </c>
       <c r="V24" t="str">
         <f t="shared" si="3"/>
-        <v>item.RateTimeout = r.FormValue("RateTimeout")</v>
+        <v>item.BackOfficeRefNo = r.FormValue("BackOfficeRefNo")</v>
       </c>
       <c r="AD24" t="str">
         <f t="shared" si="4"/>
-        <v>.RateTimeout</v>
+        <v>.BackOfficeRefNo</v>
       </c>
       <c r="AG24" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.RateTimeout = sqlRateTimeout.String</v>
+        <v>sienaAccount.BackOfficeRefNo = sqlBackOfficeRefNo.String</v>
       </c>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>RateValidation    string</v>
+        <v>PaymentSystemSienaView    string</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="5"/>
-        <v>RateValidation    string</v>
+        <v>PaymentSystemSienaView    string</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
-        <v>RateValidation:    returnRecord.RateValidation,</v>
+        <v>PaymentSystemSienaView:    returnRecord.PaymentSystemSienaView,</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="2"/>
-        <v>RateValidation:    "",</v>
+        <v>PaymentSystemSienaView:    "",</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.RateValidation = sqlCPEXRateValidation.String</v>
+        <v>sienaAccount.PaymentSystemSienaView = sqlACCTPaymentSystemSienaView.String</v>
       </c>
       <c r="V25" t="str">
         <f t="shared" si="3"/>
-        <v>item.RateValidation = r.FormValue("RateValidation")</v>
+        <v>item.PaymentSystemSienaView = r.FormValue("PaymentSystemSienaView")</v>
       </c>
       <c r="AD25" t="str">
         <f t="shared" si="4"/>
-        <v>.RateValidation</v>
+        <v>.PaymentSystemSienaView</v>
       </c>
       <c r="AG25" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.RateValidation = sqlRateValidation.String</v>
+        <v>sienaAccount.PaymentSystemSienaView = sqlPaymentSystemSienaView.String</v>
       </c>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>Registered    string</v>
+        <v>ISIN    string</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="5"/>
-        <v>Registered    string</v>
+        <v>ISIN    string</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
-        <v>Registered:    returnRecord.Registered,</v>
+        <v>ISIN:    returnRecord.ISIN,</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="2"/>
-        <v>Registered:    "",</v>
+        <v>ISIN:    "",</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.Registered = sqlCPEXRegistered.String</v>
+        <v>sienaAccount.ISIN = sqlACCTISIN.String</v>
       </c>
       <c r="V26" t="str">
         <f t="shared" si="3"/>
-        <v>item.Registered = r.FormValue("Registered")</v>
+        <v>item.ISIN = r.FormValue("ISIN")</v>
       </c>
       <c r="AD26" t="str">
         <f t="shared" si="4"/>
-        <v>.Registered</v>
+        <v>.ISIN</v>
       </c>
       <c r="AG26" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.Registered = sqlRegistered.String</v>
+        <v>sienaAccount.ISIN = sqlISIN.String</v>
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>RegulatoryCategory    string</v>
+        <v>UTI    string</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="5"/>
-        <v>RegulatoryCategory    string</v>
+        <v>UTI    string</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
-        <v>RegulatoryCategory:    returnRecord.RegulatoryCategory,</v>
+        <v>UTI:    returnRecord.UTI,</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="2"/>
-        <v>RegulatoryCategory:    "",</v>
+        <v>UTI:    "",</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.RegulatoryCategory = sqlCPEXRegulatoryCategory.String</v>
+        <v>sienaAccount.UTI = sqlACCTUTI.String</v>
       </c>
       <c r="V27" t="str">
         <f t="shared" si="3"/>
-        <v>item.RegulatoryCategory = r.FormValue("RegulatoryCategory")</v>
+        <v>item.UTI = r.FormValue("UTI")</v>
       </c>
       <c r="AD27" t="str">
         <f t="shared" si="4"/>
-        <v>.RegulatoryCategory</v>
+        <v>.UTI</v>
       </c>
       <c r="AG27" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.RegulatoryCategory = sqlRegulatoryCategory.String</v>
+        <v>sienaAccount.UTI = sqlUTI.String</v>
       </c>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>SecuredSettlement    string</v>
+        <v>CCYName    string</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="5"/>
-        <v>SecuredSettlement    string</v>
+        <v>CCYName    string</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
-        <v>SecuredSettlement:    returnRecord.SecuredSettlement,</v>
+        <v>CCYName:    returnRecord.CCYName,</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="2"/>
-        <v>SecuredSettlement:    "",</v>
+        <v>CCYName:    "",</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.SecuredSettlement = sqlCPEXSecuredSettlement.String</v>
+        <v>sienaAccount.CCYName = sqlACCTCCYName.String</v>
       </c>
       <c r="V28" t="str">
         <f t="shared" si="3"/>
-        <v>item.SecuredSettlement = r.FormValue("SecuredSettlement")</v>
+        <v>item.CCYName = r.FormValue("CCYName")</v>
       </c>
       <c r="AD28" t="str">
         <f t="shared" si="4"/>
-        <v>.SecuredSettlement</v>
+        <v>.CCYName</v>
       </c>
       <c r="AG28" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.SecuredSettlement = sqlSecuredSettlement.String</v>
+        <v>sienaAccount.CCYName = sqlCCYName.String</v>
       </c>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>SettlementLimitCarveOut    string</v>
+        <v>BookName    string</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="5"/>
-        <v>SettlementLimitCarveOut    string</v>
+        <v>BookName    string</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
-        <v>SettlementLimitCarveOut:    returnRecord.SettlementLimitCarveOut,</v>
+        <v>BookName:    returnRecord.BookName,</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="2"/>
-        <v>SettlementLimitCarveOut:    "",</v>
+        <v>BookName:    "",</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.SettlementLimitCarveOut = sqlCPEXSettlementLimitCarveOut.String</v>
+        <v>sienaAccount.BookName = sqlACCTBookName.String</v>
       </c>
       <c r="V29" t="str">
         <f t="shared" si="3"/>
-        <v>item.SettlementLimitCarveOut = r.FormValue("SettlementLimitCarveOut")</v>
+        <v>item.BookName = r.FormValue("BookName")</v>
       </c>
       <c r="AD29" t="str">
         <f t="shared" si="4"/>
-        <v>.SettlementLimitCarveOut</v>
+        <v>.BookName</v>
       </c>
       <c r="AG29" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.SettlementLimitCarveOut = sqlSettlementLimitCarveOut.String</v>
+        <v>sienaAccount.BookName = sqlBookName.String</v>
       </c>
     </row>
     <row r="30" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>SortCode    string</v>
+        <v>PortfolioName    string</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="5"/>
-        <v>SortCode    string</v>
+        <v>PortfolioName    string</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
-        <v>SortCode:    returnRecord.SortCode,</v>
+        <v>PortfolioName:    returnRecord.PortfolioName,</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="2"/>
-        <v>SortCode:    "",</v>
+        <v>PortfolioName:    "",</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.SortCode = sqlCPEXSortCode.String</v>
+        <v>sienaAccount.PortfolioName = sqlACCTPortfolioName.String</v>
       </c>
       <c r="V30" t="str">
         <f t="shared" si="3"/>
-        <v>item.SortCode = r.FormValue("SortCode")</v>
+        <v>item.PortfolioName = r.FormValue("PortfolioName")</v>
       </c>
       <c r="AD30" t="str">
         <f t="shared" si="4"/>
-        <v>.SortCode</v>
+        <v>.PortfolioName</v>
       </c>
       <c r="AG30" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.SortCode = sqlSortCode.String</v>
+        <v>sienaAccount.PortfolioName = sqlPortfolioName.String</v>
       </c>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>Training    string</v>
+        <v>Centre    string</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="5"/>
-        <v>Training    string</v>
+        <v>Centre    string</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
-        <v>Training:    returnRecord.Training,</v>
+        <v>Centre:    returnRecord.Centre,</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="2"/>
-        <v>Training:    "",</v>
+        <v>Centre:    "",</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.Training = sqlCPEXTraining.String</v>
+        <v>sienaAccount.Centre = sqlACCTCentre.String</v>
       </c>
       <c r="V31" t="str">
         <f t="shared" si="3"/>
-        <v>item.Training = r.FormValue("Training")</v>
+        <v>item.Centre = r.FormValue("Centre")</v>
       </c>
       <c r="AD31" t="str">
         <f t="shared" si="4"/>
-        <v>.Training</v>
+        <v>.Centre</v>
       </c>
       <c r="AG31" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.Training = sqlTraining.String</v>
+        <v>sienaAccount.Centre = sqlCentre.String</v>
       </c>
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>TrainingCode    string</v>
+        <v>Firm    string</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="5"/>
-        <v>TrainingCode    string</v>
+        <v>Firm    string</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
-        <v>TrainingCode:    returnRecord.TrainingCode,</v>
+        <v>Firm:    returnRecord.Firm,</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="2"/>
-        <v>TrainingCode:    "",</v>
+        <v>Firm:    "",</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.TrainingCode = sqlCPEXTrainingCode.String</v>
+        <v>sienaAccount.Firm = sqlACCTFirm.String</v>
       </c>
       <c r="V32" t="str">
         <f t="shared" si="3"/>
-        <v>item.TrainingCode = r.FormValue("TrainingCode")</v>
+        <v>item.Firm = r.FormValue("Firm")</v>
       </c>
       <c r="AD32" t="str">
         <f t="shared" si="4"/>
-        <v>.TrainingCode</v>
+        <v>.Firm</v>
       </c>
       <c r="AG32" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.TrainingCode = sqlTrainingCode.String</v>
+        <v>sienaAccount.Firm = sqlFirm.String</v>
       </c>
     </row>
     <row r="33" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>TrainingReceived    string</v>
+        <v>CCYDp    string</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="5"/>
-        <v>TrainingReceived    string</v>
+        <v>CCYDp    string</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
-        <v>TrainingReceived:    returnRecord.TrainingReceived,</v>
+        <v>CCYDp:    returnRecord.CCYDp,</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="2"/>
-        <v>TrainingReceived:    "",</v>
+        <v>CCYDp:    "",</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.TrainingReceived = sqlCPEXTrainingReceived.String</v>
+        <v>sienaAccount.CCYDp = sqlACCTCCYDp.String</v>
       </c>
       <c r="V33" t="str">
         <f t="shared" si="3"/>
-        <v>item.TrainingReceived = r.FormValue("TrainingReceived")</v>
+        <v>item.CCYDp = r.FormValue("CCYDp")</v>
       </c>
       <c r="AD33" t="str">
         <f t="shared" si="4"/>
-        <v>.TrainingReceived</v>
+        <v>.CCYDp</v>
       </c>
       <c r="AG33" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.TrainingReceived = sqlTrainingReceived.String</v>
+        <v>sienaAccount.CCYDp = sqlCCYDp.String</v>
       </c>
     </row>
     <row r="34" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="B34" s="1"/>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>Unencumbered    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="5"/>
-        <v>Unencumbered    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
-        <v>Unencumbered:    returnRecord.Unencumbered,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="2"/>
-        <v>Unencumbered:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.Unencumbered = sqlCPEXUnencumbered.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V34" t="str">
         <f t="shared" si="3"/>
-        <v>item.Unencumbered = r.FormValue("Unencumbered")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD34" t="str">
         <f t="shared" si="4"/>
-        <v>.Unencumbered</v>
+        <v>.</v>
       </c>
       <c r="AG34" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.Unencumbered = sqlUnencumbered.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="35" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="B35" s="1"/>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>LEIExpiryDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="5"/>
-        <v>LEIExpiryDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
-        <v>LEIExpiryDate:    returnRecord.LEIExpiryDate,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="2"/>
-        <v>LEIExpiryDate:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.LEIExpiryDate = sqlCPEXLEIExpiryDate.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V35" t="str">
         <f t="shared" si="3"/>
-        <v>item.LEIExpiryDate = r.FormValue("LEIExpiryDate")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD35" t="str">
         <f t="shared" si="4"/>
-        <v>.LEIExpiryDate</v>
+        <v>.</v>
       </c>
       <c r="AG35" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.LEIExpiryDate = sqlLEIExpiryDate.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="36" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="B36" s="1"/>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>MIFIDReviewDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="5"/>
-        <v>MIFIDReviewDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
-        <v>MIFIDReviewDate:    returnRecord.MIFIDReviewDate,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="2"/>
-        <v>MIFIDReviewDate:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.MIFIDReviewDate = sqlCPEXMIFIDReviewDate.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V36" t="str">
         <f t="shared" si="3"/>
-        <v>item.MIFIDReviewDate = r.FormValue("MIFIDReviewDate")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD36" t="str">
         <f t="shared" si="4"/>
-        <v>.MIFIDReviewDate</v>
+        <v>.</v>
       </c>
       <c r="AG36" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.MIFIDReviewDate = sqlMIFIDReviewDate.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="37" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="B37" s="1"/>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>GDPRReviewDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="5"/>
-        <v>GDPRReviewDate    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
-        <v>GDPRReviewDate:    returnRecord.GDPRReviewDate,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="2"/>
-        <v>GDPRReviewDate:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.GDPRReviewDate = sqlCPEXGDPRReviewDate.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V37" t="str">
         <f t="shared" si="3"/>
-        <v>item.GDPRReviewDate = r.FormValue("GDPRReviewDate")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD37" t="str">
         <f t="shared" si="4"/>
-        <v>.GDPRReviewDate</v>
+        <v>.</v>
       </c>
       <c r="AG37" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.GDPRReviewDate = sqlGDPRReviewDate.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="38" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="B38" s="1"/>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>DelegatedReporting    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="5"/>
-        <v>DelegatedReporting    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
-        <v>DelegatedReporting:    returnRecord.DelegatedReporting,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="2"/>
-        <v>DelegatedReporting:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.DelegatedReporting = sqlCPEXDelegatedReporting.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V38" t="str">
         <f t="shared" si="3"/>
-        <v>item.DelegatedReporting = r.FormValue("DelegatedReporting")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD38" t="str">
         <f t="shared" si="4"/>
-        <v>.DelegatedReporting</v>
+        <v>.</v>
       </c>
       <c r="AG38" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.DelegatedReporting = sqlDelegatedReporting.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="39" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>BOReconcile    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="5"/>
-        <v>BOReconcile    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
-        <v>BOReconcile:    returnRecord.BOReconcile,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="2"/>
-        <v>BOReconcile:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.BOReconcile = sqlCPEXBOReconcile.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V39" t="str">
         <f t="shared" si="3"/>
-        <v>item.BOReconcile = r.FormValue("BOReconcile")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD39" t="str">
         <f t="shared" si="4"/>
-        <v>.BOReconcile</v>
+        <v>.</v>
       </c>
       <c r="AG39" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.BOReconcile = sqlBOReconcile.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="40" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="B40" s="1"/>
       <c r="D40" t="str">
         <f t="shared" ref="D40:D62" si="8">B40&amp;"    string"</f>
-        <v>MIFIDReportableDealsAllowed    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" ref="E40:E62" si="9">D40</f>
-        <v>MIFIDReportableDealsAllowed    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" ref="G40:G62" si="10">B40&amp;":    "&amp;$F$4&amp;B40&amp;","</f>
-        <v>MIFIDReportableDealsAllowed:    returnRecord.MIFIDReportableDealsAllowed,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" ref="H40:H62" si="11">B40&amp;":    """""&amp;","</f>
-        <v>MIFIDReportableDealsAllowed:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.MIFIDReportableDealsAllowed = sqlCPEXMIFIDReportableDealsAllowed.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V40" t="str">
         <f t="shared" ref="V40:V62" si="12">"item."&amp;B40&amp;" = r.FormValue("""&amp;B40&amp;""")"</f>
-        <v>item.MIFIDReportableDealsAllowed = r.FormValue("MIFIDReportableDealsAllowed")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD40" t="str">
         <f t="shared" ref="AD40:AD62" si="13">"."&amp;B40</f>
-        <v>.MIFIDReportableDealsAllowed</v>
+        <v>.</v>
       </c>
       <c r="AG40" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.MIFIDReportableDealsAllowed = sqlMIFIDReportableDealsAllowed.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="41" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="B41" s="1"/>
       <c r="D41" t="str">
         <f t="shared" si="8"/>
-        <v>SignedInvestmentAgreement    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="9"/>
-        <v>SignedInvestmentAgreement    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="10"/>
-        <v>SignedInvestmentAgreement:    returnRecord.SignedInvestmentAgreement,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="11"/>
-        <v>SignedInvestmentAgreement:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.SignedInvestmentAgreement = sqlCPEXSignedInvestmentAgreement.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V41" t="str">
         <f t="shared" si="12"/>
-        <v>item.SignedInvestmentAgreement = r.FormValue("SignedInvestmentAgreement")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD41" t="str">
         <f t="shared" si="13"/>
-        <v>.SignedInvestmentAgreement</v>
+        <v>.</v>
       </c>
       <c r="AG41" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.SignedInvestmentAgreement = sqlSignedInvestmentAgreement.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="42" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="B42" s="1"/>
       <c r="D42" t="str">
         <f t="shared" si="8"/>
-        <v>AppropriatenessAssessment    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="9"/>
-        <v>AppropriatenessAssessment    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="10"/>
-        <v>AppropriatenessAssessment:    returnRecord.AppropriatenessAssessment,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="11"/>
-        <v>AppropriatenessAssessment:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.AppropriatenessAssessment = sqlCPEXAppropriatenessAssessment.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V42" t="str">
         <f t="shared" si="12"/>
-        <v>item.AppropriatenessAssessment = r.FormValue("AppropriatenessAssessment")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD42" t="str">
         <f t="shared" si="13"/>
-        <v>.AppropriatenessAssessment</v>
+        <v>.</v>
       </c>
       <c r="AG42" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.AppropriatenessAssessment = sqlAppropriatenessAssessment.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="43" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="B43" s="1"/>
       <c r="D43" t="str">
         <f t="shared" si="8"/>
-        <v>FinancialCounterparty    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="9"/>
-        <v>FinancialCounterparty    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="10"/>
-        <v>FinancialCounterparty:    returnRecord.FinancialCounterparty,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="11"/>
-        <v>FinancialCounterparty:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.FinancialCounterparty = sqlCPEXFinancialCounterparty.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V43" t="str">
         <f t="shared" si="12"/>
-        <v>item.FinancialCounterparty = r.FormValue("FinancialCounterparty")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD43" t="str">
         <f t="shared" si="13"/>
-        <v>.FinancialCounterparty</v>
+        <v>.</v>
       </c>
       <c r="AG43" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.FinancialCounterparty = sqlFinancialCounterparty.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="44" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="B44" s="1"/>
       <c r="D44" t="str">
         <f t="shared" si="8"/>
-        <v>Collateralisation    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="9"/>
-        <v>Collateralisation    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="10"/>
-        <v>Collateralisation:    returnRecord.Collateralisation,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="11"/>
-        <v>Collateralisation:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.Collateralisation = sqlCPEXCollateralisation.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V44" t="str">
         <f t="shared" si="12"/>
-        <v>item.Collateralisation = r.FormValue("Collateralisation")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD44" t="str">
         <f t="shared" si="13"/>
-        <v>.Collateralisation</v>
+        <v>.</v>
       </c>
       <c r="AG44" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.Collateralisation = sqlCollateralisation.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="45" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="B45" s="1"/>
       <c r="D45" t="str">
         <f t="shared" si="8"/>
-        <v>PortfolioCode    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="9"/>
-        <v>PortfolioCode    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="10"/>
-        <v>PortfolioCode:    returnRecord.PortfolioCode,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="11"/>
-        <v>PortfolioCode:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.PortfolioCode = sqlCPEXPortfolioCode.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V45" t="str">
         <f t="shared" si="12"/>
-        <v>item.PortfolioCode = r.FormValue("PortfolioCode")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD45" t="str">
         <f t="shared" si="13"/>
-        <v>.PortfolioCode</v>
+        <v>.</v>
       </c>
       <c r="AG45" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.PortfolioCode = sqlPortfolioCode.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="46" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="B46" s="1"/>
       <c r="D46" t="str">
         <f t="shared" si="8"/>
-        <v>ReconciliationLetterFrequency    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="9"/>
-        <v>ReconciliationLetterFrequency    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="10"/>
-        <v>ReconciliationLetterFrequency:    returnRecord.ReconciliationLetterFrequency,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="11"/>
-        <v>ReconciliationLetterFrequency:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.ReconciliationLetterFrequency = sqlCPEXReconciliationLetterFrequency.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V46" t="str">
         <f t="shared" si="12"/>
-        <v>item.ReconciliationLetterFrequency = r.FormValue("ReconciliationLetterFrequency")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD46" t="str">
         <f t="shared" si="13"/>
-        <v>.ReconciliationLetterFrequency</v>
+        <v>.</v>
       </c>
       <c r="AG46" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.ReconciliationLetterFrequency = sqlReconciliationLetterFrequency.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="47" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="B47" s="1"/>
       <c r="D47" t="str">
         <f t="shared" si="8"/>
-        <v>DirectDealing    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="9"/>
-        <v>DirectDealing    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="10"/>
-        <v>DirectDealing:    returnRecord.DirectDealing,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="11"/>
-        <v>DirectDealing:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions.DirectDealing = sqlCPEXDirectDealing.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V47" t="str">
         <f t="shared" si="12"/>
-        <v>item.DirectDealing = r.FormValue("DirectDealing")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD47" t="str">
         <f t="shared" si="13"/>
-        <v>.DirectDealing</v>
+        <v>.</v>
       </c>
       <c r="AG47" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions.DirectDealing = sqlDirectDealing.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="48" spans="2:33" x14ac:dyDescent="0.2">
@@ -2268,7 +2198,7 @@
       </c>
       <c r="L48" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V48" t="str">
         <f t="shared" si="12"/>
@@ -2280,7 +2210,7 @@
       </c>
       <c r="AG48" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="49" spans="2:33" x14ac:dyDescent="0.2">
@@ -2303,7 +2233,7 @@
       </c>
       <c r="L49" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V49" t="str">
         <f t="shared" si="12"/>
@@ -2315,7 +2245,7 @@
       </c>
       <c r="AG49" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="50" spans="2:33" x14ac:dyDescent="0.2">
@@ -2338,7 +2268,7 @@
       </c>
       <c r="L50" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V50" t="str">
         <f t="shared" si="12"/>
@@ -2350,7 +2280,7 @@
       </c>
       <c r="AG50" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="51" spans="2:33" x14ac:dyDescent="0.2">
@@ -2373,7 +2303,7 @@
       </c>
       <c r="L51" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V51" t="str">
         <f t="shared" si="12"/>
@@ -2385,7 +2315,7 @@
       </c>
       <c r="AG51" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="52" spans="2:33" x14ac:dyDescent="0.2">
@@ -2408,7 +2338,7 @@
       </c>
       <c r="L52" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V52" t="str">
         <f t="shared" si="12"/>
@@ -2420,7 +2350,7 @@
       </c>
       <c r="AG52" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="53" spans="2:33" x14ac:dyDescent="0.2">
@@ -2443,7 +2373,7 @@
       </c>
       <c r="L53" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V53" t="str">
         <f t="shared" si="12"/>
@@ -2455,7 +2385,7 @@
       </c>
       <c r="AG53" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="54" spans="2:33" x14ac:dyDescent="0.2">
@@ -2478,7 +2408,7 @@
       </c>
       <c r="L54" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V54" t="str">
         <f t="shared" si="12"/>
@@ -2490,7 +2420,7 @@
       </c>
       <c r="AG54" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="55" spans="2:33" x14ac:dyDescent="0.2">
@@ -2513,7 +2443,7 @@
       </c>
       <c r="L55" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V55" t="str">
         <f t="shared" si="12"/>
@@ -2525,7 +2455,7 @@
       </c>
       <c r="AG55" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="56" spans="2:33" x14ac:dyDescent="0.2">
@@ -2548,7 +2478,7 @@
       </c>
       <c r="L56" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V56" t="str">
         <f t="shared" si="12"/>
@@ -2560,7 +2490,7 @@
       </c>
       <c r="AG56" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="57" spans="2:33" x14ac:dyDescent="0.2">
@@ -2583,7 +2513,7 @@
       </c>
       <c r="L57" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V57" t="str">
         <f t="shared" si="12"/>
@@ -2595,7 +2525,7 @@
       </c>
       <c r="AG57" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="58" spans="2:33" x14ac:dyDescent="0.2">
@@ -2618,7 +2548,7 @@
       </c>
       <c r="L58" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V58" t="str">
         <f t="shared" si="12"/>
@@ -2630,7 +2560,7 @@
       </c>
       <c r="AG58" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="59" spans="2:33" x14ac:dyDescent="0.2">
@@ -2653,7 +2583,7 @@
       </c>
       <c r="L59" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V59" t="str">
         <f t="shared" si="12"/>
@@ -2665,7 +2595,7 @@
       </c>
       <c r="AG59" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="60" spans="2:33" x14ac:dyDescent="0.2">
@@ -2688,7 +2618,7 @@
       </c>
       <c r="L60" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V60" t="str">
         <f t="shared" si="12"/>
@@ -2700,7 +2630,7 @@
       </c>
       <c r="AG60" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="61" spans="2:33" x14ac:dyDescent="0.2">
@@ -2723,7 +2653,7 @@
       </c>
       <c r="L61" t="str">
         <f t="shared" si="6"/>
-        <v>sienaCounterpartyExtensions. = sqlCPEX.String</v>
+        <v>sienaAccount. = sqlACCT.String</v>
       </c>
       <c r="V61" t="str">
         <f t="shared" si="12"/>
@@ -2735,7 +2665,7 @@
       </c>
       <c r="AG61" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="62" spans="2:33" x14ac:dyDescent="0.2">
@@ -2757,8 +2687,8 @@
         <v>:    "",</v>
       </c>
       <c r="L62" t="str">
-        <f t="shared" ref="L40:L62" si="14">$I$3&amp;"."&amp;B62&amp;" = "&amp;B62&amp;".String"</f>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <f t="shared" ref="L62" si="14">$I$3&amp;"."&amp;B62&amp;" = "&amp;B62&amp;".String"</f>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V62" t="str">
         <f t="shared" si="12"/>
@@ -2770,7 +2700,7 @@
       </c>
       <c r="AG62" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="63" spans="2:33" x14ac:dyDescent="0.2">
@@ -2793,7 +2723,7 @@
       </c>
       <c r="L63" t="str">
         <f t="shared" ref="L63:L74" si="19">$I$3&amp;"."&amp;B63&amp;" = "&amp;B63&amp;".String"</f>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V63" t="str">
         <f t="shared" ref="V63:V74" si="20">"item."&amp;B63&amp;" = r.FormValue("""&amp;B63&amp;""")"</f>
@@ -2805,7 +2735,7 @@
       </c>
       <c r="AG63" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="64" spans="2:33" x14ac:dyDescent="0.2">
@@ -2828,7 +2758,7 @@
       </c>
       <c r="L64" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V64" t="str">
         <f t="shared" si="20"/>
@@ -2840,7 +2770,7 @@
       </c>
       <c r="AG64" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="65" spans="2:33" x14ac:dyDescent="0.2">
@@ -2863,7 +2793,7 @@
       </c>
       <c r="L65" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V65" t="str">
         <f t="shared" si="20"/>
@@ -2875,7 +2805,7 @@
       </c>
       <c r="AG65" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="66" spans="2:33" x14ac:dyDescent="0.2">
@@ -2898,7 +2828,7 @@
       </c>
       <c r="L66" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V66" t="str">
         <f t="shared" si="20"/>
@@ -2910,7 +2840,7 @@
       </c>
       <c r="AG66" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="67" spans="2:33" x14ac:dyDescent="0.2">
@@ -2933,7 +2863,7 @@
       </c>
       <c r="L67" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V67" t="str">
         <f t="shared" si="20"/>
@@ -2945,7 +2875,7 @@
       </c>
       <c r="AG67" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="68" spans="2:33" x14ac:dyDescent="0.2">
@@ -2968,7 +2898,7 @@
       </c>
       <c r="L68" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V68" t="str">
         <f t="shared" si="20"/>
@@ -2980,7 +2910,7 @@
       </c>
       <c r="AG68" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="69" spans="2:33" x14ac:dyDescent="0.2">
@@ -3003,7 +2933,7 @@
       </c>
       <c r="L69" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V69" t="str">
         <f t="shared" si="20"/>
@@ -3015,7 +2945,7 @@
       </c>
       <c r="AG69" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="70" spans="2:33" x14ac:dyDescent="0.2">
@@ -3038,7 +2968,7 @@
       </c>
       <c r="L70" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V70" t="str">
         <f t="shared" si="20"/>
@@ -3050,7 +2980,7 @@
       </c>
       <c r="AG70" t="str">
         <f t="shared" si="7"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="71" spans="2:33" x14ac:dyDescent="0.2">
@@ -3073,7 +3003,7 @@
       </c>
       <c r="L71" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V71" t="str">
         <f t="shared" si="20"/>
@@ -3085,7 +3015,7 @@
       </c>
       <c r="AG71" t="str">
         <f t="shared" ref="AG71:AG74" si="22">$I$3&amp;"."&amp;B71&amp;" = sql"&amp;B71&amp;".String"</f>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="72" spans="2:33" x14ac:dyDescent="0.2">
@@ -3108,7 +3038,7 @@
       </c>
       <c r="L72" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V72" t="str">
         <f t="shared" si="20"/>
@@ -3120,7 +3050,7 @@
       </c>
       <c r="AG72" t="str">
         <f t="shared" si="22"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="73" spans="2:33" x14ac:dyDescent="0.2">
@@ -3143,7 +3073,7 @@
       </c>
       <c r="L73" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V73" t="str">
         <f t="shared" si="20"/>
@@ -3155,7 +3085,7 @@
       </c>
       <c r="AG73" t="str">
         <f t="shared" si="22"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
     <row r="74" spans="2:33" x14ac:dyDescent="0.2">
@@ -3178,7 +3108,7 @@
       </c>
       <c r="L74" t="str">
         <f t="shared" si="19"/>
-        <v>sienaCounterpartyExtensions. = .String</v>
+        <v>sienaAccount. = .String</v>
       </c>
       <c r="V74" t="str">
         <f t="shared" si="20"/>
@@ -3190,7 +3120,7 @@
       </c>
       <c r="AG74" t="str">
         <f t="shared" si="22"/>
-        <v>sienaCounterpartyExtensions. = sql.String</v>
+        <v>sienaAccount. = sql.String</v>
       </c>
     </row>
   </sheetData>
@@ -3202,8 +3132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90230AA-F0B1-6C49-B8FC-2C26A6B44982}">
   <dimension ref="A2:BK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:AR15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3216,13 +3146,13 @@
   <sheetData>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="G2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C3" t="str">
         <f>UPPER('GO Struct Bits'!B2)</f>
-        <v>CPEX</v>
+        <v>ACCT</v>
       </c>
     </row>
     <row r="6" spans="1:63" x14ac:dyDescent="0.2">
@@ -3231,130 +3161,130 @@
         <v>0</v>
       </c>
       <c r="C6" t="str">
-        <v>NameFirm</v>
+        <v>SienaReference</v>
       </c>
       <c r="D6" t="str">
-        <v>NameCentre</v>
+        <v>CustomerSienaView</v>
       </c>
       <c r="E6" t="str">
-        <v>BICCode</v>
+        <v>SienaCommonRef</v>
       </c>
       <c r="F6" t="str">
-        <v>ContactIndicator</v>
+        <v>Status</v>
       </c>
       <c r="G6" t="str">
-        <v>CoverTrade</v>
+        <v>StartDate</v>
       </c>
       <c r="H6" t="str">
-        <v>CustomerCategory</v>
+        <v>MaturityDate</v>
       </c>
       <c r="I6" t="str">
-        <v>FSCSInclusive</v>
+        <v>ContractNumber</v>
       </c>
       <c r="J6" t="str">
-        <v>FeeFactor</v>
+        <v>ExternalReference</v>
       </c>
       <c r="K6" t="str">
-        <v>InactiveStatus</v>
+        <v>CCY</v>
       </c>
       <c r="L6" t="str">
-        <v>Indemnity</v>
+        <v>Book</v>
       </c>
       <c r="M6" t="str">
-        <v>KnowYourCustomerStatus</v>
+        <v>MandatedUser</v>
       </c>
       <c r="N6" t="str">
-        <v>LERLimitCarveOut</v>
+        <v>BackOfficeNotes</v>
       </c>
       <c r="O6" t="str">
-        <v>LastAmended</v>
+        <v>CashBalance</v>
       </c>
       <c r="P6" t="str">
-        <v>LastLogin</v>
+        <v>AccountNumber</v>
       </c>
       <c r="Q6" t="str">
-        <v>LossGivenDefault</v>
+        <v>AccountName</v>
       </c>
       <c r="R6" t="str">
-        <v>MIC</v>
+        <v>LedgerBalance</v>
       </c>
       <c r="S6" t="str">
-        <v>ProtectedDepositor</v>
+        <v>Portfolio</v>
       </c>
       <c r="T6" t="str">
-        <v>RPTCurrency</v>
+        <v>AgreementId</v>
       </c>
       <c r="U6" t="str">
-        <v>RateTimeout</v>
+        <v>BackOfficeRefNo</v>
       </c>
       <c r="V6" t="str">
-        <v>RateValidation</v>
+        <v>PaymentSystemSienaView</v>
       </c>
       <c r="W6" t="str">
-        <v>Registered</v>
+        <v>ISIN</v>
       </c>
       <c r="X6" t="str">
-        <v>RegulatoryCategory</v>
+        <v>UTI</v>
       </c>
       <c r="Y6" t="str">
-        <v>SecuredSettlement</v>
+        <v>CCYName</v>
       </c>
       <c r="Z6" t="str">
-        <v>SettlementLimitCarveOut</v>
+        <v>BookName</v>
       </c>
       <c r="AA6" t="str">
-        <v>SortCode</v>
+        <v>PortfolioName</v>
       </c>
       <c r="AB6" t="str">
-        <v>Training</v>
+        <v>Centre</v>
       </c>
       <c r="AC6" t="str">
-        <v>TrainingCode</v>
+        <v>Firm</v>
       </c>
       <c r="AD6" t="str">
-        <v>TrainingReceived</v>
-      </c>
-      <c r="AE6" t="str">
-        <v>Unencumbered</v>
-      </c>
-      <c r="AF6" t="str">
-        <v>LEIExpiryDate</v>
-      </c>
-      <c r="AG6" t="str">
-        <v>MIFIDReviewDate</v>
-      </c>
-      <c r="AH6" t="str">
-        <v>GDPRReviewDate</v>
-      </c>
-      <c r="AI6" t="str">
-        <v>DelegatedReporting</v>
-      </c>
-      <c r="AJ6" t="str">
-        <v>BOReconcile</v>
-      </c>
-      <c r="AK6" t="str">
-        <v>MIFIDReportableDealsAllowed</v>
-      </c>
-      <c r="AL6" t="str">
-        <v>SignedInvestmentAgreement</v>
-      </c>
-      <c r="AM6" t="str">
-        <v>AppropriatenessAssessment</v>
-      </c>
-      <c r="AN6" t="str">
-        <v>FinancialCounterparty</v>
-      </c>
-      <c r="AO6" t="str">
-        <v>Collateralisation</v>
-      </c>
-      <c r="AP6" t="str">
-        <v>PortfolioCode</v>
-      </c>
-      <c r="AQ6" t="str">
-        <v>ReconciliationLetterFrequency</v>
-      </c>
-      <c r="AR6" t="str">
-        <v>DirectDealing</v>
+        <v>CCYDp</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
       </c>
       <c r="AS6">
         <v>0</v>
@@ -3368,179 +3298,179 @@
     </row>
     <row r="8" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="str">
         <f>"var siena"&amp;'GO Struct Bits'!B4&amp;"SQL"</f>
-        <v>var sienaCounterpartyExtensionsSQL</v>
+        <v>var sienaAccountSQL</v>
       </c>
       <c r="C8" t="str">
         <f>C6&amp;", "</f>
-        <v xml:space="preserve">NameFirm, </v>
+        <v xml:space="preserve">SienaReference, </v>
       </c>
       <c r="D8" t="str">
         <f t="shared" ref="D8:BK8" si="0">D6&amp;", "</f>
-        <v xml:space="preserve">NameCentre, </v>
+        <v xml:space="preserve">CustomerSienaView, </v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">BICCode, </v>
+        <v xml:space="preserve">SienaCommonRef, </v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ContactIndicator, </v>
+        <v xml:space="preserve">Status, </v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CoverTrade, </v>
+        <v xml:space="preserve">StartDate, </v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CustomerCategory, </v>
+        <v xml:space="preserve">MaturityDate, </v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">FSCSInclusive, </v>
+        <v xml:space="preserve">ContractNumber, </v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">FeeFactor, </v>
+        <v xml:space="preserve">ExternalReference, </v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">InactiveStatus, </v>
+        <v xml:space="preserve">CCY, </v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Indemnity, </v>
+        <v xml:space="preserve">Book, </v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">KnowYourCustomerStatus, </v>
+        <v xml:space="preserve">MandatedUser, </v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">LERLimitCarveOut, </v>
+        <v xml:space="preserve">BackOfficeNotes, </v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">LastAmended, </v>
+        <v xml:space="preserve">CashBalance, </v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">LastLogin, </v>
+        <v xml:space="preserve">AccountNumber, </v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">LossGivenDefault, </v>
+        <v xml:space="preserve">AccountName, </v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">MIC, </v>
+        <v xml:space="preserve">LedgerBalance, </v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ProtectedDepositor, </v>
+        <v xml:space="preserve">Portfolio, </v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">RPTCurrency, </v>
+        <v xml:space="preserve">AgreementId, </v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">RateTimeout, </v>
+        <v xml:space="preserve">BackOfficeRefNo, </v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">RateValidation, </v>
+        <v xml:space="preserve">PaymentSystemSienaView, </v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Registered, </v>
+        <v xml:space="preserve">ISIN, </v>
       </c>
       <c r="X8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">RegulatoryCategory, </v>
+        <v xml:space="preserve">UTI, </v>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SecuredSettlement, </v>
+        <v xml:space="preserve">CCYName, </v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SettlementLimitCarveOut, </v>
+        <v xml:space="preserve">BookName, </v>
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SortCode, </v>
+        <v xml:space="preserve">PortfolioName, </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Training, </v>
+        <v xml:space="preserve">Centre, </v>
       </c>
       <c r="AC8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">TrainingCode, </v>
+        <v xml:space="preserve">Firm, </v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">TrainingReceived, </v>
+        <v xml:space="preserve">CCYDp, </v>
       </c>
       <c r="AE8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Unencumbered, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AF8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">LEIExpiryDate, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AG8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">MIFIDReviewDate, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AH8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">GDPRReviewDate, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AI8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DelegatedReporting, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AJ8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">BOReconcile, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AK8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">MIFIDReportableDealsAllowed, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AL8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SignedInvestmentAgreement, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AM8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">AppropriatenessAssessment, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AN8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">FinancialCounterparty, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AO8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Collateralisation, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AP8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PortfolioCode, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AQ8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ReconciliationLetterFrequency, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AR8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">DirectDealing, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AS8" t="str">
         <f t="shared" si="0"/>
@@ -3622,171 +3552,171 @@
     <row r="10" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C10" t="str">
         <f>"&amp;"&amp;C8</f>
-        <v xml:space="preserve">&amp;NameFirm, </v>
+        <v xml:space="preserve">&amp;SienaReference, </v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ref="D10:BK10" si="1">"&amp;"&amp;D8</f>
-        <v xml:space="preserve">&amp;NameCentre, </v>
+        <v xml:space="preserve">&amp;CustomerSienaView, </v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;BICCode, </v>
+        <v xml:space="preserve">&amp;SienaCommonRef, </v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ContactIndicator, </v>
+        <v xml:space="preserve">&amp;Status, </v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;CoverTrade, </v>
+        <v xml:space="preserve">&amp;StartDate, </v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;CustomerCategory, </v>
+        <v xml:space="preserve">&amp;MaturityDate, </v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;FSCSInclusive, </v>
+        <v xml:space="preserve">&amp;ContractNumber, </v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;FeeFactor, </v>
+        <v xml:space="preserve">&amp;ExternalReference, </v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;InactiveStatus, </v>
+        <v xml:space="preserve">&amp;CCY, </v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Indemnity, </v>
+        <v xml:space="preserve">&amp;Book, </v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;KnowYourCustomerStatus, </v>
+        <v xml:space="preserve">&amp;MandatedUser, </v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;LERLimitCarveOut, </v>
+        <v xml:space="preserve">&amp;BackOfficeNotes, </v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;LastAmended, </v>
+        <v xml:space="preserve">&amp;CashBalance, </v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;LastLogin, </v>
+        <v xml:space="preserve">&amp;AccountNumber, </v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;LossGivenDefault, </v>
+        <v xml:space="preserve">&amp;AccountName, </v>
       </c>
       <c r="R10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;MIC, </v>
+        <v xml:space="preserve">&amp;LedgerBalance, </v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ProtectedDepositor, </v>
+        <v xml:space="preserve">&amp;Portfolio, </v>
       </c>
       <c r="T10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;RPTCurrency, </v>
+        <v xml:space="preserve">&amp;AgreementId, </v>
       </c>
       <c r="U10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;RateTimeout, </v>
+        <v xml:space="preserve">&amp;BackOfficeRefNo, </v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;RateValidation, </v>
+        <v xml:space="preserve">&amp;PaymentSystemSienaView, </v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Registered, </v>
+        <v xml:space="preserve">&amp;ISIN, </v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;RegulatoryCategory, </v>
+        <v xml:space="preserve">&amp;UTI, </v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;SecuredSettlement, </v>
+        <v xml:space="preserve">&amp;CCYName, </v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;SettlementLimitCarveOut, </v>
+        <v xml:space="preserve">&amp;BookName, </v>
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;SortCode, </v>
+        <v xml:space="preserve">&amp;PortfolioName, </v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Training, </v>
+        <v xml:space="preserve">&amp;Centre, </v>
       </c>
       <c r="AC10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;TrainingCode, </v>
+        <v xml:space="preserve">&amp;Firm, </v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;TrainingReceived, </v>
+        <v xml:space="preserve">&amp;CCYDp, </v>
       </c>
       <c r="AE10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Unencumbered, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AF10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;LEIExpiryDate, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AG10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;MIFIDReviewDate, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AH10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;GDPRReviewDate, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AI10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;DelegatedReporting, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AJ10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;BOReconcile, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AK10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;MIFIDReportableDealsAllowed, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AL10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;SignedInvestmentAgreement, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AM10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;AppropriatenessAssessment, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AN10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;FinancialCounterparty, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AO10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Collateralisation, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AP10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;PortfolioCode, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AQ10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ReconciliationLetterFrequency, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AR10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;DirectDealing, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AS10" t="str">
         <f t="shared" si="1"/>
@@ -3871,372 +3801,372 @@
       </c>
       <c r="C13" t="str">
         <f>"sql"&amp;$C$3&amp;""&amp;C8</f>
-        <v xml:space="preserve">sqlCPEXNameFirm, </v>
+        <v xml:space="preserve">sqlACCTSienaReference, </v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ref="D13:AY13" si="2">"sql"&amp;$C$3&amp;""&amp;D8</f>
-        <v xml:space="preserve">sqlCPEXNameCentre, </v>
+        <v xml:space="preserve">sqlACCTCustomerSienaView, </v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXBICCode, </v>
+        <v xml:space="preserve">sqlACCTSienaCommonRef, </v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXContactIndicator, </v>
+        <v xml:space="preserve">sqlACCTStatus, </v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXCoverTrade, </v>
+        <v xml:space="preserve">sqlACCTStartDate, </v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXCustomerCategory, </v>
+        <v xml:space="preserve">sqlACCTMaturityDate, </v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXFSCSInclusive, </v>
+        <v xml:space="preserve">sqlACCTContractNumber, </v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXFeeFactor, </v>
+        <v xml:space="preserve">sqlACCTExternalReference, </v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXInactiveStatus, </v>
+        <v xml:space="preserve">sqlACCTCCY, </v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXIndemnity, </v>
+        <v xml:space="preserve">sqlACCTBook, </v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXKnowYourCustomerStatus, </v>
+        <v xml:space="preserve">sqlACCTMandatedUser, </v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXLERLimitCarveOut, </v>
+        <v xml:space="preserve">sqlACCTBackOfficeNotes, </v>
       </c>
       <c r="O13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXLastAmended, </v>
+        <v xml:space="preserve">sqlACCTCashBalance, </v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXLastLogin, </v>
+        <v xml:space="preserve">sqlACCTAccountNumber, </v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXLossGivenDefault, </v>
+        <v xml:space="preserve">sqlACCTAccountName, </v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXMIC, </v>
+        <v xml:space="preserve">sqlACCTLedgerBalance, </v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXProtectedDepositor, </v>
+        <v xml:space="preserve">sqlACCTPortfolio, </v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXRPTCurrency, </v>
+        <v xml:space="preserve">sqlACCTAgreementId, </v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXRateTimeout, </v>
+        <v xml:space="preserve">sqlACCTBackOfficeRefNo, </v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXRateValidation, </v>
+        <v xml:space="preserve">sqlACCTPaymentSystemSienaView, </v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXRegistered, </v>
+        <v xml:space="preserve">sqlACCTISIN, </v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXRegulatoryCategory, </v>
+        <v xml:space="preserve">sqlACCTUTI, </v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXSecuredSettlement, </v>
+        <v xml:space="preserve">sqlACCTCCYName, </v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXSettlementLimitCarveOut, </v>
+        <v xml:space="preserve">sqlACCTBookName, </v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXSortCode, </v>
+        <v xml:space="preserve">sqlACCTPortfolioName, </v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXTraining, </v>
+        <v xml:space="preserve">sqlACCTCentre, </v>
       </c>
       <c r="AC13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXTrainingCode, </v>
+        <v xml:space="preserve">sqlACCTFirm, </v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXTrainingReceived, </v>
+        <v xml:space="preserve">sqlACCTCCYDp, </v>
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXUnencumbered, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AF13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXLEIExpiryDate, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AG13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXMIFIDReviewDate, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AH13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXGDPRReviewDate, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AI13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXDelegatedReporting, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AJ13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXBOReconcile, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AK13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXMIFIDReportableDealsAllowed, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AL13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXSignedInvestmentAgreement, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AM13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXAppropriatenessAssessment, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AN13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXFinancialCounterparty, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AO13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXCollateralisation, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AP13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXPortfolioCode, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AQ13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXReconciliationLetterFrequency, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AR13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEXDirectDealing, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AS13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEX0, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AT13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEX0, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AU13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEX0, </v>
+        <v xml:space="preserve">sqlACCT0, </v>
       </c>
       <c r="AV13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEX, </v>
+        <v xml:space="preserve">sqlACCT, </v>
       </c>
       <c r="AW13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEX, </v>
+        <v xml:space="preserve">sqlACCT, </v>
       </c>
       <c r="AX13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEX, </v>
+        <v xml:space="preserve">sqlACCT, </v>
       </c>
       <c r="AY13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlCPEX, </v>
+        <v xml:space="preserve">sqlACCT, </v>
       </c>
     </row>
     <row r="15" spans="1:63" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="str">
         <f>"&amp;"&amp;C13</f>
-        <v xml:space="preserve">&amp;sqlCPEXNameFirm, </v>
+        <v xml:space="preserve">&amp;sqlACCTSienaReference, </v>
       </c>
       <c r="D15" t="str">
         <f t="shared" ref="D15:AR15" si="3">"&amp;"&amp;D13</f>
-        <v xml:space="preserve">&amp;sqlCPEXNameCentre, </v>
+        <v xml:space="preserve">&amp;sqlACCTCustomerSienaView, </v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXBICCode, </v>
+        <v xml:space="preserve">&amp;sqlACCTSienaCommonRef, </v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXContactIndicator, </v>
+        <v xml:space="preserve">&amp;sqlACCTStatus, </v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXCoverTrade, </v>
+        <v xml:space="preserve">&amp;sqlACCTStartDate, </v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXCustomerCategory, </v>
+        <v xml:space="preserve">&amp;sqlACCTMaturityDate, </v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXFSCSInclusive, </v>
+        <v xml:space="preserve">&amp;sqlACCTContractNumber, </v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXFeeFactor, </v>
+        <v xml:space="preserve">&amp;sqlACCTExternalReference, </v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXInactiveStatus, </v>
+        <v xml:space="preserve">&amp;sqlACCTCCY, </v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXIndemnity, </v>
+        <v xml:space="preserve">&amp;sqlACCTBook, </v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXKnowYourCustomerStatus, </v>
+        <v xml:space="preserve">&amp;sqlACCTMandatedUser, </v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXLERLimitCarveOut, </v>
+        <v xml:space="preserve">&amp;sqlACCTBackOfficeNotes, </v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXLastAmended, </v>
+        <v xml:space="preserve">&amp;sqlACCTCashBalance, </v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXLastLogin, </v>
+        <v xml:space="preserve">&amp;sqlACCTAccountNumber, </v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXLossGivenDefault, </v>
+        <v xml:space="preserve">&amp;sqlACCTAccountName, </v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXMIC, </v>
+        <v xml:space="preserve">&amp;sqlACCTLedgerBalance, </v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXProtectedDepositor, </v>
+        <v xml:space="preserve">&amp;sqlACCTPortfolio, </v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXRPTCurrency, </v>
+        <v xml:space="preserve">&amp;sqlACCTAgreementId, </v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXRateTimeout, </v>
+        <v xml:space="preserve">&amp;sqlACCTBackOfficeRefNo, </v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXRateValidation, </v>
+        <v xml:space="preserve">&amp;sqlACCTPaymentSystemSienaView, </v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXRegistered, </v>
+        <v xml:space="preserve">&amp;sqlACCTISIN, </v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXRegulatoryCategory, </v>
+        <v xml:space="preserve">&amp;sqlACCTUTI, </v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXSecuredSettlement, </v>
+        <v xml:space="preserve">&amp;sqlACCTCCYName, </v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXSettlementLimitCarveOut, </v>
+        <v xml:space="preserve">&amp;sqlACCTBookName, </v>
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXSortCode, </v>
+        <v xml:space="preserve">&amp;sqlACCTPortfolioName, </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXTraining, </v>
+        <v xml:space="preserve">&amp;sqlACCTCentre, </v>
       </c>
       <c r="AC15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXTrainingCode, </v>
+        <v xml:space="preserve">&amp;sqlACCTFirm, </v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXTrainingReceived, </v>
+        <v xml:space="preserve">&amp;sqlACCTCCYDp, </v>
       </c>
       <c r="AE15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXUnencumbered, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AF15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXLEIExpiryDate, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AG15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXMIFIDReviewDate, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AH15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXGDPRReviewDate, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AI15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXDelegatedReporting, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AJ15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXBOReconcile, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AK15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXMIFIDReportableDealsAllowed, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AL15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXSignedInvestmentAgreement, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AM15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXAppropriatenessAssessment, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AN15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXFinancialCounterparty, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AO15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXCollateralisation, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AP15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXPortfolioCode, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AQ15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXReconciliationLetterFrequency, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
       <c r="AR15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlCPEXDirectDealing, </v>
+        <v xml:space="preserve">&amp;sqlACCT0, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major Style Update + Some Fixes - Pre Prototype Dashboard
</commit_message>
<xml_diff>
--- a/design/sienaDataArraysBuilder.xlsx
+++ b/design/sienaDataArraysBuilder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10317"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matttownsend/go/mwt-go-dev/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA68C24-E5A4-D44F-ABEB-645181ECE1F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71080FED-0869-1149-9071-080FBEA7B38B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34660" yWindow="-3580" windowWidth="26320" windowHeight="18000" xr2:uid="{8265F428-BA81-814D-9171-A3F66298AE69}"/>
+    <workbookView xWindow="-38400" yWindow="-5600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{8265F428-BA81-814D-9171-A3F66298AE69}"/>
   </bookViews>
   <sheets>
     <sheet name="GO Struct Bits" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>returnRecord.</t>
   </si>
@@ -81,94 +81,28 @@
     <t>ROWS&gt;&gt;&gt;&gt;</t>
   </si>
   <si>
-    <t>Account</t>
+    <t>CAL</t>
   </si>
   <si>
-    <t>ACCT</t>
+    <t>Calender</t>
   </si>
   <si>
-    <t>SienaReference</t>
+    <t>ID</t>
   </si>
   <si>
-    <t>CustomerSienaView</t>
+    <t>Source</t>
   </si>
   <si>
-    <t>SienaCommonRef</t>
+    <t>Date</t>
   </si>
   <si>
-    <t>Status</t>
+    <t>Time</t>
   </si>
   <si>
-    <t>StartDate</t>
+    <t>ShortName</t>
   </si>
   <si>
-    <t>MaturityDate</t>
-  </si>
-  <si>
-    <t>ContractNumber</t>
-  </si>
-  <si>
-    <t>ExternalReference</t>
-  </si>
-  <si>
-    <t>CCY</t>
-  </si>
-  <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>MandatedUser</t>
-  </si>
-  <si>
-    <t>BackOfficeNotes</t>
-  </si>
-  <si>
-    <t>CashBalance</t>
-  </si>
-  <si>
-    <t>AccountNumber</t>
-  </si>
-  <si>
-    <t>AccountName</t>
-  </si>
-  <si>
-    <t>LedgerBalance</t>
-  </si>
-  <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
-    <t>AgreementId</t>
-  </si>
-  <si>
-    <t>BackOfficeRefNo</t>
-  </si>
-  <si>
-    <t>PaymentSystemSienaView</t>
-  </si>
-  <si>
-    <t>ISIN</t>
-  </si>
-  <si>
-    <t>UTI</t>
-  </si>
-  <si>
-    <t>CCYName</t>
-  </si>
-  <si>
-    <t>BookName</t>
-  </si>
-  <si>
-    <t>PortfolioName</t>
-  </si>
-  <si>
-    <t>Centre</t>
-  </si>
-  <si>
-    <t>Firm</t>
-  </si>
-  <si>
-    <t>CCYDp</t>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -587,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4CE648-3973-0F42-A3A6-4E494BE264E6}">
   <dimension ref="B2:AG74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,37 +547,37 @@
   <sheetData>
     <row r="2" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="str">
         <f>"siena"&amp;B4&amp;".go"</f>
-        <v>sienaAccount.go</v>
+        <v>sienaCalender.go</v>
       </c>
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.2">
       <c r="I3" t="str">
         <f>"siena"&amp;B4</f>
-        <v>sienaAccount</v>
+        <v>sienaCalender</v>
       </c>
     </row>
     <row r="4" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>"siena"&amp;B4&amp;"Page"</f>
-        <v>sienaAccountPage</v>
+        <v>sienaCalenderPage</v>
       </c>
       <c r="E4" s="2" t="str">
         <f>"siena"&amp;B4&amp;"Item"</f>
-        <v>sienaAccountItem</v>
+        <v>sienaCalenderItem</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="str">
         <f>"newSiena"&amp;B4&amp;"Handler"</f>
-        <v>newSienaAccountHandler</v>
+        <v>newSienaCalenderHandler</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>2</v>
@@ -658,35 +592,35 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" ref="D6:D39" si="0">B6&amp;"    string"</f>
-        <v>SienaReference    string</v>
+        <v>ID    string</v>
       </c>
       <c r="E6" t="str">
         <f>D6</f>
-        <v>SienaReference    string</v>
+        <v>ID    string</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ref="G6:G39" si="1">B6&amp;":    "&amp;$F$4&amp;B6&amp;","</f>
-        <v>SienaReference:    returnRecord.SienaReference,</v>
+        <v>ID:    returnRecord.ID,</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" ref="H6:H39" si="2">B6&amp;":    """""&amp;","</f>
-        <v>SienaReference:    "",</v>
+        <v>ID:    "",</v>
       </c>
       <c r="L6" t="str">
         <f>$I$3&amp;"."&amp;B6&amp;" = sql"&amp;$B$2&amp;B6&amp;".String"</f>
-        <v>sienaAccount.SienaReference = sqlACCTSienaReference.String</v>
+        <v>sienaCalender.ID = sqlCALID.String</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" ref="V6:V39" si="3">"item."&amp;B6&amp;" = r.FormValue("""&amp;B6&amp;""")"</f>
-        <v>item.SienaReference = r.FormValue("SienaReference")</v>
+        <v>item.ID = r.FormValue("ID")</v>
       </c>
       <c r="AD6" t="str">
         <f t="shared" ref="AD6:AD39" si="4">"."&amp;B6</f>
-        <v>.SienaReference</v>
+        <v>.ID</v>
       </c>
       <c r="AG6" t="str">
         <f>$I$3&amp;"."&amp;B6&amp;" = sql"&amp;B6&amp;".String"</f>
-        <v>sienaAccount.SienaReference = sqlSienaReference.String</v>
+        <v>sienaCalender.ID = sqlID.String</v>
       </c>
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.2">
@@ -695,35 +629,35 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>CustomerSienaView    string</v>
+        <v>Source    string</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" ref="E7:E39" si="5">D7</f>
-        <v>CustomerSienaView    string</v>
+        <v>Source    string</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>CustomerSienaView:    returnRecord.CustomerSienaView,</v>
+        <v>Source:    returnRecord.Source,</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="2"/>
-        <v>CustomerSienaView:    "",</v>
+        <v>Source:    "",</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ref="L7:L61" si="6">$I$3&amp;"."&amp;B7&amp;" = sql"&amp;$B$2&amp;B7&amp;".String"</f>
-        <v>sienaAccount.CustomerSienaView = sqlACCTCustomerSienaView.String</v>
+        <v>sienaCalender.Source = sqlCALSource.String</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="3"/>
-        <v>item.CustomerSienaView = r.FormValue("CustomerSienaView")</v>
+        <v>item.Source = r.FormValue("Source")</v>
       </c>
       <c r="AD7" t="str">
         <f t="shared" si="4"/>
-        <v>.CustomerSienaView</v>
+        <v>.Source</v>
       </c>
       <c r="AG7" t="str">
         <f t="shared" ref="AG7:AG70" si="7">$I$3&amp;"."&amp;B7&amp;" = sql"&amp;B7&amp;".String"</f>
-        <v>sienaAccount.CustomerSienaView = sqlCustomerSienaView.String</v>
+        <v>sienaCalender.Source = sqlSource.String</v>
       </c>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.2">
@@ -732,35 +666,35 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>SienaCommonRef    string</v>
+        <v>Date    string</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="5"/>
-        <v>SienaCommonRef    string</v>
+        <v>Date    string</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>SienaCommonRef:    returnRecord.SienaCommonRef,</v>
+        <v>Date:    returnRecord.Date,</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="2"/>
-        <v>SienaCommonRef:    "",</v>
+        <v>Date:    "",</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.SienaCommonRef = sqlACCTSienaCommonRef.String</v>
+        <v>sienaCalender.Date = sqlCALDate.String</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="3"/>
-        <v>item.SienaCommonRef = r.FormValue("SienaCommonRef")</v>
+        <v>item.Date = r.FormValue("Date")</v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="4"/>
-        <v>.SienaCommonRef</v>
+        <v>.Date</v>
       </c>
       <c r="AG8" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.SienaCommonRef = sqlSienaCommonRef.String</v>
+        <v>sienaCalender.Date = sqlDate.String</v>
       </c>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.2">
@@ -769,35 +703,35 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>Status    string</v>
+        <v>Time    string</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="5"/>
-        <v>Status    string</v>
+        <v>Time    string</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>Status:    returnRecord.Status,</v>
+        <v>Time:    returnRecord.Time,</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="2"/>
-        <v>Status:    "",</v>
+        <v>Time:    "",</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.Status = sqlACCTStatus.String</v>
+        <v>sienaCalender.Time = sqlCALTime.String</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="3"/>
-        <v>item.Status = r.FormValue("Status")</v>
+        <v>item.Time = r.FormValue("Time")</v>
       </c>
       <c r="AD9" t="str">
         <f t="shared" si="4"/>
-        <v>.Status</v>
+        <v>.Time</v>
       </c>
       <c r="AG9" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.Status = sqlStatus.String</v>
+        <v>sienaCalender.Time = sqlTime.String</v>
       </c>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.2">
@@ -806,35 +740,35 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>StartDate    string</v>
+        <v>ShortName    string</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="5"/>
-        <v>StartDate    string</v>
+        <v>ShortName    string</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>StartDate:    returnRecord.StartDate,</v>
+        <v>ShortName:    returnRecord.ShortName,</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="2"/>
-        <v>StartDate:    "",</v>
+        <v>ShortName:    "",</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.StartDate = sqlACCTStartDate.String</v>
+        <v>sienaCalender.ShortName = sqlCALShortName.String</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="3"/>
-        <v>item.StartDate = r.FormValue("StartDate")</v>
+        <v>item.ShortName = r.FormValue("ShortName")</v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="4"/>
-        <v>.StartDate</v>
+        <v>.ShortName</v>
       </c>
       <c r="AG10" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.StartDate = sqlStartDate.String</v>
+        <v>sienaCalender.ShortName = sqlShortName.String</v>
       </c>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.2">
@@ -843,849 +777,805 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>MaturityDate    string</v>
+        <v>Description    string</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="5"/>
-        <v>MaturityDate    string</v>
+        <v>Description    string</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
-        <v>MaturityDate:    returnRecord.MaturityDate,</v>
+        <v>Description:    returnRecord.Description,</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="2"/>
-        <v>MaturityDate:    "",</v>
+        <v>Description:    "",</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.MaturityDate = sqlACCTMaturityDate.String</v>
+        <v>sienaCalender.Description = sqlCALDescription.String</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="3"/>
-        <v>item.MaturityDate = r.FormValue("MaturityDate")</v>
+        <v>item.Description = r.FormValue("Description")</v>
       </c>
       <c r="AD11" t="str">
         <f t="shared" si="4"/>
-        <v>.MaturityDate</v>
+        <v>.Description</v>
       </c>
       <c r="AG11" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.MaturityDate = sqlMaturityDate.String</v>
+        <v>sienaCalender.Description = sqlDescription.String</v>
       </c>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>ContractNumber    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="5"/>
-        <v>ContractNumber    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
-        <v>ContractNumber:    returnRecord.ContractNumber,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="2"/>
-        <v>ContractNumber:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.ContractNumber = sqlACCTContractNumber.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="3"/>
-        <v>item.ContractNumber = r.FormValue("ContractNumber")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD12" t="str">
         <f t="shared" si="4"/>
-        <v>.ContractNumber</v>
+        <v>.</v>
       </c>
       <c r="AG12" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.ContractNumber = sqlContractNumber.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>ExternalReference    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="5"/>
-        <v>ExternalReference    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
-        <v>ExternalReference:    returnRecord.ExternalReference,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
-        <v>ExternalReference:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.ExternalReference = sqlACCTExternalReference.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="3"/>
-        <v>item.ExternalReference = r.FormValue("ExternalReference")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="4"/>
-        <v>.ExternalReference</v>
+        <v>.</v>
       </c>
       <c r="AG13" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.ExternalReference = sqlExternalReference.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>CCY    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="5"/>
-        <v>CCY    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
-        <v>CCY:    returnRecord.CCY,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="2"/>
-        <v>CCY:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.CCY = sqlACCTCCY.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="3"/>
-        <v>item.CCY = r.FormValue("CCY")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD14" t="str">
         <f t="shared" si="4"/>
-        <v>.CCY</v>
+        <v>.</v>
       </c>
       <c r="AG14" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.CCY = sqlCCY.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="15" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>Book    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="5"/>
-        <v>Book    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>Book:    returnRecord.Book,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="2"/>
-        <v>Book:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.Book = sqlACCTBook.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="3"/>
-        <v>item.Book = r.FormValue("Book")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="4"/>
-        <v>.Book</v>
+        <v>.</v>
       </c>
       <c r="AG15" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.Book = sqlBook.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="16" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B16" s="1"/>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>MandatedUser    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="5"/>
-        <v>MandatedUser    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>MandatedUser:    returnRecord.MandatedUser,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="2"/>
-        <v>MandatedUser:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.MandatedUser = sqlACCTMandatedUser.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="3"/>
-        <v>item.MandatedUser = r.FormValue("MandatedUser")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD16" t="str">
         <f t="shared" si="4"/>
-        <v>.MandatedUser</v>
+        <v>.</v>
       </c>
       <c r="AG16" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.MandatedUser = sqlMandatedUser.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>BackOfficeNotes    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="5"/>
-        <v>BackOfficeNotes    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>BackOfficeNotes:    returnRecord.BackOfficeNotes,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="2"/>
-        <v>BackOfficeNotes:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.BackOfficeNotes = sqlACCTBackOfficeNotes.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="3"/>
-        <v>item.BackOfficeNotes = r.FormValue("BackOfficeNotes")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD17" t="str">
         <f t="shared" si="4"/>
-        <v>.BackOfficeNotes</v>
+        <v>.</v>
       </c>
       <c r="AG17" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.BackOfficeNotes = sqlBackOfficeNotes.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>CashBalance    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="5"/>
-        <v>CashBalance    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
-        <v>CashBalance:    returnRecord.CashBalance,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="2"/>
-        <v>CashBalance:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.CashBalance = sqlACCTCashBalance.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="3"/>
-        <v>item.CashBalance = r.FormValue("CashBalance")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD18" t="str">
         <f t="shared" si="4"/>
-        <v>.CashBalance</v>
+        <v>.</v>
       </c>
       <c r="AG18" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.CashBalance = sqlCashBalance.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>AccountNumber    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="5"/>
-        <v>AccountNumber    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>AccountNumber:    returnRecord.AccountNumber,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="2"/>
-        <v>AccountNumber:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.AccountNumber = sqlACCTAccountNumber.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="3"/>
-        <v>item.AccountNumber = r.FormValue("AccountNumber")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD19" t="str">
         <f t="shared" si="4"/>
-        <v>.AccountNumber</v>
+        <v>.</v>
       </c>
       <c r="AG19" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.AccountNumber = sqlAccountNumber.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>AccountName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="5"/>
-        <v>AccountName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
-        <v>AccountName:    returnRecord.AccountName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="2"/>
-        <v>AccountName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.AccountName = sqlACCTAccountName.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="3"/>
-        <v>item.AccountName = r.FormValue("AccountName")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD20" t="str">
         <f t="shared" si="4"/>
-        <v>.AccountName</v>
+        <v>.</v>
       </c>
       <c r="AG20" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.AccountName = sqlAccountName.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B21" s="1"/>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>LedgerBalance    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="5"/>
-        <v>LedgerBalance    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
-        <v>LedgerBalance:    returnRecord.LedgerBalance,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="2"/>
-        <v>LedgerBalance:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.LedgerBalance = sqlACCTLedgerBalance.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="3"/>
-        <v>item.LedgerBalance = r.FormValue("LedgerBalance")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD21" t="str">
         <f t="shared" si="4"/>
-        <v>.LedgerBalance</v>
+        <v>.</v>
       </c>
       <c r="AG21" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.LedgerBalance = sqlLedgerBalance.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B22" s="1"/>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>Portfolio    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="5"/>
-        <v>Portfolio    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
-        <v>Portfolio:    returnRecord.Portfolio,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="2"/>
-        <v>Portfolio:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.Portfolio = sqlACCTPortfolio.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="3"/>
-        <v>item.Portfolio = r.FormValue("Portfolio")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD22" t="str">
         <f t="shared" si="4"/>
-        <v>.Portfolio</v>
+        <v>.</v>
       </c>
       <c r="AG22" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.Portfolio = sqlPortfolio.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>AgreementId    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="5"/>
-        <v>AgreementId    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
-        <v>AgreementId:    returnRecord.AgreementId,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="2"/>
-        <v>AgreementId:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.AgreementId = sqlACCTAgreementId.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V23" t="str">
         <f t="shared" si="3"/>
-        <v>item.AgreementId = r.FormValue("AgreementId")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD23" t="str">
         <f t="shared" si="4"/>
-        <v>.AgreementId</v>
+        <v>.</v>
       </c>
       <c r="AG23" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.AgreementId = sqlAgreementId.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B24" s="1"/>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>BackOfficeRefNo    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="5"/>
-        <v>BackOfficeRefNo    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
-        <v>BackOfficeRefNo:    returnRecord.BackOfficeRefNo,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="2"/>
-        <v>BackOfficeRefNo:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.BackOfficeRefNo = sqlACCTBackOfficeRefNo.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V24" t="str">
         <f t="shared" si="3"/>
-        <v>item.BackOfficeRefNo = r.FormValue("BackOfficeRefNo")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD24" t="str">
         <f t="shared" si="4"/>
-        <v>.BackOfficeRefNo</v>
+        <v>.</v>
       </c>
       <c r="AG24" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.BackOfficeRefNo = sqlBackOfficeRefNo.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B25" s="1"/>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>PaymentSystemSienaView    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="5"/>
-        <v>PaymentSystemSienaView    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
-        <v>PaymentSystemSienaView:    returnRecord.PaymentSystemSienaView,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="2"/>
-        <v>PaymentSystemSienaView:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.PaymentSystemSienaView = sqlACCTPaymentSystemSienaView.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V25" t="str">
         <f t="shared" si="3"/>
-        <v>item.PaymentSystemSienaView = r.FormValue("PaymentSystemSienaView")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD25" t="str">
         <f t="shared" si="4"/>
-        <v>.PaymentSystemSienaView</v>
+        <v>.</v>
       </c>
       <c r="AG25" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.PaymentSystemSienaView = sqlPaymentSystemSienaView.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B26" s="1"/>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>ISIN    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="5"/>
-        <v>ISIN    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
-        <v>ISIN:    returnRecord.ISIN,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="2"/>
-        <v>ISIN:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.ISIN = sqlACCTISIN.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V26" t="str">
         <f t="shared" si="3"/>
-        <v>item.ISIN = r.FormValue("ISIN")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD26" t="str">
         <f t="shared" si="4"/>
-        <v>.ISIN</v>
+        <v>.</v>
       </c>
       <c r="AG26" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.ISIN = sqlISIN.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>UTI    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="5"/>
-        <v>UTI    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
-        <v>UTI:    returnRecord.UTI,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="2"/>
-        <v>UTI:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.UTI = sqlACCTUTI.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V27" t="str">
         <f t="shared" si="3"/>
-        <v>item.UTI = r.FormValue("UTI")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD27" t="str">
         <f t="shared" si="4"/>
-        <v>.UTI</v>
+        <v>.</v>
       </c>
       <c r="AG27" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.UTI = sqlUTI.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="B28" s="1"/>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>CCYName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="5"/>
-        <v>CCYName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
-        <v>CCYName:    returnRecord.CCYName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="2"/>
-        <v>CCYName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.CCYName = sqlACCTCCYName.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V28" t="str">
         <f t="shared" si="3"/>
-        <v>item.CCYName = r.FormValue("CCYName")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD28" t="str">
         <f t="shared" si="4"/>
-        <v>.CCYName</v>
+        <v>.</v>
       </c>
       <c r="AG28" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.CCYName = sqlCCYName.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="B29" s="1"/>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>BookName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="5"/>
-        <v>BookName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
-        <v>BookName:    returnRecord.BookName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="2"/>
-        <v>BookName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.BookName = sqlACCTBookName.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V29" t="str">
         <f t="shared" si="3"/>
-        <v>item.BookName = r.FormValue("BookName")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD29" t="str">
         <f t="shared" si="4"/>
-        <v>.BookName</v>
+        <v>.</v>
       </c>
       <c r="AG29" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.BookName = sqlBookName.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="30" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>PortfolioName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="5"/>
-        <v>PortfolioName    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
-        <v>PortfolioName:    returnRecord.PortfolioName,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="2"/>
-        <v>PortfolioName:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.PortfolioName = sqlACCTPortfolioName.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V30" t="str">
         <f t="shared" si="3"/>
-        <v>item.PortfolioName = r.FormValue("PortfolioName")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD30" t="str">
         <f t="shared" si="4"/>
-        <v>.PortfolioName</v>
+        <v>.</v>
       </c>
       <c r="AG30" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.PortfolioName = sqlPortfolioName.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="B31" s="1"/>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>Centre    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="5"/>
-        <v>Centre    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
-        <v>Centre:    returnRecord.Centre,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="2"/>
-        <v>Centre:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.Centre = sqlACCTCentre.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V31" t="str">
         <f t="shared" si="3"/>
-        <v>item.Centre = r.FormValue("Centre")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD31" t="str">
         <f t="shared" si="4"/>
-        <v>.Centre</v>
+        <v>.</v>
       </c>
       <c r="AG31" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.Centre = sqlCentre.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="B32" s="1"/>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>Firm    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="5"/>
-        <v>Firm    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
-        <v>Firm:    returnRecord.Firm,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="2"/>
-        <v>Firm:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.Firm = sqlACCTFirm.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V32" t="str">
         <f t="shared" si="3"/>
-        <v>item.Firm = r.FormValue("Firm")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD32" t="str">
         <f t="shared" si="4"/>
-        <v>.Firm</v>
+        <v>.</v>
       </c>
       <c r="AG32" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.Firm = sqlFirm.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="33" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="B33" s="1"/>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>CCYDp    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="5"/>
-        <v>CCYDp    string</v>
+        <v xml:space="preserve">    string</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
-        <v>CCYDp:    returnRecord.CCYDp,</v>
+        <v>:    returnRecord.,</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="2"/>
-        <v>CCYDp:    "",</v>
+        <v>:    "",</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount.CCYDp = sqlACCTCCYDp.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V33" t="str">
         <f t="shared" si="3"/>
-        <v>item.CCYDp = r.FormValue("CCYDp")</v>
+        <v>item. = r.FormValue("")</v>
       </c>
       <c r="AD33" t="str">
         <f t="shared" si="4"/>
-        <v>.CCYDp</v>
+        <v>.</v>
       </c>
       <c r="AG33" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount.CCYDp = sqlCCYDp.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="34" spans="2:33" x14ac:dyDescent="0.2">
@@ -1708,7 +1598,7 @@
       </c>
       <c r="L34" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V34" t="str">
         <f t="shared" si="3"/>
@@ -1720,7 +1610,7 @@
       </c>
       <c r="AG34" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="35" spans="2:33" x14ac:dyDescent="0.2">
@@ -1743,7 +1633,7 @@
       </c>
       <c r="L35" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V35" t="str">
         <f t="shared" si="3"/>
@@ -1755,7 +1645,7 @@
       </c>
       <c r="AG35" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="36" spans="2:33" x14ac:dyDescent="0.2">
@@ -1778,7 +1668,7 @@
       </c>
       <c r="L36" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V36" t="str">
         <f t="shared" si="3"/>
@@ -1790,7 +1680,7 @@
       </c>
       <c r="AG36" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="37" spans="2:33" x14ac:dyDescent="0.2">
@@ -1813,7 +1703,7 @@
       </c>
       <c r="L37" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V37" t="str">
         <f t="shared" si="3"/>
@@ -1825,7 +1715,7 @@
       </c>
       <c r="AG37" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="38" spans="2:33" x14ac:dyDescent="0.2">
@@ -1848,7 +1738,7 @@
       </c>
       <c r="L38" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V38" t="str">
         <f t="shared" si="3"/>
@@ -1860,7 +1750,7 @@
       </c>
       <c r="AG38" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="39" spans="2:33" x14ac:dyDescent="0.2">
@@ -1883,7 +1773,7 @@
       </c>
       <c r="L39" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V39" t="str">
         <f t="shared" si="3"/>
@@ -1895,7 +1785,7 @@
       </c>
       <c r="AG39" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="40" spans="2:33" x14ac:dyDescent="0.2">
@@ -1918,7 +1808,7 @@
       </c>
       <c r="L40" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V40" t="str">
         <f t="shared" ref="V40:V62" si="12">"item."&amp;B40&amp;" = r.FormValue("""&amp;B40&amp;""")"</f>
@@ -1930,7 +1820,7 @@
       </c>
       <c r="AG40" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="41" spans="2:33" x14ac:dyDescent="0.2">
@@ -1953,7 +1843,7 @@
       </c>
       <c r="L41" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V41" t="str">
         <f t="shared" si="12"/>
@@ -1965,7 +1855,7 @@
       </c>
       <c r="AG41" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="42" spans="2:33" x14ac:dyDescent="0.2">
@@ -1988,7 +1878,7 @@
       </c>
       <c r="L42" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V42" t="str">
         <f t="shared" si="12"/>
@@ -2000,7 +1890,7 @@
       </c>
       <c r="AG42" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="43" spans="2:33" x14ac:dyDescent="0.2">
@@ -2023,7 +1913,7 @@
       </c>
       <c r="L43" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V43" t="str">
         <f t="shared" si="12"/>
@@ -2035,7 +1925,7 @@
       </c>
       <c r="AG43" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="44" spans="2:33" x14ac:dyDescent="0.2">
@@ -2058,7 +1948,7 @@
       </c>
       <c r="L44" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V44" t="str">
         <f t="shared" si="12"/>
@@ -2070,7 +1960,7 @@
       </c>
       <c r="AG44" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="45" spans="2:33" x14ac:dyDescent="0.2">
@@ -2093,7 +1983,7 @@
       </c>
       <c r="L45" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V45" t="str">
         <f t="shared" si="12"/>
@@ -2105,7 +1995,7 @@
       </c>
       <c r="AG45" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="46" spans="2:33" x14ac:dyDescent="0.2">
@@ -2128,7 +2018,7 @@
       </c>
       <c r="L46" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V46" t="str">
         <f t="shared" si="12"/>
@@ -2140,7 +2030,7 @@
       </c>
       <c r="AG46" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="47" spans="2:33" x14ac:dyDescent="0.2">
@@ -2163,7 +2053,7 @@
       </c>
       <c r="L47" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V47" t="str">
         <f t="shared" si="12"/>
@@ -2175,7 +2065,7 @@
       </c>
       <c r="AG47" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="48" spans="2:33" x14ac:dyDescent="0.2">
@@ -2198,7 +2088,7 @@
       </c>
       <c r="L48" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V48" t="str">
         <f t="shared" si="12"/>
@@ -2210,7 +2100,7 @@
       </c>
       <c r="AG48" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="49" spans="2:33" x14ac:dyDescent="0.2">
@@ -2233,7 +2123,7 @@
       </c>
       <c r="L49" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V49" t="str">
         <f t="shared" si="12"/>
@@ -2245,7 +2135,7 @@
       </c>
       <c r="AG49" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="50" spans="2:33" x14ac:dyDescent="0.2">
@@ -2268,7 +2158,7 @@
       </c>
       <c r="L50" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V50" t="str">
         <f t="shared" si="12"/>
@@ -2280,7 +2170,7 @@
       </c>
       <c r="AG50" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="51" spans="2:33" x14ac:dyDescent="0.2">
@@ -2303,7 +2193,7 @@
       </c>
       <c r="L51" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V51" t="str">
         <f t="shared" si="12"/>
@@ -2315,7 +2205,7 @@
       </c>
       <c r="AG51" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="52" spans="2:33" x14ac:dyDescent="0.2">
@@ -2338,7 +2228,7 @@
       </c>
       <c r="L52" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V52" t="str">
         <f t="shared" si="12"/>
@@ -2350,7 +2240,7 @@
       </c>
       <c r="AG52" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="53" spans="2:33" x14ac:dyDescent="0.2">
@@ -2373,7 +2263,7 @@
       </c>
       <c r="L53" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V53" t="str">
         <f t="shared" si="12"/>
@@ -2385,7 +2275,7 @@
       </c>
       <c r="AG53" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="54" spans="2:33" x14ac:dyDescent="0.2">
@@ -2408,7 +2298,7 @@
       </c>
       <c r="L54" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V54" t="str">
         <f t="shared" si="12"/>
@@ -2420,7 +2310,7 @@
       </c>
       <c r="AG54" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="55" spans="2:33" x14ac:dyDescent="0.2">
@@ -2443,7 +2333,7 @@
       </c>
       <c r="L55" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V55" t="str">
         <f t="shared" si="12"/>
@@ -2455,7 +2345,7 @@
       </c>
       <c r="AG55" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="56" spans="2:33" x14ac:dyDescent="0.2">
@@ -2478,7 +2368,7 @@
       </c>
       <c r="L56" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V56" t="str">
         <f t="shared" si="12"/>
@@ -2490,7 +2380,7 @@
       </c>
       <c r="AG56" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="57" spans="2:33" x14ac:dyDescent="0.2">
@@ -2513,7 +2403,7 @@
       </c>
       <c r="L57" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V57" t="str">
         <f t="shared" si="12"/>
@@ -2525,7 +2415,7 @@
       </c>
       <c r="AG57" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="58" spans="2:33" x14ac:dyDescent="0.2">
@@ -2548,7 +2438,7 @@
       </c>
       <c r="L58" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V58" t="str">
         <f t="shared" si="12"/>
@@ -2560,7 +2450,7 @@
       </c>
       <c r="AG58" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="59" spans="2:33" x14ac:dyDescent="0.2">
@@ -2583,7 +2473,7 @@
       </c>
       <c r="L59" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V59" t="str">
         <f t="shared" si="12"/>
@@ -2595,7 +2485,7 @@
       </c>
       <c r="AG59" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="60" spans="2:33" x14ac:dyDescent="0.2">
@@ -2618,7 +2508,7 @@
       </c>
       <c r="L60" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V60" t="str">
         <f t="shared" si="12"/>
@@ -2630,7 +2520,7 @@
       </c>
       <c r="AG60" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="61" spans="2:33" x14ac:dyDescent="0.2">
@@ -2653,7 +2543,7 @@
       </c>
       <c r="L61" t="str">
         <f t="shared" si="6"/>
-        <v>sienaAccount. = sqlACCT.String</v>
+        <v>sienaCalender. = sqlCAL.String</v>
       </c>
       <c r="V61" t="str">
         <f t="shared" si="12"/>
@@ -2665,7 +2555,7 @@
       </c>
       <c r="AG61" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="62" spans="2:33" x14ac:dyDescent="0.2">
@@ -2688,7 +2578,7 @@
       </c>
       <c r="L62" t="str">
         <f t="shared" ref="L62" si="14">$I$3&amp;"."&amp;B62&amp;" = "&amp;B62&amp;".String"</f>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V62" t="str">
         <f t="shared" si="12"/>
@@ -2700,7 +2590,7 @@
       </c>
       <c r="AG62" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="63" spans="2:33" x14ac:dyDescent="0.2">
@@ -2723,7 +2613,7 @@
       </c>
       <c r="L63" t="str">
         <f t="shared" ref="L63:L74" si="19">$I$3&amp;"."&amp;B63&amp;" = "&amp;B63&amp;".String"</f>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V63" t="str">
         <f t="shared" ref="V63:V74" si="20">"item."&amp;B63&amp;" = r.FormValue("""&amp;B63&amp;""")"</f>
@@ -2735,7 +2625,7 @@
       </c>
       <c r="AG63" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="64" spans="2:33" x14ac:dyDescent="0.2">
@@ -2758,7 +2648,7 @@
       </c>
       <c r="L64" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V64" t="str">
         <f t="shared" si="20"/>
@@ -2770,7 +2660,7 @@
       </c>
       <c r="AG64" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="65" spans="2:33" x14ac:dyDescent="0.2">
@@ -2793,7 +2683,7 @@
       </c>
       <c r="L65" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V65" t="str">
         <f t="shared" si="20"/>
@@ -2805,7 +2695,7 @@
       </c>
       <c r="AG65" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="66" spans="2:33" x14ac:dyDescent="0.2">
@@ -2828,7 +2718,7 @@
       </c>
       <c r="L66" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V66" t="str">
         <f t="shared" si="20"/>
@@ -2840,7 +2730,7 @@
       </c>
       <c r="AG66" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="67" spans="2:33" x14ac:dyDescent="0.2">
@@ -2863,7 +2753,7 @@
       </c>
       <c r="L67" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V67" t="str">
         <f t="shared" si="20"/>
@@ -2875,7 +2765,7 @@
       </c>
       <c r="AG67" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="68" spans="2:33" x14ac:dyDescent="0.2">
@@ -2898,7 +2788,7 @@
       </c>
       <c r="L68" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V68" t="str">
         <f t="shared" si="20"/>
@@ -2910,7 +2800,7 @@
       </c>
       <c r="AG68" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="69" spans="2:33" x14ac:dyDescent="0.2">
@@ -2933,7 +2823,7 @@
       </c>
       <c r="L69" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V69" t="str">
         <f t="shared" si="20"/>
@@ -2945,7 +2835,7 @@
       </c>
       <c r="AG69" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="70" spans="2:33" x14ac:dyDescent="0.2">
@@ -2968,7 +2858,7 @@
       </c>
       <c r="L70" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V70" t="str">
         <f t="shared" si="20"/>
@@ -2980,7 +2870,7 @@
       </c>
       <c r="AG70" t="str">
         <f t="shared" si="7"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="71" spans="2:33" x14ac:dyDescent="0.2">
@@ -3003,7 +2893,7 @@
       </c>
       <c r="L71" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V71" t="str">
         <f t="shared" si="20"/>
@@ -3015,7 +2905,7 @@
       </c>
       <c r="AG71" t="str">
         <f t="shared" ref="AG71:AG74" si="22">$I$3&amp;"."&amp;B71&amp;" = sql"&amp;B71&amp;".String"</f>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="72" spans="2:33" x14ac:dyDescent="0.2">
@@ -3038,7 +2928,7 @@
       </c>
       <c r="L72" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V72" t="str">
         <f t="shared" si="20"/>
@@ -3050,7 +2940,7 @@
       </c>
       <c r="AG72" t="str">
         <f t="shared" si="22"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="73" spans="2:33" x14ac:dyDescent="0.2">
@@ -3073,7 +2963,7 @@
       </c>
       <c r="L73" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V73" t="str">
         <f t="shared" si="20"/>
@@ -3085,7 +2975,7 @@
       </c>
       <c r="AG73" t="str">
         <f t="shared" si="22"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
     <row r="74" spans="2:33" x14ac:dyDescent="0.2">
@@ -3108,7 +2998,7 @@
       </c>
       <c r="L74" t="str">
         <f t="shared" si="19"/>
-        <v>sienaAccount. = .String</v>
+        <v>sienaCalender. = .String</v>
       </c>
       <c r="V74" t="str">
         <f t="shared" si="20"/>
@@ -3120,7 +3010,7 @@
       </c>
       <c r="AG74" t="str">
         <f t="shared" si="22"/>
-        <v>sienaAccount. = sql.String</v>
+        <v>sienaCalender. = sql.String</v>
       </c>
     </row>
   </sheetData>
@@ -3132,8 +3022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90230AA-F0B1-6C49-B8FC-2C26A6B44982}">
   <dimension ref="A2:BK15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:AD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3152,7 +3042,7 @@
     <row r="3" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C3" t="str">
         <f>UPPER('GO Struct Bits'!B2)</f>
-        <v>ACCT</v>
+        <v>CAL</v>
       </c>
     </row>
     <row r="6" spans="1:63" x14ac:dyDescent="0.2">
@@ -3161,88 +3051,88 @@
         <v>0</v>
       </c>
       <c r="C6" t="str">
-        <v>SienaReference</v>
+        <v>ID</v>
       </c>
       <c r="D6" t="str">
-        <v>CustomerSienaView</v>
+        <v>Source</v>
       </c>
       <c r="E6" t="str">
-        <v>SienaCommonRef</v>
+        <v>Date</v>
       </c>
       <c r="F6" t="str">
-        <v>Status</v>
+        <v>Time</v>
       </c>
       <c r="G6" t="str">
-        <v>StartDate</v>
+        <v>ShortName</v>
       </c>
       <c r="H6" t="str">
-        <v>MaturityDate</v>
-      </c>
-      <c r="I6" t="str">
-        <v>ContractNumber</v>
-      </c>
-      <c r="J6" t="str">
-        <v>ExternalReference</v>
-      </c>
-      <c r="K6" t="str">
-        <v>CCY</v>
-      </c>
-      <c r="L6" t="str">
-        <v>Book</v>
-      </c>
-      <c r="M6" t="str">
-        <v>MandatedUser</v>
-      </c>
-      <c r="N6" t="str">
-        <v>BackOfficeNotes</v>
-      </c>
-      <c r="O6" t="str">
-        <v>CashBalance</v>
-      </c>
-      <c r="P6" t="str">
-        <v>AccountNumber</v>
-      </c>
-      <c r="Q6" t="str">
-        <v>AccountName</v>
-      </c>
-      <c r="R6" t="str">
-        <v>LedgerBalance</v>
-      </c>
-      <c r="S6" t="str">
-        <v>Portfolio</v>
-      </c>
-      <c r="T6" t="str">
-        <v>AgreementId</v>
-      </c>
-      <c r="U6" t="str">
-        <v>BackOfficeRefNo</v>
-      </c>
-      <c r="V6" t="str">
-        <v>PaymentSystemSienaView</v>
-      </c>
-      <c r="W6" t="str">
-        <v>ISIN</v>
-      </c>
-      <c r="X6" t="str">
-        <v>UTI</v>
-      </c>
-      <c r="Y6" t="str">
-        <v>CCYName</v>
-      </c>
-      <c r="Z6" t="str">
-        <v>BookName</v>
-      </c>
-      <c r="AA6" t="str">
-        <v>PortfolioName</v>
-      </c>
-      <c r="AB6" t="str">
-        <v>Centre</v>
-      </c>
-      <c r="AC6" t="str">
-        <v>Firm</v>
-      </c>
-      <c r="AD6" t="str">
-        <v>CCYDp</v>
+        <v>Description</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
       </c>
       <c r="AE6">
         <v>0</v>
@@ -3302,119 +3192,119 @@
       </c>
       <c r="B8" t="str">
         <f>"var siena"&amp;'GO Struct Bits'!B4&amp;"SQL"</f>
-        <v>var sienaAccountSQL</v>
+        <v>var sienaCalenderSQL</v>
       </c>
       <c r="C8" t="str">
         <f>C6&amp;", "</f>
-        <v xml:space="preserve">SienaReference, </v>
+        <v xml:space="preserve">ID, </v>
       </c>
       <c r="D8" t="str">
         <f t="shared" ref="D8:BK8" si="0">D6&amp;", "</f>
-        <v xml:space="preserve">CustomerSienaView, </v>
+        <v xml:space="preserve">Source, </v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">SienaCommonRef, </v>
+        <v xml:space="preserve">Date, </v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Status, </v>
+        <v xml:space="preserve">Time, </v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">StartDate, </v>
+        <v xml:space="preserve">ShortName, </v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">MaturityDate, </v>
+        <v xml:space="preserve">Description, </v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ContractNumber, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ExternalReference, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CCY, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Book, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">MandatedUser, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">BackOfficeNotes, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CashBalance, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">AccountNumber, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">AccountName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">LedgerBalance, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Portfolio, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">AgreementId, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">BackOfficeRefNo, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PaymentSystemSienaView, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ISIN, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="X8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">UTI, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CCYName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">BookName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PortfolioName, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Centre, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AC8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Firm, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CCYDp, </v>
+        <v xml:space="preserve">0, </v>
       </c>
       <c r="AE8" t="str">
         <f t="shared" si="0"/>
@@ -3552,115 +3442,115 @@
     <row r="10" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C10" t="str">
         <f>"&amp;"&amp;C8</f>
-        <v xml:space="preserve">&amp;SienaReference, </v>
+        <v xml:space="preserve">&amp;ID, </v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ref="D10:BK10" si="1">"&amp;"&amp;D8</f>
-        <v xml:space="preserve">&amp;CustomerSienaView, </v>
+        <v xml:space="preserve">&amp;Source, </v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;SienaCommonRef, </v>
+        <v xml:space="preserve">&amp;Date, </v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Status, </v>
+        <v xml:space="preserve">&amp;Time, </v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;StartDate, </v>
+        <v xml:space="preserve">&amp;ShortName, </v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;MaturityDate, </v>
+        <v xml:space="preserve">&amp;Description, </v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ContractNumber, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ExternalReference, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;CCY, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Book, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;MandatedUser, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;BackOfficeNotes, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;CashBalance, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;AccountNumber, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;AccountName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="R10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;LedgerBalance, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Portfolio, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="T10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;AgreementId, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="U10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;BackOfficeRefNo, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;PaymentSystemSienaView, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;ISIN, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;UTI, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;CCYName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;BookName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;PortfolioName, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Centre, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AC10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;Firm, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">&amp;CCYDp, </v>
+        <v xml:space="preserve">&amp;0, </v>
       </c>
       <c r="AE10" t="str">
         <f t="shared" si="1"/>
@@ -3801,199 +3691,199 @@
       </c>
       <c r="C13" t="str">
         <f>"sql"&amp;$C$3&amp;""&amp;C8</f>
-        <v xml:space="preserve">sqlACCTSienaReference, </v>
+        <v xml:space="preserve">sqlCALID, </v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ref="D13:AY13" si="2">"sql"&amp;$C$3&amp;""&amp;D8</f>
-        <v xml:space="preserve">sqlACCTCustomerSienaView, </v>
+        <v xml:space="preserve">sqlCALSource, </v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTSienaCommonRef, </v>
+        <v xml:space="preserve">sqlCALDate, </v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTStatus, </v>
+        <v xml:space="preserve">sqlCALTime, </v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTStartDate, </v>
+        <v xml:space="preserve">sqlCALShortName, </v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTMaturityDate, </v>
+        <v xml:space="preserve">sqlCALDescription, </v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTContractNumber, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTExternalReference, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTCCY, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTBook, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTMandatedUser, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTBackOfficeNotes, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="O13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTCashBalance, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTAccountNumber, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTAccountName, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTLedgerBalance, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTPortfolio, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTAgreementId, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTBackOfficeRefNo, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTPaymentSystemSienaView, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTISIN, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTUTI, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTCCYName, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTBookName, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTPortfolioName, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTCentre, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AC13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTFirm, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCTCCYDp, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AF13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AG13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AH13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AI13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AJ13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AK13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AL13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AM13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AN13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AO13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AP13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AQ13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AR13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AS13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AT13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AU13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT0, </v>
+        <v xml:space="preserve">sqlCAL0, </v>
       </c>
       <c r="AV13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT, </v>
+        <v xml:space="preserve">sqlCAL, </v>
       </c>
       <c r="AW13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT, </v>
+        <v xml:space="preserve">sqlCAL, </v>
       </c>
       <c r="AX13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT, </v>
+        <v xml:space="preserve">sqlCAL, </v>
       </c>
       <c r="AY13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">sqlACCT, </v>
+        <v xml:space="preserve">sqlCAL, </v>
       </c>
     </row>
     <row r="15" spans="1:63" x14ac:dyDescent="0.2">
@@ -4002,171 +3892,171 @@
       </c>
       <c r="C15" t="str">
         <f>"&amp;"&amp;C13</f>
-        <v xml:space="preserve">&amp;sqlACCTSienaReference, </v>
+        <v xml:space="preserve">&amp;sqlCALID, </v>
       </c>
       <c r="D15" t="str">
         <f t="shared" ref="D15:AR15" si="3">"&amp;"&amp;D13</f>
-        <v xml:space="preserve">&amp;sqlACCTCustomerSienaView, </v>
+        <v xml:space="preserve">&amp;sqlCALSource, </v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTSienaCommonRef, </v>
+        <v xml:space="preserve">&amp;sqlCALDate, </v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTStatus, </v>
+        <v xml:space="preserve">&amp;sqlCALTime, </v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTStartDate, </v>
+        <v xml:space="preserve">&amp;sqlCALShortName, </v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTMaturityDate, </v>
+        <v xml:space="preserve">&amp;sqlCALDescription, </v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTContractNumber, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTExternalReference, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTCCY, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTBook, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTMandatedUser, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTBackOfficeNotes, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTCashBalance, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTAccountNumber, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTAccountName, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTLedgerBalance, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTPortfolio, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTAgreementId, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTBackOfficeRefNo, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTPaymentSystemSienaView, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTISIN, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTUTI, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTCCYName, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTBookName, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTPortfolioName, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTCentre, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AC15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTFirm, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCTCCYDp, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AE15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AF15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AG15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AH15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AI15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AJ15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AK15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AL15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AM15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AN15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AO15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AP15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AQ15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
       <c r="AR15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;sqlACCT0, </v>
+        <v xml:space="preserve">&amp;sqlCAL0, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>